<commit_message>
fixed and improved hatshop
</commit_message>
<xml_diff>
--- a/HutListe.xlsx
+++ b/HutListe.xlsx
@@ -24,15 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="226">
   <si>
     <t>states/schaf.png</t>
-  </si>
-  <si>
-    <t>states/newuser.png</t>
-  </si>
-  <si>
-    <t>states/vip.png</t>
   </si>
   <si>
     <t>states/away.png</t>
@@ -728,30 +722,12 @@
     <t>a57</t>
   </si>
   <si>
-    <t>a58</t>
-  </si>
-  <si>
-    <t>a59</t>
-  </si>
-  <si>
-    <t>a60</t>
-  </si>
-  <si>
-    <t>a61</t>
-  </si>
-  <si>
-    <t>a62</t>
-  </si>
-  <si>
     <t>category:</t>
   </si>
   <si>
     <t>Chips</t>
   </si>
   <si>
-    <t>Besonders</t>
-  </si>
-  <si>
     <t>Abstrakt</t>
   </si>
   <si>
@@ -954,6 +930,108 @@
   </si>
   <si>
     <t>},</t>
+  </si>
+  <si>
+    <t>states/newUser.png</t>
+  </si>
+  <si>
+    <t>states/icon_vip.png</t>
+  </si>
+  <si>
+    <t>Kategorie</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Bild</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Preis</t>
+  </si>
+  <si>
+    <t>Spalte1</t>
+  </si>
+  <si>
+    <t>Spalte2</t>
+  </si>
+  <si>
+    <t>Spalte3</t>
+  </si>
+  <si>
+    <t>Spalte4</t>
+  </si>
+  <si>
+    <t>Spalte5</t>
+  </si>
+  <si>
+    <t>Spalte6</t>
+  </si>
+  <si>
+    <t>Spalte7</t>
+  </si>
+  <si>
+    <t>Spalte8</t>
+  </si>
+  <si>
+    <t>Spalte9</t>
+  </si>
+  <si>
+    <t>Spalte10</t>
+  </si>
+  <si>
+    <t>Spalte11</t>
+  </si>
+  <si>
+    <t>Spalte12</t>
+  </si>
+  <si>
+    <t>_SPECIAL_</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>&amp;00</t>
+  </si>
+  <si>
+    <t>&amp;01</t>
+  </si>
+  <si>
+    <t>&amp;02</t>
+  </si>
+  <si>
+    <t>&amp;03</t>
+  </si>
+  <si>
+    <t>NPF</t>
+  </si>
+  <si>
+    <t>NPM</t>
+  </si>
+  <si>
+    <t>a00</t>
+  </si>
+  <si>
+    <t>chips/chip_100.png</t>
+  </si>
+  <si>
+    <t>Das sind schon einige Punkte!</t>
+  </si>
+  <si>
+    <t>Das könnte teuer werden!</t>
+  </si>
+  <si>
+    <t>chips/chip_500.png</t>
+  </si>
+  <si>
+    <t>chips/chip_1M.png</t>
+  </si>
+  <si>
+    <t>Da spielt jemand mit richtig viel!</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1098,44 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFA9B7C6"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFA9B7C6"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1031,6 +1146,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:Q66" totalsRowShown="0">
+  <autoFilter ref="A1:Q66"/>
+  <sortState ref="A2:Q63">
+    <sortCondition ref="G1:G63"/>
+  </sortState>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Spalte1"/>
+    <tableColumn id="2" name="Spalte2"/>
+    <tableColumn id="3" name="ID"/>
+    <tableColumn id="4" name="Spalte3"/>
+    <tableColumn id="5" name="Spalte4"/>
+    <tableColumn id="6" name="Spalte5"/>
+    <tableColumn id="7" name="Kategorie"/>
+    <tableColumn id="8" name="Spalte6"/>
+    <tableColumn id="9" name="Spalte7"/>
+    <tableColumn id="10" name="Spalte8"/>
+    <tableColumn id="11" name="Bild" dataDxfId="1"/>
+    <tableColumn id="12" name="Spalte9" dataDxfId="0"/>
+    <tableColumn id="13" name="Spalte10"/>
+    <tableColumn id="14" name="Beschreibung"/>
+    <tableColumn id="15" name="Spalte11"/>
+    <tableColumn id="16" name="Preis"/>
+    <tableColumn id="17" name="Spalte12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1296,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q63"/>
+  <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1309,3294 +1453,3509 @@
     <col min="14" max="14" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" t="s">
+        <v>205</v>
+      </c>
+      <c r="J1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="M1" t="s">
+        <v>208</v>
+      </c>
+      <c r="N1" t="s">
+        <v>197</v>
+      </c>
+      <c r="O1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>210</v>
+      </c>
+    </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>133</v>
+        <v>211</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
+        <v>132</v>
+      </c>
+      <c r="O2" t="s">
+        <v>190</v>
+      </c>
+      <c r="P2">
         <v>0</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" t="s">
-        <v>138</v>
-      </c>
-      <c r="O2" t="s">
-        <v>198</v>
-      </c>
-      <c r="P2">
-        <v>200</v>
-      </c>
       <c r="Q2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>133</v>
+        <v>211</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="O3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>214</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>211</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="O4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>137</v>
+        <v>211</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="O5" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>217</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>211</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="O6" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>130</v>
+        <v>211</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="O7" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>216</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>211</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N8" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="O8" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P8">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="O9" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P9">
         <v>25</v>
       </c>
       <c r="Q9" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="O10" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P10">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="Q10" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="O11" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P11">
         <v>25</v>
       </c>
       <c r="Q11" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O12" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P12">
         <v>25</v>
       </c>
       <c r="Q12" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O13" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P13">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="Q13" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O14" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P14">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="Q14" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="O15" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P15">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="Q15" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G16" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="O16" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P16">
-        <v>50</v>
+        <v>10000</v>
       </c>
       <c r="Q16" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" t="s">
         <v>129</v>
       </c>
-      <c r="F17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" t="s">
-        <v>135</v>
-      </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N17" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="O17" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P17">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="Q17" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" t="s">
         <v>129</v>
       </c>
-      <c r="F18" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" t="s">
-        <v>137</v>
-      </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="O18" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P18">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="Q18" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" t="s">
         <v>129</v>
       </c>
-      <c r="F19" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" t="s">
-        <v>137</v>
-      </c>
       <c r="H19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N19" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="O19" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P19">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="Q19" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" t="s">
         <v>129</v>
       </c>
-      <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" t="s">
-        <v>132</v>
-      </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N20" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="O20" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P20">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="Q20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" t="s">
         <v>129</v>
       </c>
-      <c r="F21" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" t="s">
-        <v>132</v>
-      </c>
       <c r="H21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N21" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="O21" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P21">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="Q21" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" t="s">
         <v>129</v>
       </c>
-      <c r="F22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" t="s">
-        <v>135</v>
-      </c>
       <c r="H22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N22" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="O22" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P22">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="Q22" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" t="s">
         <v>129</v>
       </c>
-      <c r="F23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" t="s">
-        <v>135</v>
-      </c>
       <c r="H23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N23" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="O23" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P23">
-        <v>100</v>
+        <v>2500</v>
       </c>
       <c r="Q23" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" t="s">
         <v>129</v>
       </c>
-      <c r="F24" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" t="s">
-        <v>135</v>
-      </c>
       <c r="H24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N24" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="O24" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P24">
-        <v>50</v>
+        <v>5000</v>
       </c>
       <c r="Q24" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" t="s">
         <v>129</v>
       </c>
-      <c r="F25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" t="s">
-        <v>135</v>
-      </c>
       <c r="H25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N25" t="s">
         <v>161</v>
       </c>
       <c r="O25" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P25">
-        <v>250</v>
+        <v>1000000</v>
       </c>
       <c r="Q25" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" t="s">
         <v>129</v>
       </c>
-      <c r="F26" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" t="s">
-        <v>135</v>
-      </c>
       <c r="H26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="O26" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P26">
-        <v>200</v>
+        <v>100000000</v>
       </c>
       <c r="Q26" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G27" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="H27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N27" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="O27" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P27">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="Q27" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="H28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N28" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="O28" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P28">
-        <v>2500</v>
+        <v>5</v>
       </c>
       <c r="Q28" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E29" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="H29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N29" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="O29" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P29">
-        <v>5000</v>
+        <v>10</v>
       </c>
       <c r="Q29" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N30" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="O30" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P30">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="Q30" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G31" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N31" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="O31" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P31">
-        <v>500</v>
+        <v>25</v>
       </c>
       <c r="Q31" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E32" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G32" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>23</v>
+        <v>220</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N32" t="s">
-        <v>167</v>
+        <v>221</v>
       </c>
       <c r="O32" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P32">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="Q32" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G33" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="H33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>24</v>
+        <v>223</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N33" t="s">
-        <v>167</v>
+        <v>222</v>
       </c>
       <c r="O33" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P33">
         <v>500</v>
       </c>
       <c r="Q33" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E34" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G34" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="H34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>36</v>
+        <v>224</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N34" t="s">
-        <v>168</v>
+        <v>225</v>
       </c>
       <c r="O34" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P34">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="Q34" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E35" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G35" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N35" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="O35" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P35">
-        <v>1000000</v>
+        <v>10</v>
       </c>
       <c r="Q35" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G36" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N36" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="O36" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P36">
-        <v>500000</v>
+        <v>150</v>
       </c>
       <c r="Q36" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E37" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G37" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N37" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="O37" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P37">
-        <v>100000000</v>
+        <v>150</v>
       </c>
       <c r="Q37" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G38" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N38" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="O38" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P38">
-        <v>500</v>
+        <v>150</v>
       </c>
       <c r="Q38" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E39" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G39" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N39" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="O39" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P39">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="Q39" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G40" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N40" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="O40" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P40">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="Q40" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E41" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G41" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M41" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N41" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="O41" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P41">
-        <v>50000</v>
+        <v>200</v>
       </c>
       <c r="Q41" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E42" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G42" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H42" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N42" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O42" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P42">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="Q42" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E43" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G43" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N43" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="O43" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P43">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="Q43" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E44" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G44" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J44" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N44" t="s">
         <v>186</v>
       </c>
       <c r="O44" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P44">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="Q44" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E45" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M45" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N45" t="s">
         <v>187</v>
       </c>
       <c r="O45" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P45">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="Q45" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E46" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G46" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H46" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N46" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="O46" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P46">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="Q46" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E47" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G47" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M47" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N47" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O47" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P47">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="Q47" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E48" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G48" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O48" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P48">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="Q48" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E49" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G49" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N49" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="O49" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P49">
-        <v>150</v>
+        <v>100000</v>
       </c>
       <c r="Q49" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E50" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G50" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N50" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="O50" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P50">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="Q50" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E51" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G51" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H51" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I51" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N51" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="O51" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P51">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="Q51" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E52" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G52" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M52" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N52" t="s">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="O52" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P52">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="Q52" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E53" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G53" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H53" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N53" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="O53" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P53">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="Q53" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D54" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E54" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G54" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H54" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I54" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N54" t="s">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="O54" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P54">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="Q54" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E55" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G55" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I55" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N55" t="s">
-        <v>197</v>
+        <v>145</v>
       </c>
       <c r="O55" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P55">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="Q55" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E56" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F56" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G56" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H56" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I56" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J56" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N56" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="O56" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P56">
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="Q56" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D57" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E57" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F57" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G57" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="H57" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J57" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N57" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="O57" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P57">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="Q57" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E58" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G58" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M58" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N58" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="O58" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P58">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q58" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E59" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G59" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M59" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N59" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="O59" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P59">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q59" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E60" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G60" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N60" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="O60" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P60">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="Q60" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C61" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" t="s">
+        <v>122</v>
+      </c>
+      <c r="F61" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" t="s">
         <v>126</v>
       </c>
-      <c r="D61" t="s">
-        <v>65</v>
-      </c>
-      <c r="E61" t="s">
-        <v>129</v>
-      </c>
-      <c r="F61" t="s">
-        <v>64</v>
-      </c>
-      <c r="G61" t="s">
-        <v>131</v>
-      </c>
       <c r="H61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J61" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M61" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N61" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="O61" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P61">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="Q61" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D62" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E62" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G62" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H62" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M62" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N62" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="O62" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P62">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="Q62" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E63" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G63" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="H63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>46</v>
+        <v>192</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M63" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N63" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="O63" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="P63">
-        <v>2500</v>
+        <v>50</v>
       </c>
       <c r="Q63" t="s">
-        <v>199</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" t="s">
+        <v>63</v>
+      </c>
+      <c r="E64" t="s">
+        <v>122</v>
+      </c>
+      <c r="F64" t="s">
+        <v>62</v>
+      </c>
+      <c r="G64" t="s">
+        <v>125</v>
+      </c>
+      <c r="H64" t="s">
+        <v>63</v>
+      </c>
+      <c r="I64" t="s">
+        <v>60</v>
+      </c>
+      <c r="J64" t="s">
+        <v>62</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M64" t="s">
+        <v>64</v>
+      </c>
+      <c r="N64" t="s">
+        <v>130</v>
+      </c>
+      <c r="O64" t="s">
+        <v>190</v>
+      </c>
+      <c r="P64">
+        <v>200</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" t="s">
+        <v>122</v>
+      </c>
+      <c r="F65" t="s">
+        <v>62</v>
+      </c>
+      <c r="G65" t="s">
+        <v>125</v>
+      </c>
+      <c r="H65" t="s">
+        <v>63</v>
+      </c>
+      <c r="I65" t="s">
+        <v>60</v>
+      </c>
+      <c r="J65" t="s">
+        <v>62</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M65" t="s">
+        <v>64</v>
+      </c>
+      <c r="N65" t="s">
+        <v>167</v>
+      </c>
+      <c r="O65" t="s">
+        <v>190</v>
+      </c>
+      <c r="P65">
+        <v>50000</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" t="s">
+        <v>62</v>
+      </c>
+      <c r="C66" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" t="s">
+        <v>122</v>
+      </c>
+      <c r="F66" t="s">
+        <v>62</v>
+      </c>
+      <c r="G66" t="s">
+        <v>125</v>
+      </c>
+      <c r="H66" t="s">
+        <v>63</v>
+      </c>
+      <c r="I66" t="s">
+        <v>60</v>
+      </c>
+      <c r="J66" t="s">
+        <v>62</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M66" t="s">
+        <v>64</v>
+      </c>
+      <c r="N66" t="s">
+        <v>162</v>
+      </c>
+      <c r="O66" t="s">
+        <v>190</v>
+      </c>
+      <c r="P66">
+        <v>500000</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed game to work in single player
</commit_message>
<xml_diff>
--- a/HutListe.xlsx
+++ b/HutListe.xlsx
@@ -953,42 +953,9 @@
     <t>Preis</t>
   </si>
   <si>
-    <t>Spalte1</t>
-  </si>
-  <si>
-    <t>Spalte2</t>
-  </si>
-  <si>
-    <t>Spalte3</t>
-  </si>
-  <si>
     <t>Spalte4</t>
   </si>
   <si>
-    <t>Spalte5</t>
-  </si>
-  <si>
-    <t>Spalte6</t>
-  </si>
-  <si>
-    <t>Spalte7</t>
-  </si>
-  <si>
-    <t>Spalte8</t>
-  </si>
-  <si>
-    <t>Spalte9</t>
-  </si>
-  <si>
-    <t>Spalte10</t>
-  </si>
-  <si>
-    <t>Spalte11</t>
-  </si>
-  <si>
-    <t>Spalte12</t>
-  </si>
-  <si>
     <t>_SPECIAL_</t>
   </si>
   <si>
@@ -1032,6 +999,39 @@
   </si>
   <si>
     <t>Da spielt jemand mit richtig viel!</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Q</t>
   </si>
 </sst>
 </file>
@@ -1155,23 +1155,23 @@
     <sortCondition ref="G1:G63"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" name="Spalte1"/>
-    <tableColumn id="2" name="Spalte2"/>
+    <tableColumn id="1" name="A"/>
+    <tableColumn id="2" name="B"/>
     <tableColumn id="3" name="ID"/>
-    <tableColumn id="4" name="Spalte3"/>
+    <tableColumn id="4" name="D"/>
     <tableColumn id="5" name="Spalte4"/>
-    <tableColumn id="6" name="Spalte5"/>
+    <tableColumn id="6" name="F"/>
     <tableColumn id="7" name="Kategorie"/>
-    <tableColumn id="8" name="Spalte6"/>
-    <tableColumn id="9" name="Spalte7"/>
-    <tableColumn id="10" name="Spalte8"/>
+    <tableColumn id="8" name="H"/>
+    <tableColumn id="9" name="I"/>
+    <tableColumn id="10" name="J"/>
     <tableColumn id="11" name="Bild" dataDxfId="1"/>
-    <tableColumn id="12" name="Spalte9" dataDxfId="0"/>
-    <tableColumn id="13" name="Spalte10"/>
+    <tableColumn id="12" name="L" dataDxfId="0"/>
+    <tableColumn id="13" name="M"/>
     <tableColumn id="14" name="Beschreibung"/>
-    <tableColumn id="15" name="Spalte11"/>
+    <tableColumn id="15" name="O"/>
     <tableColumn id="16" name="Preis"/>
-    <tableColumn id="17" name="Spalte12"/>
+    <tableColumn id="17" name="Q"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1443,67 +1443,79 @@
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="45.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" style="2"/>
+    <col min="12" max="12" width="4.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.21875" customWidth="1"/>
+    <col min="15" max="15" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
         <v>195</v>
       </c>
       <c r="D1" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="E1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F1" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="G1" t="s">
         <v>194</v>
       </c>
       <c r="H1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="I1" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="J1" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>196</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="M1" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="N1" t="s">
         <v>197</v>
       </c>
       <c r="O1" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="P1" t="s">
         <v>198</v>
       </c>
       <c r="Q1" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1514,7 +1526,7 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -1526,7 +1538,7 @@
         <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H2" t="s">
         <v>63</v>
@@ -1567,7 +1579,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -1579,7 +1591,7 @@
         <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H3" t="s">
         <v>63</v>
@@ -1620,7 +1632,7 @@
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
@@ -1632,7 +1644,7 @@
         <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H4" t="s">
         <v>63</v>
@@ -1673,7 +1685,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
@@ -1685,7 +1697,7 @@
         <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H5" t="s">
         <v>63</v>
@@ -1726,7 +1738,7 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -1738,7 +1750,7 @@
         <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H6" t="s">
         <v>63</v>
@@ -1779,7 +1791,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -1791,7 +1803,7 @@
         <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H7" t="s">
         <v>63</v>
@@ -1832,7 +1844,7 @@
         <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -1844,7 +1856,7 @@
         <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H8" t="s">
         <v>63</v>
@@ -1885,7 +1897,7 @@
         <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -3128,7 +3140,7 @@
         <v>62</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>63</v>
@@ -3137,7 +3149,7 @@
         <v>64</v>
       </c>
       <c r="N32" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="O32" t="s">
         <v>190</v>
@@ -3181,7 +3193,7 @@
         <v>62</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>63</v>
@@ -3190,7 +3202,7 @@
         <v>64</v>
       </c>
       <c r="N33" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="O33" t="s">
         <v>190</v>
@@ -3234,7 +3246,7 @@
         <v>62</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>63</v>
@@ -3243,7 +3255,7 @@
         <v>64</v>
       </c>
       <c r="N34" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="O34" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
added a lot of new hats
</commit_message>
<xml_diff>
--- a/HutListe.xlsx
+++ b/HutListe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="302">
   <si>
     <t>states/schaf.png</t>
   </si>
@@ -846,9 +846,6 @@
     <t>Jeder echte Fußballfan hat das!</t>
   </si>
   <si>
-    <t>Eine Belohnung für tolles Spielen!</t>
-  </si>
-  <si>
     <t>Damit kann man winken!</t>
   </si>
   <si>
@@ -861,9 +858,6 @@
     <t>Für Leute die nicht gerne alleine sind!</t>
   </si>
   <si>
-    <t>Dieses Symbol haben nur Gewinner!</t>
-  </si>
-  <si>
     <t>Dieses Symbol bekommen nur die Besten der Besten!</t>
   </si>
   <si>
@@ -1027,13 +1021,247 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>b01</t>
+  </si>
+  <si>
+    <t>b02</t>
+  </si>
+  <si>
+    <t>b03</t>
+  </si>
+  <si>
+    <t>b04</t>
+  </si>
+  <si>
+    <t>b05</t>
+  </si>
+  <si>
+    <t>b06</t>
+  </si>
+  <si>
+    <t>Damit fühlst du dich wohl wie ein Fisch in Wasser!</t>
+  </si>
+  <si>
+    <t>Nachtaktiv!</t>
+  </si>
+  <si>
+    <t>Der Gejagte? Oder der Jäger?</t>
+  </si>
+  <si>
+    <t>Quaak!</t>
+  </si>
+  <si>
+    <t>Damit zeigst du dass du so richtig gemütlich, und kuschelig bist!</t>
+  </si>
+  <si>
+    <t>Nur für Leute mit der richtigen Tankfüllung!</t>
+  </si>
+  <si>
+    <t>b07</t>
+  </si>
+  <si>
+    <t>b08</t>
+  </si>
+  <si>
+    <t>Hiermit kannst du auch das Kleingedruckte lesen!</t>
+  </si>
+  <si>
+    <t>b09</t>
+  </si>
+  <si>
+    <t>b10</t>
+  </si>
+  <si>
+    <t>b11</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>b13</t>
+  </si>
+  <si>
+    <t>b14</t>
+  </si>
+  <si>
+    <t>Erreicht wenn du 1.000 Punkte in der Saison März geschafft hast.</t>
+  </si>
+  <si>
+    <t>Belohnung für die Besten am Ende einer Saison!</t>
+  </si>
+  <si>
+    <t>Damit kannst du allen zeigen, dass du auch richtig gut in Knuddelonia bist!</t>
+  </si>
+  <si>
+    <t>Gesundheit!</t>
+  </si>
+  <si>
+    <t>Wartest du darauf aufgeschlossen zu werden, oder bist du einfach nur verschlossen?</t>
+  </si>
+  <si>
+    <t>Du bist ein echtes Geschenk vom Himmel!</t>
+  </si>
+  <si>
+    <t>Purer Spaß beim Baden!</t>
+  </si>
+  <si>
+    <t>b15</t>
+  </si>
+  <si>
+    <t>b16</t>
+  </si>
+  <si>
+    <t>b17</t>
+  </si>
+  <si>
+    <t>b18</t>
+  </si>
+  <si>
+    <t>b19</t>
+  </si>
+  <si>
+    <t>Rebel without a cause !</t>
+  </si>
+  <si>
+    <t>Hier wird's härter!</t>
+  </si>
+  <si>
+    <t>Du hast noch ein Zeitungsabo!</t>
+  </si>
+  <si>
+    <t>Die Brille verschafft dir den Durchblick!</t>
+  </si>
+  <si>
+    <t>Du weißt auch nicht so recht, was das soll. Wie geht das schon wieder?</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison April.</t>
+  </si>
+  <si>
+    <t>b20</t>
+  </si>
+  <si>
+    <t>b21</t>
+  </si>
+  <si>
+    <t>b22</t>
+  </si>
+  <si>
+    <t>b23</t>
+  </si>
+  <si>
+    <t>Grün ist einfach die beste Farbe!</t>
+  </si>
+  <si>
+    <t>Hier wird scharf geschossen!</t>
+  </si>
+  <si>
+    <t>Das Torten-Katapult!</t>
+  </si>
+  <si>
+    <t>Damit sitzt du schon fast auf einem Thron.</t>
+  </si>
+  <si>
+    <t>b24</t>
+  </si>
+  <si>
+    <t>b25</t>
+  </si>
+  <si>
+    <t>Du bist ein begeistert vom Box-Sport!</t>
+  </si>
+  <si>
+    <t>Damit behälst du alle im Blick!</t>
+  </si>
+  <si>
+    <t>Wichtig ist nur, dass du nicht aus dem Bildschirm fällst!</t>
+  </si>
+  <si>
+    <t>Buntes</t>
+  </si>
+  <si>
+    <t>pics/fisch.gif</t>
+  </si>
+  <si>
+    <t>pics/fledermaus.gif</t>
+  </si>
+  <si>
+    <t>pics/hai.gif</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_14-03_costumes_frog.png</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_14-03_costumes_panda.png</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_14-03_costumes_tiger.png</t>
+  </si>
+  <si>
+    <t>pics/icon_magnifying_glass.my_2.gif</t>
+  </si>
+  <si>
+    <t>pics/mumie.gif</t>
+  </si>
+  <si>
+    <t>pics/nose.gif</t>
+  </si>
+  <si>
+    <t>pics/padlock.gif</t>
+  </si>
+  <si>
+    <t>pics/present_2.gif</t>
+  </si>
+  <si>
+    <t>pics/quietscheente.png</t>
+  </si>
+  <si>
+    <t>pics/sm_14.gif</t>
+  </si>
+  <si>
+    <t>pics/sm_667.gif</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_11-04_break.gif</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_13-04_nerd.gif</t>
+  </si>
+  <si>
+    <t>pics/sm_abo-wlcm2012_UNKNOWN.gif</t>
+  </si>
+  <si>
+    <t>pics/sm_cardsB_03b.b.my_11.h_27.gif</t>
+  </si>
+  <si>
+    <t>pics/sm_creep.b.gif</t>
+  </si>
+  <si>
+    <t>pics/snowfight_cannon.png</t>
+  </si>
+  <si>
+    <t>pics/snowfight_catapult.png</t>
+  </si>
+  <si>
+    <t>pics/smileywars/icon_skills_king_001.png</t>
+  </si>
+  <si>
+    <t>pics/smileywars/icons_skills_attackdistance-1.png</t>
+  </si>
+  <si>
+    <t>pics/smileywars/icons_skills_sightdistance.png</t>
+  </si>
+  <si>
+    <t>pics/smileywars/chat_toggle_sticky-enabled.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,6 +1290,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1083,12 +1318,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1144,10 +1383,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:Q66" totalsRowShown="0">
-  <autoFilter ref="A1:Q66"/>
-  <sortState ref="A2:Q66">
-    <sortCondition ref="G1:G66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:Q92" totalsRowShown="0">
+  <autoFilter ref="A1:Q92"/>
+  <sortState ref="A2:Q92">
+    <sortCondition ref="G1:G92"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" name="A"/>
@@ -1427,7 +1666,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1435,10 +1674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="A2" sqref="A2:Q91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1460,57 +1699,57 @@
     <col min="17" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
         <v>215</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" t="s">
         <v>216</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="M1" t="s">
+        <v>221</v>
+      </c>
+      <c r="N1" t="s">
         <v>195</v>
       </c>
-      <c r="D1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I1" t="s">
-        <v>221</v>
-      </c>
-      <c r="J1" t="s">
-        <v>220</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" t="s">
+        <v>222</v>
+      </c>
+      <c r="P1" t="s">
         <v>196</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>223</v>
-      </c>
-      <c r="N1" t="s">
-        <v>197</v>
-      </c>
-      <c r="O1" t="s">
-        <v>224</v>
-      </c>
-      <c r="P1" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1521,7 +1760,7 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -1533,7 +1772,7 @@
         <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H2" t="s">
         <v>63</v>
@@ -1545,7 +1784,7 @@
         <v>62</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>63</v>
@@ -1557,13 +1796,13 @@
         <v>132</v>
       </c>
       <c r="O2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1574,7 +1813,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -1586,7 +1825,7 @@
         <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H3" t="s">
         <v>63</v>
@@ -1607,16 +1846,16 @@
         <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>165</v>
+        <v>245</v>
       </c>
       <c r="O3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1627,7 +1866,7 @@
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
@@ -1639,7 +1878,7 @@
         <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H4" t="s">
         <v>63</v>
@@ -1660,16 +1899,16 @@
         <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="O4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1680,7 +1919,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
@@ -1692,7 +1931,7 @@
         <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H5" t="s">
         <v>63</v>
@@ -1713,16 +1952,16 @@
         <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="O5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1733,7 +1972,7 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -1745,7 +1984,7 @@
         <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H6" t="s">
         <v>63</v>
@@ -1766,16 +2005,16 @@
         <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1786,7 +2025,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -1798,7 +2037,7 @@
         <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H7" t="s">
         <v>63</v>
@@ -1819,16 +2058,16 @@
         <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="O7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1839,7 +2078,7 @@
         <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -1851,7 +2090,7 @@
         <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H8" t="s">
         <v>63</v>
@@ -1872,16 +2111,16 @@
         <v>64</v>
       </c>
       <c r="N8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="O8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1892,7 +2131,7 @@
         <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>208</v>
+        <v>255</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -1904,7 +2143,7 @@
         <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>124</v>
+        <v>198</v>
       </c>
       <c r="H9" t="s">
         <v>63</v>
@@ -1915,8 +2154,8 @@
       <c r="J9" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>27</v>
+      <c r="K9" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>63</v>
@@ -1925,16 +2164,16 @@
         <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>139</v>
+        <v>262</v>
       </c>
       <c r="O9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P9">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1945,7 +2184,7 @@
         <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>206</v>
       </c>
       <c r="D10" t="s">
         <v>63</v>
@@ -1969,7 +2208,7 @@
         <v>62</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>63</v>
@@ -1978,16 +2217,16 @@
         <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P10">
         <v>25</v>
       </c>
       <c r="Q10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1998,7 +2237,7 @@
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
         <v>63</v>
@@ -2022,7 +2261,7 @@
         <v>62</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>63</v>
@@ -2031,16 +2270,16 @@
         <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P11">
         <v>25</v>
       </c>
       <c r="Q11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -2051,7 +2290,7 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
@@ -2075,7 +2314,7 @@
         <v>62</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>63</v>
@@ -2084,16 +2323,16 @@
         <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P12">
         <v>25</v>
       </c>
       <c r="Q12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -2104,7 +2343,7 @@
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
@@ -2128,7 +2367,7 @@
         <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>63</v>
@@ -2137,16 +2376,16 @@
         <v>64</v>
       </c>
       <c r="N13" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P13">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -2157,7 +2396,7 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
@@ -2181,7 +2420,7 @@
         <v>62</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>63</v>
@@ -2190,16 +2429,16 @@
         <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P14">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -2210,7 +2449,7 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
         <v>63</v>
@@ -2234,7 +2473,7 @@
         <v>62</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>63</v>
@@ -2243,16 +2482,16 @@
         <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="O15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P15">
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="Q15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -2263,7 +2502,7 @@
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>254</v>
       </c>
       <c r="D16" t="s">
         <v>63</v>
@@ -2286,8 +2525,8 @@
       <c r="J16" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>34</v>
+      <c r="K16" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>63</v>
@@ -2296,16 +2535,16 @@
         <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>160</v>
+        <v>261</v>
       </c>
       <c r="O16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P16">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="Q16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -2316,7 +2555,7 @@
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>272</v>
       </c>
       <c r="D17" t="s">
         <v>63</v>
@@ -2328,7 +2567,7 @@
         <v>62</v>
       </c>
       <c r="G17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H17" t="s">
         <v>63</v>
@@ -2339,8 +2578,8 @@
       <c r="J17" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>1</v>
+      <c r="K17" s="3" t="s">
+        <v>301</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>63</v>
@@ -2349,16 +2588,16 @@
         <v>64</v>
       </c>
       <c r="N17" t="s">
-        <v>133</v>
+        <v>275</v>
       </c>
       <c r="O17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P17">
-        <v>50</v>
+        <v>2500</v>
       </c>
       <c r="Q17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2369,7 +2608,7 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
         <v>63</v>
@@ -2381,7 +2620,7 @@
         <v>62</v>
       </c>
       <c r="G18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H18" t="s">
         <v>63</v>
@@ -2393,7 +2632,7 @@
         <v>62</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>63</v>
@@ -2402,16 +2641,16 @@
         <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="O18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P18">
-        <v>1000</v>
+        <v>5000</v>
       </c>
       <c r="Q18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2422,7 +2661,7 @@
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>236</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -2434,7 +2673,7 @@
         <v>62</v>
       </c>
       <c r="G19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H19" t="s">
         <v>63</v>
@@ -2445,8 +2684,8 @@
       <c r="J19" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>24</v>
+      <c r="K19" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>63</v>
@@ -2455,16 +2694,16 @@
         <v>64</v>
       </c>
       <c r="N19" t="s">
-        <v>164</v>
+        <v>238</v>
       </c>
       <c r="O19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P19">
-        <v>5000</v>
+        <v>7500</v>
       </c>
       <c r="Q19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2475,7 +2714,7 @@
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
@@ -2487,7 +2726,7 @@
         <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H20" t="s">
         <v>63</v>
@@ -2499,7 +2738,7 @@
         <v>62</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>63</v>
@@ -2508,16 +2747,16 @@
         <v>64</v>
       </c>
       <c r="N20" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="O20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P20">
         <v>10000</v>
       </c>
       <c r="Q20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2528,7 +2767,7 @@
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>240</v>
       </c>
       <c r="D21" t="s">
         <v>63</v>
@@ -2540,7 +2779,7 @@
         <v>62</v>
       </c>
       <c r="G21" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H21" t="s">
         <v>63</v>
@@ -2551,8 +2790,8 @@
       <c r="J21" t="s">
         <v>62</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>38</v>
+      <c r="K21" s="4" t="s">
+        <v>286</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>63</v>
@@ -2561,16 +2800,16 @@
         <v>64</v>
       </c>
       <c r="N21" t="s">
-        <v>169</v>
+        <v>249</v>
       </c>
       <c r="O21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P21">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="Q21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2581,7 +2820,7 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
         <v>63</v>
@@ -2605,7 +2844,7 @@
         <v>62</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>63</v>
@@ -2614,16 +2853,16 @@
         <v>64</v>
       </c>
       <c r="N22" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="O22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P22">
-        <v>100000</v>
+        <v>50</v>
       </c>
       <c r="Q22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -2634,7 +2873,7 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>237</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
@@ -2657,8 +2896,8 @@
       <c r="J23" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>44</v>
+      <c r="K23" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>63</v>
@@ -2667,16 +2906,16 @@
         <v>64</v>
       </c>
       <c r="N23" t="s">
-        <v>175</v>
+        <v>247</v>
       </c>
       <c r="O23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P23">
-        <v>500000</v>
+        <v>500</v>
       </c>
       <c r="Q23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -2687,7 +2926,7 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
@@ -2711,7 +2950,7 @@
         <v>62</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>63</v>
@@ -2720,16 +2959,16 @@
         <v>64</v>
       </c>
       <c r="N24" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P24">
-        <v>1000000</v>
+        <v>1000</v>
       </c>
       <c r="Q24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -2740,7 +2979,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>243</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -2763,8 +3002,8 @@
       <c r="J25" t="s">
         <v>62</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>35</v>
+      <c r="K25" s="4" t="s">
+        <v>289</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>63</v>
@@ -2773,16 +3012,16 @@
         <v>64</v>
       </c>
       <c r="N25" t="s">
-        <v>161</v>
+        <v>257</v>
       </c>
       <c r="O25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P25">
-        <v>10000000</v>
+        <v>2500</v>
       </c>
       <c r="Q25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -2793,7 +3032,7 @@
         <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
         <v>63</v>
@@ -2817,7 +3056,7 @@
         <v>62</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>63</v>
@@ -2826,16 +3065,16 @@
         <v>64</v>
       </c>
       <c r="N26" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="O26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P26">
-        <v>100000000</v>
+        <v>5000</v>
       </c>
       <c r="Q26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -2846,7 +3085,7 @@
         <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>266</v>
       </c>
       <c r="D27" t="s">
         <v>63</v>
@@ -2858,7 +3097,7 @@
         <v>62</v>
       </c>
       <c r="G27" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H27" t="s">
         <v>63</v>
@@ -2869,8 +3108,8 @@
       <c r="J27" t="s">
         <v>62</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>2</v>
+      <c r="K27" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>63</v>
@@ -2879,16 +3118,16 @@
         <v>64</v>
       </c>
       <c r="N27" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="O27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P27">
-        <v>1</v>
+        <v>7500</v>
       </c>
       <c r="Q27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -2899,7 +3138,7 @@
         <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
         <v>63</v>
@@ -2911,7 +3150,7 @@
         <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H28" t="s">
         <v>63</v>
@@ -2923,7 +3162,7 @@
         <v>62</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>63</v>
@@ -2932,16 +3171,16 @@
         <v>64</v>
       </c>
       <c r="N28" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="O28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P28">
-        <v>5</v>
+        <v>10000</v>
       </c>
       <c r="Q28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -2952,7 +3191,7 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>253</v>
       </c>
       <c r="D29" t="s">
         <v>63</v>
@@ -2964,7 +3203,7 @@
         <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H29" t="s">
         <v>63</v>
@@ -2975,8 +3214,8 @@
       <c r="J29" t="s">
         <v>62</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>3</v>
+      <c r="K29" s="3" t="s">
+        <v>292</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>63</v>
@@ -2985,16 +3224,16 @@
         <v>64</v>
       </c>
       <c r="N29" t="s">
-        <v>135</v>
+        <v>260</v>
       </c>
       <c r="O29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P29">
-        <v>10</v>
+        <v>25000</v>
       </c>
       <c r="Q29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -3005,7 +3244,7 @@
         <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
         <v>63</v>
@@ -3017,7 +3256,7 @@
         <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H30" t="s">
         <v>63</v>
@@ -3029,7 +3268,7 @@
         <v>62</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>63</v>
@@ -3038,16 +3277,16 @@
         <v>64</v>
       </c>
       <c r="N30" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="O30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P30">
-        <v>20</v>
+        <v>50000</v>
       </c>
       <c r="Q30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -3058,7 +3297,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>265</v>
       </c>
       <c r="D31" t="s">
         <v>63</v>
@@ -3070,7 +3309,7 @@
         <v>62</v>
       </c>
       <c r="G31" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H31" t="s">
         <v>63</v>
@@ -3081,8 +3320,8 @@
       <c r="J31" t="s">
         <v>62</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>5</v>
+      <c r="K31" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>63</v>
@@ -3091,16 +3330,16 @@
         <v>64</v>
       </c>
       <c r="N31" t="s">
-        <v>137</v>
+        <v>270</v>
       </c>
       <c r="O31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P31">
-        <v>25</v>
+        <v>75000</v>
       </c>
       <c r="Q31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -3111,7 +3350,7 @@
         <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
         <v>63</v>
@@ -3123,7 +3362,7 @@
         <v>62</v>
       </c>
       <c r="G32" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H32" t="s">
         <v>63</v>
@@ -3135,7 +3374,7 @@
         <v>62</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>63</v>
@@ -3144,16 +3383,16 @@
         <v>64</v>
       </c>
       <c r="N32" t="s">
-        <v>210</v>
+        <v>146</v>
       </c>
       <c r="O32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P32">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="Q32" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -3164,7 +3403,7 @@
         <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D33" t="s">
         <v>63</v>
@@ -3176,7 +3415,7 @@
         <v>62</v>
       </c>
       <c r="G33" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H33" t="s">
         <v>63</v>
@@ -3188,7 +3427,7 @@
         <v>62</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>212</v>
+        <v>44</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>63</v>
@@ -3197,16 +3436,16 @@
         <v>64</v>
       </c>
       <c r="N33" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="O33" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P33">
-        <v>500</v>
+        <v>250000</v>
       </c>
       <c r="Q33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -3217,7 +3456,7 @@
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D34" t="s">
         <v>63</v>
@@ -3229,7 +3468,7 @@
         <v>62</v>
       </c>
       <c r="G34" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H34" t="s">
         <v>63</v>
@@ -3241,7 +3480,7 @@
         <v>62</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>213</v>
+        <v>9</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>63</v>
@@ -3250,16 +3489,16 @@
         <v>64</v>
       </c>
       <c r="N34" t="s">
-        <v>214</v>
+        <v>147</v>
       </c>
       <c r="O34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P34">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="Q34" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -3270,7 +3509,7 @@
         <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>244</v>
       </c>
       <c r="D35" t="s">
         <v>63</v>
@@ -3282,7 +3521,7 @@
         <v>62</v>
       </c>
       <c r="G35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H35" t="s">
         <v>63</v>
@@ -3293,8 +3532,8 @@
       <c r="J35" t="s">
         <v>62</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>45</v>
+      <c r="K35" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>63</v>
@@ -3303,16 +3542,16 @@
         <v>64</v>
       </c>
       <c r="N35" t="s">
-        <v>176</v>
+        <v>258</v>
       </c>
       <c r="O35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P35">
-        <v>10</v>
+        <v>750000</v>
       </c>
       <c r="Q35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -3323,7 +3562,7 @@
         <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>
@@ -3335,7 +3574,7 @@
         <v>62</v>
       </c>
       <c r="G36" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H36" t="s">
         <v>63</v>
@@ -3347,7 +3586,7 @@
         <v>62</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>63</v>
@@ -3356,16 +3595,16 @@
         <v>64</v>
       </c>
       <c r="N36" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="O36" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P36">
-        <v>150</v>
+        <v>1000000</v>
       </c>
       <c r="Q36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -3376,7 +3615,7 @@
         <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
         <v>63</v>
@@ -3388,7 +3627,7 @@
         <v>62</v>
       </c>
       <c r="G37" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H37" t="s">
         <v>63</v>
@@ -3400,7 +3639,7 @@
         <v>62</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>63</v>
@@ -3409,16 +3648,16 @@
         <v>64</v>
       </c>
       <c r="N37" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="O37" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P37">
-        <v>150</v>
+        <v>2500000</v>
       </c>
       <c r="Q37" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -3429,7 +3668,7 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>264</v>
       </c>
       <c r="D38" t="s">
         <v>63</v>
@@ -3441,7 +3680,7 @@
         <v>62</v>
       </c>
       <c r="G38" t="s">
-        <v>128</v>
+        <v>276</v>
       </c>
       <c r="H38" t="s">
         <v>63</v>
@@ -3452,8 +3691,8 @@
       <c r="J38" t="s">
         <v>62</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>54</v>
+      <c r="K38" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>63</v>
@@ -3462,16 +3701,16 @@
         <v>64</v>
       </c>
       <c r="N38" t="s">
-        <v>183</v>
+        <v>269</v>
       </c>
       <c r="O38" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P38">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="Q38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -3482,7 +3721,7 @@
         <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>239</v>
       </c>
       <c r="D39" t="s">
         <v>63</v>
@@ -3494,7 +3733,7 @@
         <v>62</v>
       </c>
       <c r="G39" t="s">
-        <v>128</v>
+        <v>276</v>
       </c>
       <c r="H39" t="s">
         <v>63</v>
@@ -3505,8 +3744,8 @@
       <c r="J39" t="s">
         <v>62</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>56</v>
+      <c r="K39" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>63</v>
@@ -3515,16 +3754,16 @@
         <v>64</v>
       </c>
       <c r="N39" t="s">
-        <v>185</v>
+        <v>248</v>
       </c>
       <c r="O39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P39">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="Q39" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -3535,7 +3774,7 @@
         <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>241</v>
       </c>
       <c r="D40" t="s">
         <v>63</v>
@@ -3547,7 +3786,7 @@
         <v>62</v>
       </c>
       <c r="G40" t="s">
-        <v>128</v>
+        <v>276</v>
       </c>
       <c r="H40" t="s">
         <v>63</v>
@@ -3558,8 +3797,8 @@
       <c r="J40" t="s">
         <v>62</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>51</v>
+      <c r="K40" s="4" t="s">
+        <v>287</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>63</v>
@@ -3568,16 +3807,16 @@
         <v>64</v>
       </c>
       <c r="N40" t="s">
-        <v>180</v>
+        <v>250</v>
       </c>
       <c r="O40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P40">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="Q40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -3588,7 +3827,7 @@
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>263</v>
       </c>
       <c r="D41" t="s">
         <v>63</v>
@@ -3600,7 +3839,7 @@
         <v>62</v>
       </c>
       <c r="G41" t="s">
-        <v>128</v>
+        <v>276</v>
       </c>
       <c r="H41" t="s">
         <v>63</v>
@@ -3611,8 +3850,8 @@
       <c r="J41" t="s">
         <v>62</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>46</v>
+      <c r="K41" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>63</v>
@@ -3621,16 +3860,16 @@
         <v>64</v>
       </c>
       <c r="N41" t="s">
-        <v>189</v>
+        <v>268</v>
       </c>
       <c r="O41" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P41">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="Q41" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -3641,7 +3880,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>271</v>
       </c>
       <c r="D42" t="s">
         <v>63</v>
@@ -3653,7 +3892,7 @@
         <v>62</v>
       </c>
       <c r="G42" t="s">
-        <v>128</v>
+        <v>276</v>
       </c>
       <c r="H42" t="s">
         <v>63</v>
@@ -3664,8 +3903,8 @@
       <c r="J42" t="s">
         <v>62</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>52</v>
+      <c r="K42" s="3" t="s">
+        <v>300</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>63</v>
@@ -3674,16 +3913,16 @@
         <v>64</v>
       </c>
       <c r="N42" t="s">
-        <v>181</v>
+        <v>274</v>
       </c>
       <c r="O42" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P42">
-        <v>1000</v>
+        <v>7500</v>
       </c>
       <c r="Q42" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -3694,7 +3933,7 @@
         <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>242</v>
       </c>
       <c r="D43" t="s">
         <v>63</v>
@@ -3706,7 +3945,7 @@
         <v>62</v>
       </c>
       <c r="G43" t="s">
-        <v>128</v>
+        <v>276</v>
       </c>
       <c r="H43" t="s">
         <v>63</v>
@@ -3717,8 +3956,8 @@
       <c r="J43" t="s">
         <v>62</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>53</v>
+      <c r="K43" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>63</v>
@@ -3727,16 +3966,16 @@
         <v>64</v>
       </c>
       <c r="N43" t="s">
-        <v>182</v>
+        <v>251</v>
       </c>
       <c r="O43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P43">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="Q43" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -3747,7 +3986,7 @@
         <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="D44" t="s">
         <v>63</v>
@@ -3759,7 +3998,7 @@
         <v>62</v>
       </c>
       <c r="G44" t="s">
-        <v>128</v>
+        <v>276</v>
       </c>
       <c r="H44" t="s">
         <v>63</v>
@@ -3770,8 +4009,8 @@
       <c r="J44" t="s">
         <v>62</v>
       </c>
-      <c r="K44" s="1" t="s">
-        <v>57</v>
+      <c r="K44" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>63</v>
@@ -3780,16 +4019,16 @@
         <v>64</v>
       </c>
       <c r="N44" t="s">
-        <v>186</v>
+        <v>259</v>
       </c>
       <c r="O44" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P44">
-        <v>2500</v>
+        <v>25000</v>
       </c>
       <c r="Q44" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -3800,7 +4039,7 @@
         <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>256</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -3812,7 +4051,7 @@
         <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>128</v>
+        <v>276</v>
       </c>
       <c r="H45" t="s">
         <v>63</v>
@@ -3823,8 +4062,8 @@
       <c r="J45" t="s">
         <v>62</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>59</v>
+      <c r="K45" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>63</v>
@@ -3833,16 +4072,16 @@
         <v>64</v>
       </c>
       <c r="N45" t="s">
-        <v>187</v>
+        <v>267</v>
       </c>
       <c r="O45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P45">
-        <v>2500</v>
+        <v>50000</v>
       </c>
       <c r="Q45" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -3853,7 +4092,7 @@
         <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s">
         <v>63</v>
@@ -3865,7 +4104,7 @@
         <v>62</v>
       </c>
       <c r="G46" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H46" t="s">
         <v>63</v>
@@ -3877,7 +4116,7 @@
         <v>62</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>63</v>
@@ -3886,16 +4125,16 @@
         <v>64</v>
       </c>
       <c r="N46" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="O46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P46">
-        <v>5000</v>
+        <v>1</v>
       </c>
       <c r="Q46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -3906,7 +4145,7 @@
         <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D47" t="s">
         <v>63</v>
@@ -3918,7 +4157,7 @@
         <v>62</v>
       </c>
       <c r="G47" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H47" t="s">
         <v>63</v>
@@ -3930,7 +4169,7 @@
         <v>62</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>63</v>
@@ -3939,16 +4178,16 @@
         <v>64</v>
       </c>
       <c r="N47" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="O47" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P47">
-        <v>10000</v>
+        <v>5</v>
       </c>
       <c r="Q47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -3959,7 +4198,7 @@
         <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D48" t="s">
         <v>63</v>
@@ -3971,7 +4210,7 @@
         <v>62</v>
       </c>
       <c r="G48" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H48" t="s">
         <v>63</v>
@@ -3983,7 +4222,7 @@
         <v>62</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>63</v>
@@ -3992,16 +4231,16 @@
         <v>64</v>
       </c>
       <c r="N48" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="O48" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P48">
-        <v>50000</v>
+        <v>10</v>
       </c>
       <c r="Q48" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -4012,7 +4251,7 @@
         <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D49" t="s">
         <v>63</v>
@@ -4024,7 +4263,7 @@
         <v>62</v>
       </c>
       <c r="G49" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H49" t="s">
         <v>63</v>
@@ -4036,7 +4275,7 @@
         <v>62</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>63</v>
@@ -4045,16 +4284,16 @@
         <v>64</v>
       </c>
       <c r="N49" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="O49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P49">
-        <v>100000</v>
+        <v>20</v>
       </c>
       <c r="Q49" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -4065,7 +4304,7 @@
         <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
         <v>63</v>
@@ -4077,7 +4316,7 @@
         <v>62</v>
       </c>
       <c r="G50" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H50" t="s">
         <v>63</v>
@@ -4089,7 +4328,7 @@
         <v>62</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>63</v>
@@ -4098,16 +4337,16 @@
         <v>64</v>
       </c>
       <c r="N50" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="O50" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P50">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="Q50" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -4118,7 +4357,7 @@
         <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D51" t="s">
         <v>63</v>
@@ -4130,7 +4369,7 @@
         <v>62</v>
       </c>
       <c r="G51" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H51" t="s">
         <v>63</v>
@@ -4142,7 +4381,7 @@
         <v>62</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>13</v>
+        <v>207</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>63</v>
@@ -4151,16 +4390,16 @@
         <v>64</v>
       </c>
       <c r="N51" t="s">
-        <v>151</v>
+        <v>208</v>
       </c>
       <c r="O51" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P51">
         <v>100</v>
       </c>
       <c r="Q51" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -4171,7 +4410,7 @@
         <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="D52" t="s">
         <v>63</v>
@@ -4183,7 +4422,7 @@
         <v>62</v>
       </c>
       <c r="G52" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H52" t="s">
         <v>63</v>
@@ -4195,7 +4434,7 @@
         <v>62</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>16</v>
+        <v>210</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>63</v>
@@ -4204,16 +4443,16 @@
         <v>64</v>
       </c>
       <c r="N52" t="s">
-        <v>154</v>
+        <v>209</v>
       </c>
       <c r="O52" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P52">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="Q52" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -4224,7 +4463,7 @@
         <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D53" t="s">
         <v>63</v>
@@ -4236,7 +4475,7 @@
         <v>62</v>
       </c>
       <c r="G53" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H53" t="s">
         <v>63</v>
@@ -4248,7 +4487,7 @@
         <v>62</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>15</v>
+        <v>211</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>63</v>
@@ -4257,16 +4496,16 @@
         <v>64</v>
       </c>
       <c r="N53" t="s">
-        <v>153</v>
+        <v>212</v>
       </c>
       <c r="O53" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P53">
-        <v>500</v>
+        <v>1000000</v>
       </c>
       <c r="Q53" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
@@ -4277,7 +4516,7 @@
         <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="D54" t="s">
         <v>63</v>
@@ -4289,7 +4528,7 @@
         <v>62</v>
       </c>
       <c r="G54" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H54" t="s">
         <v>63</v>
@@ -4301,7 +4540,7 @@
         <v>62</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>63</v>
@@ -4310,16 +4549,16 @@
         <v>64</v>
       </c>
       <c r="N54" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="O54" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P54">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="Q54" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -4330,7 +4569,7 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="D55" t="s">
         <v>63</v>
@@ -4342,7 +4581,7 @@
         <v>62</v>
       </c>
       <c r="G55" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H55" t="s">
         <v>63</v>
@@ -4354,7 +4593,7 @@
         <v>62</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>63</v>
@@ -4363,16 +4602,16 @@
         <v>64</v>
       </c>
       <c r="N55" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="O55" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P55">
-        <v>2500</v>
+        <v>150</v>
       </c>
       <c r="Q55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -4383,7 +4622,7 @@
         <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D56" t="s">
         <v>63</v>
@@ -4395,7 +4634,7 @@
         <v>62</v>
       </c>
       <c r="G56" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H56" t="s">
         <v>63</v>
@@ -4407,7 +4646,7 @@
         <v>62</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>63</v>
@@ -4416,16 +4655,16 @@
         <v>64</v>
       </c>
       <c r="N56" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="O56" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P56">
-        <v>5000</v>
+        <v>150</v>
       </c>
       <c r="Q56" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -4436,7 +4675,7 @@
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D57" t="s">
         <v>63</v>
@@ -4448,7 +4687,7 @@
         <v>62</v>
       </c>
       <c r="G57" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H57" t="s">
         <v>63</v>
@@ -4460,7 +4699,7 @@
         <v>62</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>63</v>
@@ -4469,16 +4708,16 @@
         <v>64</v>
       </c>
       <c r="N57" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="O57" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P57">
-        <v>10000</v>
+        <v>250</v>
       </c>
       <c r="Q57" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -4489,7 +4728,7 @@
         <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D58" t="s">
         <v>63</v>
@@ -4501,7 +4740,7 @@
         <v>62</v>
       </c>
       <c r="G58" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H58" t="s">
         <v>63</v>
@@ -4513,7 +4752,7 @@
         <v>62</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>63</v>
@@ -4522,16 +4761,16 @@
         <v>64</v>
       </c>
       <c r="N58" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="O58" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P58">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="Q58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -4542,7 +4781,7 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D59" t="s">
         <v>63</v>
@@ -4554,7 +4793,7 @@
         <v>62</v>
       </c>
       <c r="G59" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H59" t="s">
         <v>63</v>
@@ -4566,7 +4805,7 @@
         <v>62</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>63</v>
@@ -4575,16 +4814,16 @@
         <v>64</v>
       </c>
       <c r="N59" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="O59" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P59">
         <v>500</v>
       </c>
       <c r="Q59" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -4595,7 +4834,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D60" t="s">
         <v>63</v>
@@ -4607,7 +4846,7 @@
         <v>62</v>
       </c>
       <c r="G60" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H60" t="s">
         <v>63</v>
@@ -4619,7 +4858,7 @@
         <v>62</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>63</v>
@@ -4628,16 +4867,16 @@
         <v>64</v>
       </c>
       <c r="N60" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="O60" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P60">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q60" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -4648,7 +4887,7 @@
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -4660,7 +4899,7 @@
         <v>62</v>
       </c>
       <c r="G61" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H61" t="s">
         <v>63</v>
@@ -4672,7 +4911,7 @@
         <v>62</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>63</v>
@@ -4681,16 +4920,16 @@
         <v>64</v>
       </c>
       <c r="N61" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="O61" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P61">
         <v>1000</v>
       </c>
       <c r="Q61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -4701,7 +4940,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="D62" t="s">
         <v>63</v>
@@ -4713,7 +4952,7 @@
         <v>62</v>
       </c>
       <c r="G62" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H62" t="s">
         <v>63</v>
@@ -4725,7 +4964,7 @@
         <v>62</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>63</v>
@@ -4734,16 +4973,16 @@
         <v>64</v>
       </c>
       <c r="N62" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="O62" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P62">
         <v>1000</v>
       </c>
       <c r="Q62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -4754,7 +4993,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="D63" t="s">
         <v>63</v>
@@ -4766,7 +5005,7 @@
         <v>62</v>
       </c>
       <c r="G63" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H63" t="s">
         <v>63</v>
@@ -4778,7 +5017,7 @@
         <v>62</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>192</v>
+        <v>57</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>63</v>
@@ -4787,16 +5026,16 @@
         <v>64</v>
       </c>
       <c r="N63" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="O63" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P63">
-        <v>50</v>
+        <v>2500</v>
       </c>
       <c r="Q63" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -4807,7 +5046,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
         <v>63</v>
@@ -4819,7 +5058,7 @@
         <v>62</v>
       </c>
       <c r="G64" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H64" t="s">
         <v>63</v>
@@ -4831,7 +5070,7 @@
         <v>62</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>63</v>
@@ -4840,16 +5079,16 @@
         <v>64</v>
       </c>
       <c r="N64" t="s">
-        <v>130</v>
+        <v>185</v>
       </c>
       <c r="O64" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P64">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="Q64" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -4860,7 +5099,7 @@
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="D65" t="s">
         <v>63</v>
@@ -4872,7 +5111,7 @@
         <v>62</v>
       </c>
       <c r="G65" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="H65" t="s">
         <v>63</v>
@@ -4884,7 +5123,7 @@
         <v>62</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>63</v>
@@ -4893,16 +5132,16 @@
         <v>64</v>
       </c>
       <c r="N65" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="O65" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P65">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="Q65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -4913,50 +5152,1379 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D66" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" t="s">
+        <v>122</v>
+      </c>
+      <c r="F66" t="s">
+        <v>62</v>
+      </c>
+      <c r="G66" t="s">
+        <v>128</v>
+      </c>
+      <c r="H66" t="s">
+        <v>63</v>
+      </c>
+      <c r="I66" t="s">
+        <v>60</v>
+      </c>
+      <c r="J66" t="s">
+        <v>62</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M66" t="s">
+        <v>64</v>
+      </c>
+      <c r="N66" t="s">
+        <v>186</v>
+      </c>
+      <c r="O66" t="s">
+        <v>188</v>
+      </c>
+      <c r="P66">
+        <v>10000</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" t="s">
+        <v>95</v>
+      </c>
+      <c r="D67" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" t="s">
+        <v>122</v>
+      </c>
+      <c r="F67" t="s">
+        <v>62</v>
+      </c>
+      <c r="G67" t="s">
+        <v>128</v>
+      </c>
+      <c r="H67" t="s">
+        <v>63</v>
+      </c>
+      <c r="I67" t="s">
+        <v>60</v>
+      </c>
+      <c r="J67" t="s">
+        <v>62</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M67" t="s">
+        <v>64</v>
+      </c>
+      <c r="N67" t="s">
+        <v>177</v>
+      </c>
+      <c r="O67" t="s">
+        <v>188</v>
+      </c>
+      <c r="P67">
+        <v>50000</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68" t="s">
+        <v>122</v>
+      </c>
+      <c r="F68" t="s">
+        <v>62</v>
+      </c>
+      <c r="G68" t="s">
+        <v>128</v>
+      </c>
+      <c r="H68" t="s">
+        <v>63</v>
+      </c>
+      <c r="I68" t="s">
+        <v>60</v>
+      </c>
+      <c r="J68" t="s">
+        <v>62</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M68" t="s">
+        <v>64</v>
+      </c>
+      <c r="N68" t="s">
+        <v>167</v>
+      </c>
+      <c r="O68" t="s">
+        <v>188</v>
+      </c>
+      <c r="P68">
+        <v>100000</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" t="s">
+        <v>63</v>
+      </c>
+      <c r="E69" t="s">
+        <v>122</v>
+      </c>
+      <c r="F69" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" t="s">
+        <v>127</v>
+      </c>
+      <c r="H69" t="s">
+        <v>63</v>
+      </c>
+      <c r="I69" t="s">
+        <v>60</v>
+      </c>
+      <c r="J69" t="s">
+        <v>62</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M69" t="s">
+        <v>64</v>
+      </c>
+      <c r="N69" t="s">
+        <v>152</v>
+      </c>
+      <c r="O69" t="s">
+        <v>188</v>
+      </c>
+      <c r="P69">
+        <v>50</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" t="s">
+        <v>106</v>
+      </c>
+      <c r="D70" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" t="s">
+        <v>122</v>
+      </c>
+      <c r="F70" t="s">
+        <v>62</v>
+      </c>
+      <c r="G70" t="s">
+        <v>127</v>
+      </c>
+      <c r="H70" t="s">
+        <v>63</v>
+      </c>
+      <c r="I70" t="s">
+        <v>60</v>
+      </c>
+      <c r="J70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M70" t="s">
+        <v>64</v>
+      </c>
+      <c r="N70" t="s">
+        <v>151</v>
+      </c>
+      <c r="O70" t="s">
+        <v>188</v>
+      </c>
+      <c r="P70">
+        <v>100</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" t="s">
+        <v>107</v>
+      </c>
+      <c r="D71" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" t="s">
+        <v>122</v>
+      </c>
+      <c r="F71" t="s">
+        <v>62</v>
+      </c>
+      <c r="G71" t="s">
+        <v>127</v>
+      </c>
+      <c r="H71" t="s">
+        <v>63</v>
+      </c>
+      <c r="I71" t="s">
+        <v>60</v>
+      </c>
+      <c r="J71" t="s">
+        <v>62</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M71" t="s">
+        <v>64</v>
+      </c>
+      <c r="N71" t="s">
+        <v>154</v>
+      </c>
+      <c r="O71" t="s">
+        <v>188</v>
+      </c>
+      <c r="P71">
+        <v>200</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" t="s">
+        <v>62</v>
+      </c>
+      <c r="C72" t="s">
+        <v>108</v>
+      </c>
+      <c r="D72" t="s">
+        <v>63</v>
+      </c>
+      <c r="E72" t="s">
+        <v>122</v>
+      </c>
+      <c r="F72" t="s">
+        <v>62</v>
+      </c>
+      <c r="G72" t="s">
+        <v>127</v>
+      </c>
+      <c r="H72" t="s">
+        <v>63</v>
+      </c>
+      <c r="I72" t="s">
+        <v>60</v>
+      </c>
+      <c r="J72" t="s">
+        <v>62</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M72" t="s">
+        <v>64</v>
+      </c>
+      <c r="N72" t="s">
+        <v>153</v>
+      </c>
+      <c r="O72" t="s">
+        <v>188</v>
+      </c>
+      <c r="P72">
+        <v>500</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B73" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" t="s">
+        <v>109</v>
+      </c>
+      <c r="D73" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" t="s">
+        <v>122</v>
+      </c>
+      <c r="F73" t="s">
+        <v>62</v>
+      </c>
+      <c r="G73" t="s">
+        <v>127</v>
+      </c>
+      <c r="H73" t="s">
+        <v>63</v>
+      </c>
+      <c r="I73" t="s">
+        <v>60</v>
+      </c>
+      <c r="J73" t="s">
+        <v>62</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M73" t="s">
+        <v>64</v>
+      </c>
+      <c r="N73" t="s">
+        <v>150</v>
+      </c>
+      <c r="O73" t="s">
+        <v>188</v>
+      </c>
+      <c r="P73">
+        <v>1000</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" t="s">
+        <v>112</v>
+      </c>
+      <c r="D74" t="s">
+        <v>63</v>
+      </c>
+      <c r="E74" t="s">
+        <v>122</v>
+      </c>
+      <c r="F74" t="s">
+        <v>62</v>
+      </c>
+      <c r="G74" t="s">
+        <v>127</v>
+      </c>
+      <c r="H74" t="s">
+        <v>63</v>
+      </c>
+      <c r="I74" t="s">
+        <v>60</v>
+      </c>
+      <c r="J74" t="s">
+        <v>62</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M74" t="s">
+        <v>64</v>
+      </c>
+      <c r="N74" t="s">
+        <v>156</v>
+      </c>
+      <c r="O74" t="s">
+        <v>188</v>
+      </c>
+      <c r="P74">
+        <v>2500</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" t="s">
+        <v>63</v>
+      </c>
+      <c r="E75" t="s">
+        <v>122</v>
+      </c>
+      <c r="F75" t="s">
+        <v>62</v>
+      </c>
+      <c r="G75" t="s">
+        <v>127</v>
+      </c>
+      <c r="H75" t="s">
+        <v>63</v>
+      </c>
+      <c r="I75" t="s">
+        <v>60</v>
+      </c>
+      <c r="J75" t="s">
+        <v>62</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M75" t="s">
+        <v>64</v>
+      </c>
+      <c r="N75" t="s">
+        <v>155</v>
+      </c>
+      <c r="O75" t="s">
+        <v>188</v>
+      </c>
+      <c r="P75">
+        <v>5000</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>61</v>
+      </c>
+      <c r="B76" t="s">
+        <v>62</v>
+      </c>
+      <c r="C76" t="s">
+        <v>110</v>
+      </c>
+      <c r="D76" t="s">
+        <v>63</v>
+      </c>
+      <c r="E76" t="s">
+        <v>122</v>
+      </c>
+      <c r="F76" t="s">
+        <v>62</v>
+      </c>
+      <c r="G76" t="s">
+        <v>127</v>
+      </c>
+      <c r="H76" t="s">
+        <v>63</v>
+      </c>
+      <c r="I76" t="s">
+        <v>60</v>
+      </c>
+      <c r="J76" t="s">
+        <v>62</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M76" t="s">
+        <v>64</v>
+      </c>
+      <c r="N76" t="s">
+        <v>145</v>
+      </c>
+      <c r="O76" t="s">
+        <v>188</v>
+      </c>
+      <c r="P76">
+        <v>10000</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B77" t="s">
+        <v>62</v>
+      </c>
+      <c r="C77" t="s">
+        <v>115</v>
+      </c>
+      <c r="D77" t="s">
+        <v>63</v>
+      </c>
+      <c r="E77" t="s">
+        <v>122</v>
+      </c>
+      <c r="F77" t="s">
+        <v>62</v>
+      </c>
+      <c r="G77" t="s">
+        <v>126</v>
+      </c>
+      <c r="H77" t="s">
+        <v>63</v>
+      </c>
+      <c r="I77" t="s">
+        <v>60</v>
+      </c>
+      <c r="J77" t="s">
+        <v>62</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M77" t="s">
+        <v>64</v>
+      </c>
+      <c r="N77" t="s">
+        <v>159</v>
+      </c>
+      <c r="O77" t="s">
+        <v>188</v>
+      </c>
+      <c r="P77">
+        <v>1000</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>61</v>
+      </c>
+      <c r="B78" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" t="s">
+        <v>116</v>
+      </c>
+      <c r="D78" t="s">
+        <v>63</v>
+      </c>
+      <c r="E78" t="s">
+        <v>122</v>
+      </c>
+      <c r="F78" t="s">
+        <v>62</v>
+      </c>
+      <c r="G78" t="s">
+        <v>126</v>
+      </c>
+      <c r="H78" t="s">
+        <v>63</v>
+      </c>
+      <c r="I78" t="s">
+        <v>60</v>
+      </c>
+      <c r="J78" t="s">
+        <v>62</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M78" t="s">
+        <v>64</v>
+      </c>
+      <c r="N78" t="s">
+        <v>159</v>
+      </c>
+      <c r="O78" t="s">
+        <v>188</v>
+      </c>
+      <c r="P78">
+        <v>1000</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79" t="s">
+        <v>117</v>
+      </c>
+      <c r="D79" t="s">
+        <v>63</v>
+      </c>
+      <c r="E79" t="s">
+        <v>122</v>
+      </c>
+      <c r="F79" t="s">
+        <v>62</v>
+      </c>
+      <c r="G79" t="s">
+        <v>126</v>
+      </c>
+      <c r="H79" t="s">
+        <v>63</v>
+      </c>
+      <c r="I79" t="s">
+        <v>60</v>
+      </c>
+      <c r="J79" t="s">
+        <v>62</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M79" t="s">
+        <v>64</v>
+      </c>
+      <c r="N79" t="s">
+        <v>159</v>
+      </c>
+      <c r="O79" t="s">
+        <v>188</v>
+      </c>
+      <c r="P79">
+        <v>1000</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>61</v>
+      </c>
+      <c r="B80" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80" t="s">
+        <v>113</v>
+      </c>
+      <c r="D80" t="s">
+        <v>63</v>
+      </c>
+      <c r="E80" t="s">
+        <v>122</v>
+      </c>
+      <c r="F80" t="s">
+        <v>62</v>
+      </c>
+      <c r="G80" t="s">
+        <v>126</v>
+      </c>
+      <c r="H80" t="s">
+        <v>63</v>
+      </c>
+      <c r="I80" t="s">
+        <v>60</v>
+      </c>
+      <c r="J80" t="s">
+        <v>62</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M80" t="s">
+        <v>64</v>
+      </c>
+      <c r="N80" t="s">
+        <v>144</v>
+      </c>
+      <c r="O80" t="s">
+        <v>188</v>
+      </c>
+      <c r="P80">
+        <v>2500</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>61</v>
+      </c>
+      <c r="B81" t="s">
+        <v>62</v>
+      </c>
+      <c r="C81" t="s">
+        <v>114</v>
+      </c>
+      <c r="D81" t="s">
+        <v>63</v>
+      </c>
+      <c r="E81" t="s">
+        <v>122</v>
+      </c>
+      <c r="F81" t="s">
+        <v>62</v>
+      </c>
+      <c r="G81" t="s">
+        <v>126</v>
+      </c>
+      <c r="H81" t="s">
+        <v>63</v>
+      </c>
+      <c r="I81" t="s">
+        <v>60</v>
+      </c>
+      <c r="J81" t="s">
+        <v>62</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M81" t="s">
+        <v>64</v>
+      </c>
+      <c r="N81" t="s">
+        <v>158</v>
+      </c>
+      <c r="O81" t="s">
+        <v>188</v>
+      </c>
+      <c r="P81">
+        <v>5000</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>61</v>
+      </c>
+      <c r="B82" t="s">
+        <v>62</v>
+      </c>
+      <c r="C82" t="s">
+        <v>118</v>
+      </c>
+      <c r="D82" t="s">
+        <v>63</v>
+      </c>
+      <c r="E82" t="s">
+        <v>122</v>
+      </c>
+      <c r="F82" t="s">
+        <v>62</v>
+      </c>
+      <c r="G82" t="s">
+        <v>125</v>
+      </c>
+      <c r="H82" t="s">
+        <v>63</v>
+      </c>
+      <c r="I82" t="s">
+        <v>60</v>
+      </c>
+      <c r="J82" t="s">
+        <v>62</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M82" t="s">
+        <v>64</v>
+      </c>
+      <c r="N82" t="s">
+        <v>131</v>
+      </c>
+      <c r="O82" t="s">
+        <v>188</v>
+      </c>
+      <c r="P82">
+        <v>50</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>61</v>
+      </c>
+      <c r="B83" t="s">
+        <v>62</v>
+      </c>
+      <c r="C83" t="s">
+        <v>119</v>
+      </c>
+      <c r="D83" t="s">
+        <v>63</v>
+      </c>
+      <c r="E83" t="s">
+        <v>122</v>
+      </c>
+      <c r="F83" t="s">
+        <v>62</v>
+      </c>
+      <c r="G83" t="s">
+        <v>125</v>
+      </c>
+      <c r="H83" t="s">
+        <v>63</v>
+      </c>
+      <c r="I83" t="s">
+        <v>60</v>
+      </c>
+      <c r="J83" t="s">
+        <v>62</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M83" t="s">
+        <v>64</v>
+      </c>
+      <c r="N83" t="s">
+        <v>130</v>
+      </c>
+      <c r="O83" t="s">
+        <v>188</v>
+      </c>
+      <c r="P83">
+        <v>200</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>61</v>
+      </c>
+      <c r="B84" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" t="s">
+        <v>224</v>
+      </c>
+      <c r="D84" t="s">
+        <v>63</v>
+      </c>
+      <c r="E84" t="s">
+        <v>122</v>
+      </c>
+      <c r="F84" t="s">
+        <v>62</v>
+      </c>
+      <c r="G84" t="s">
+        <v>125</v>
+      </c>
+      <c r="H84" t="s">
+        <v>63</v>
+      </c>
+      <c r="I84" t="s">
+        <v>60</v>
+      </c>
+      <c r="J84" t="s">
+        <v>62</v>
+      </c>
+      <c r="K84" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M84" t="s">
+        <v>64</v>
+      </c>
+      <c r="N84" t="s">
+        <v>230</v>
+      </c>
+      <c r="O84" t="s">
+        <v>188</v>
+      </c>
+      <c r="P84">
+        <v>500</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>61</v>
+      </c>
+      <c r="B85" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" t="s">
+        <v>227</v>
+      </c>
+      <c r="D85" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" t="s">
+        <v>122</v>
+      </c>
+      <c r="F85" t="s">
+        <v>62</v>
+      </c>
+      <c r="G85" t="s">
+        <v>125</v>
+      </c>
+      <c r="H85" t="s">
+        <v>63</v>
+      </c>
+      <c r="I85" t="s">
+        <v>60</v>
+      </c>
+      <c r="J85" t="s">
+        <v>62</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M85" t="s">
+        <v>64</v>
+      </c>
+      <c r="N85" t="s">
+        <v>233</v>
+      </c>
+      <c r="O85" t="s">
+        <v>188</v>
+      </c>
+      <c r="P85">
+        <v>1000</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>61</v>
+      </c>
+      <c r="B86" t="s">
+        <v>62</v>
+      </c>
+      <c r="C86" t="s">
+        <v>229</v>
+      </c>
+      <c r="D86" t="s">
+        <v>63</v>
+      </c>
+      <c r="E86" t="s">
+        <v>122</v>
+      </c>
+      <c r="F86" t="s">
+        <v>62</v>
+      </c>
+      <c r="G86" t="s">
+        <v>125</v>
+      </c>
+      <c r="H86" t="s">
+        <v>63</v>
+      </c>
+      <c r="I86" t="s">
+        <v>60</v>
+      </c>
+      <c r="J86" t="s">
+        <v>62</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M86" t="s">
+        <v>64</v>
+      </c>
+      <c r="N86" t="s">
+        <v>235</v>
+      </c>
+      <c r="O86" t="s">
+        <v>188</v>
+      </c>
+      <c r="P86">
+        <v>10000</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>61</v>
+      </c>
+      <c r="B87" t="s">
+        <v>62</v>
+      </c>
+      <c r="C87" t="s">
+        <v>228</v>
+      </c>
+      <c r="D87" t="s">
+        <v>63</v>
+      </c>
+      <c r="E87" t="s">
+        <v>122</v>
+      </c>
+      <c r="F87" t="s">
+        <v>62</v>
+      </c>
+      <c r="G87" t="s">
+        <v>125</v>
+      </c>
+      <c r="H87" t="s">
+        <v>63</v>
+      </c>
+      <c r="I87" t="s">
+        <v>60</v>
+      </c>
+      <c r="J87" t="s">
+        <v>62</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="L87" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M87" t="s">
+        <v>64</v>
+      </c>
+      <c r="N87" t="s">
+        <v>234</v>
+      </c>
+      <c r="O87" t="s">
+        <v>188</v>
+      </c>
+      <c r="P87">
+        <v>25000</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B88" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" t="s">
+        <v>120</v>
+      </c>
+      <c r="D88" t="s">
+        <v>63</v>
+      </c>
+      <c r="E88" t="s">
+        <v>122</v>
+      </c>
+      <c r="F88" t="s">
+        <v>62</v>
+      </c>
+      <c r="G88" t="s">
+        <v>125</v>
+      </c>
+      <c r="H88" t="s">
+        <v>63</v>
+      </c>
+      <c r="I88" t="s">
+        <v>60</v>
+      </c>
+      <c r="J88" t="s">
+        <v>62</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L88" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M88" t="s">
+        <v>64</v>
+      </c>
+      <c r="N88" t="s">
+        <v>166</v>
+      </c>
+      <c r="O88" t="s">
+        <v>188</v>
+      </c>
+      <c r="P88">
+        <v>50000</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>61</v>
+      </c>
+      <c r="B89" t="s">
+        <v>62</v>
+      </c>
+      <c r="C89" t="s">
+        <v>225</v>
+      </c>
+      <c r="D89" t="s">
+        <v>63</v>
+      </c>
+      <c r="E89" t="s">
+        <v>122</v>
+      </c>
+      <c r="F89" t="s">
+        <v>62</v>
+      </c>
+      <c r="G89" t="s">
+        <v>125</v>
+      </c>
+      <c r="H89" t="s">
+        <v>63</v>
+      </c>
+      <c r="I89" t="s">
+        <v>60</v>
+      </c>
+      <c r="J89" t="s">
+        <v>62</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="L89" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M89" t="s">
+        <v>64</v>
+      </c>
+      <c r="N89" t="s">
+        <v>231</v>
+      </c>
+      <c r="O89" t="s">
+        <v>188</v>
+      </c>
+      <c r="P89">
+        <v>75000</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>61</v>
+      </c>
+      <c r="B90" t="s">
+        <v>62</v>
+      </c>
+      <c r="C90" t="s">
+        <v>226</v>
+      </c>
+      <c r="D90" t="s">
+        <v>63</v>
+      </c>
+      <c r="E90" t="s">
+        <v>122</v>
+      </c>
+      <c r="F90" t="s">
+        <v>62</v>
+      </c>
+      <c r="G90" t="s">
+        <v>125</v>
+      </c>
+      <c r="H90" t="s">
+        <v>63</v>
+      </c>
+      <c r="I90" t="s">
+        <v>60</v>
+      </c>
+      <c r="J90" t="s">
+        <v>62</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M90" t="s">
+        <v>64</v>
+      </c>
+      <c r="N90" t="s">
+        <v>232</v>
+      </c>
+      <c r="O90" t="s">
+        <v>188</v>
+      </c>
+      <c r="P90">
+        <v>100000</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>61</v>
+      </c>
+      <c r="B91" t="s">
+        <v>62</v>
+      </c>
+      <c r="C91" t="s">
         <v>121</v>
       </c>
-      <c r="D66" t="s">
-        <v>63</v>
-      </c>
-      <c r="E66" t="s">
-        <v>122</v>
-      </c>
-      <c r="F66" t="s">
-        <v>62</v>
-      </c>
-      <c r="G66" t="s">
+      <c r="D91" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91" t="s">
+        <v>122</v>
+      </c>
+      <c r="F91" t="s">
+        <v>62</v>
+      </c>
+      <c r="G91" t="s">
         <v>125</v>
       </c>
-      <c r="H66" t="s">
-        <v>63</v>
-      </c>
-      <c r="I66" t="s">
-        <v>60</v>
-      </c>
-      <c r="J66" t="s">
-        <v>62</v>
-      </c>
-      <c r="K66" s="1" t="s">
+      <c r="H91" t="s">
+        <v>63</v>
+      </c>
+      <c r="I91" t="s">
+        <v>60</v>
+      </c>
+      <c r="J91" t="s">
+        <v>62</v>
+      </c>
+      <c r="K91" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L66" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M66" t="s">
-        <v>64</v>
-      </c>
-      <c r="N66" t="s">
+      <c r="L91" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M91" t="s">
+        <v>64</v>
+      </c>
+      <c r="N91" t="s">
         <v>162</v>
       </c>
-      <c r="O66" t="s">
-        <v>190</v>
-      </c>
-      <c r="P66">
+      <c r="O91" t="s">
+        <v>188</v>
+      </c>
+      <c r="P91">
         <v>500000</v>
       </c>
-      <c r="Q66" t="s">
-        <v>191</v>
-      </c>
+      <c r="Q91" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed special hat b14, moved crown to different category
</commit_message>
<xml_diff>
--- a/HutListe.xlsx
+++ b/HutListe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="303">
   <si>
     <t>states/schaf.png</t>
   </si>
@@ -1255,6 +1255,9 @@
   </si>
   <si>
     <t>pics/smileywars/chat_toggle_sticky-enabled.png</t>
+  </si>
+  <si>
+    <t>_HIDDEN_</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1669,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1676,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q91"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="P81" sqref="A2:Q92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1760,7 +1763,7 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -1772,7 +1775,7 @@
         <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>198</v>
+        <v>302</v>
       </c>
       <c r="H2" t="s">
         <v>63</v>
@@ -1783,8 +1786,8 @@
       <c r="J2" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>191</v>
+      <c r="K2" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>63</v>
@@ -1793,7 +1796,7 @@
         <v>64</v>
       </c>
       <c r="N2" t="s">
-        <v>132</v>
+        <v>258</v>
       </c>
       <c r="O2" t="s">
         <v>188</v>
@@ -1813,7 +1816,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -1837,7 +1840,7 @@
         <v>62</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>25</v>
+        <v>191</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>63</v>
@@ -1846,7 +1849,7 @@
         <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>245</v>
+        <v>132</v>
       </c>
       <c r="O3" t="s">
         <v>188</v>
@@ -1866,7 +1869,7 @@
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
@@ -1890,7 +1893,7 @@
         <v>62</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>63</v>
@@ -1899,7 +1902,7 @@
         <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O4" t="s">
         <v>188</v>
@@ -1919,7 +1922,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
@@ -1943,7 +1946,7 @@
         <v>62</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>63</v>
@@ -1952,7 +1955,7 @@
         <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>169</v>
+        <v>246</v>
       </c>
       <c r="O5" t="s">
         <v>188</v>
@@ -1972,7 +1975,7 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -1996,7 +1999,7 @@
         <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>63</v>
@@ -2005,7 +2008,7 @@
         <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O6" t="s">
         <v>188</v>
@@ -2025,7 +2028,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -2049,7 +2052,7 @@
         <v>62</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>63</v>
@@ -2058,7 +2061,7 @@
         <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O7" t="s">
         <v>188</v>
@@ -2078,7 +2081,7 @@
         <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -2102,7 +2105,7 @@
         <v>62</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>63</v>
@@ -2111,7 +2114,7 @@
         <v>64</v>
       </c>
       <c r="N8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O8" t="s">
         <v>188</v>
@@ -2131,7 +2134,7 @@
         <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -2154,8 +2157,8 @@
       <c r="J9" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>294</v>
+      <c r="K9" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>63</v>
@@ -2164,7 +2167,7 @@
         <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>262</v>
+        <v>172</v>
       </c>
       <c r="O9" t="s">
         <v>188</v>
@@ -2184,7 +2187,7 @@
         <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
+        <v>255</v>
       </c>
       <c r="D10" t="s">
         <v>63</v>
@@ -2196,7 +2199,7 @@
         <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>198</v>
       </c>
       <c r="H10" t="s">
         <v>63</v>
@@ -2207,8 +2210,8 @@
       <c r="J10" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>27</v>
+      <c r="K10" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>63</v>
@@ -2217,13 +2220,13 @@
         <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>139</v>
+        <v>262</v>
       </c>
       <c r="O10" t="s">
         <v>188</v>
       </c>
       <c r="P10">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="s">
         <v>189</v>
@@ -2237,7 +2240,7 @@
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>206</v>
       </c>
       <c r="D11" t="s">
         <v>63</v>
@@ -2261,7 +2264,7 @@
         <v>62</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>63</v>
@@ -2270,7 +2273,7 @@
         <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O11" t="s">
         <v>188</v>
@@ -2290,7 +2293,7 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
@@ -2314,7 +2317,7 @@
         <v>62</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>63</v>
@@ -2323,7 +2326,7 @@
         <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O12" t="s">
         <v>188</v>
@@ -2343,7 +2346,7 @@
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
@@ -2367,7 +2370,7 @@
         <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>63</v>
@@ -2376,7 +2379,7 @@
         <v>64</v>
       </c>
       <c r="N13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O13" t="s">
         <v>188</v>
@@ -2396,7 +2399,7 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
@@ -2420,7 +2423,7 @@
         <v>62</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>63</v>
@@ -2429,13 +2432,13 @@
         <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O14" t="s">
         <v>188</v>
       </c>
       <c r="P14">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q14" t="s">
         <v>189</v>
@@ -2449,7 +2452,7 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>63</v>
@@ -2473,7 +2476,7 @@
         <v>62</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>63</v>
@@ -2482,13 +2485,13 @@
         <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O15" t="s">
         <v>188</v>
       </c>
       <c r="P15">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q15" t="s">
         <v>189</v>
@@ -2502,7 +2505,7 @@
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
         <v>63</v>
@@ -2525,8 +2528,8 @@
       <c r="J16" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>293</v>
+      <c r="K16" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>63</v>
@@ -2535,13 +2538,13 @@
         <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>261</v>
+        <v>149</v>
       </c>
       <c r="O16" t="s">
         <v>188</v>
       </c>
       <c r="P16">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="Q16" t="s">
         <v>189</v>
@@ -2555,7 +2558,7 @@
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="D17" t="s">
         <v>63</v>
@@ -2579,7 +2582,7 @@
         <v>62</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>63</v>
@@ -2588,13 +2591,13 @@
         <v>64</v>
       </c>
       <c r="N17" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="O17" t="s">
         <v>188</v>
       </c>
       <c r="P17">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q17" t="s">
         <v>189</v>
@@ -2608,7 +2611,7 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>272</v>
       </c>
       <c r="D18" t="s">
         <v>63</v>
@@ -2631,8 +2634,8 @@
       <c r="J18" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>19</v>
+      <c r="K18" s="3" t="s">
+        <v>301</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>63</v>
@@ -2641,13 +2644,13 @@
         <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>157</v>
+        <v>275</v>
       </c>
       <c r="O18" t="s">
         <v>188</v>
       </c>
       <c r="P18">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q18" t="s">
         <v>189</v>
@@ -2661,7 +2664,7 @@
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>236</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -2684,8 +2687,8 @@
       <c r="J19" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>283</v>
+      <c r="K19" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>63</v>
@@ -2694,13 +2697,13 @@
         <v>64</v>
       </c>
       <c r="N19" t="s">
-        <v>238</v>
+        <v>157</v>
       </c>
       <c r="O19" t="s">
         <v>188</v>
       </c>
       <c r="P19">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="Q19" t="s">
         <v>189</v>
@@ -2714,7 +2717,7 @@
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>236</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
@@ -2737,8 +2740,8 @@
       <c r="J20" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>34</v>
+      <c r="K20" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>63</v>
@@ -2747,13 +2750,13 @@
         <v>64</v>
       </c>
       <c r="N20" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="O20" t="s">
         <v>188</v>
       </c>
       <c r="P20">
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="Q20" t="s">
         <v>189</v>
@@ -2767,7 +2770,7 @@
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>240</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
         <v>63</v>
@@ -2790,8 +2793,8 @@
       <c r="J21" t="s">
         <v>62</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>286</v>
+      <c r="K21" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>63</v>
@@ -2800,13 +2803,13 @@
         <v>64</v>
       </c>
       <c r="N21" t="s">
-        <v>249</v>
+        <v>160</v>
       </c>
       <c r="O21" t="s">
         <v>188</v>
       </c>
       <c r="P21">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="Q21" t="s">
         <v>189</v>
@@ -2820,7 +2823,7 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="D22" t="s">
         <v>63</v>
@@ -2832,7 +2835,7 @@
         <v>62</v>
       </c>
       <c r="G22" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H22" t="s">
         <v>63</v>
@@ -2843,8 +2846,8 @@
       <c r="J22" t="s">
         <v>62</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>1</v>
+      <c r="K22" s="4" t="s">
+        <v>286</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>63</v>
@@ -2853,13 +2856,13 @@
         <v>64</v>
       </c>
       <c r="N22" t="s">
-        <v>133</v>
+        <v>249</v>
       </c>
       <c r="O22" t="s">
         <v>188</v>
       </c>
       <c r="P22">
-        <v>50</v>
+        <v>25000</v>
       </c>
       <c r="Q22" t="s">
         <v>189</v>
@@ -2873,7 +2876,7 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>237</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
@@ -2896,8 +2899,8 @@
       <c r="J23" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>284</v>
+      <c r="K23" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>63</v>
@@ -2906,13 +2909,13 @@
         <v>64</v>
       </c>
       <c r="N23" t="s">
-        <v>247</v>
+        <v>133</v>
       </c>
       <c r="O23" t="s">
         <v>188</v>
       </c>
       <c r="P23">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="Q23" t="s">
         <v>189</v>
@@ -2926,7 +2929,7 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>237</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
@@ -2949,8 +2952,8 @@
       <c r="J24" t="s">
         <v>62</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>31</v>
+      <c r="K24" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>63</v>
@@ -2959,13 +2962,13 @@
         <v>64</v>
       </c>
       <c r="N24" t="s">
-        <v>143</v>
+        <v>247</v>
       </c>
       <c r="O24" t="s">
         <v>188</v>
       </c>
       <c r="P24">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q24" t="s">
         <v>189</v>
@@ -2979,7 +2982,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>243</v>
+        <v>73</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -3002,8 +3005,8 @@
       <c r="J25" t="s">
         <v>62</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>289</v>
+      <c r="K25" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>63</v>
@@ -3012,13 +3015,13 @@
         <v>64</v>
       </c>
       <c r="N25" t="s">
-        <v>257</v>
+        <v>143</v>
       </c>
       <c r="O25" t="s">
         <v>188</v>
       </c>
       <c r="P25">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q25" t="s">
         <v>189</v>
@@ -3032,7 +3035,7 @@
         <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>243</v>
       </c>
       <c r="D26" t="s">
         <v>63</v>
@@ -3055,8 +3058,8 @@
       <c r="J26" t="s">
         <v>62</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>24</v>
+      <c r="K26" s="4" t="s">
+        <v>289</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>63</v>
@@ -3065,13 +3068,13 @@
         <v>64</v>
       </c>
       <c r="N26" t="s">
-        <v>164</v>
+        <v>257</v>
       </c>
       <c r="O26" t="s">
         <v>188</v>
       </c>
       <c r="P26">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q26" t="s">
         <v>189</v>
@@ -3085,7 +3088,7 @@
         <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>266</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
         <v>63</v>
@@ -3108,8 +3111,8 @@
       <c r="J27" t="s">
         <v>62</v>
       </c>
-      <c r="K27" s="4" t="s">
-        <v>299</v>
+      <c r="K27" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>63</v>
@@ -3118,13 +3121,13 @@
         <v>64</v>
       </c>
       <c r="N27" t="s">
-        <v>273</v>
+        <v>164</v>
       </c>
       <c r="O27" t="s">
         <v>188</v>
       </c>
       <c r="P27">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="Q27" t="s">
         <v>189</v>
@@ -3138,7 +3141,7 @@
         <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>266</v>
       </c>
       <c r="D28" t="s">
         <v>63</v>
@@ -3161,8 +3164,8 @@
       <c r="J28" t="s">
         <v>62</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>26</v>
+      <c r="K28" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>63</v>
@@ -3171,13 +3174,13 @@
         <v>64</v>
       </c>
       <c r="N28" t="s">
-        <v>165</v>
+        <v>273</v>
       </c>
       <c r="O28" t="s">
         <v>188</v>
       </c>
       <c r="P28">
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="Q28" t="s">
         <v>189</v>
@@ -3191,7 +3194,7 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>253</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
         <v>63</v>
@@ -3214,8 +3217,8 @@
       <c r="J29" t="s">
         <v>62</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>292</v>
+      <c r="K29" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>63</v>
@@ -3224,13 +3227,13 @@
         <v>64</v>
       </c>
       <c r="N29" t="s">
-        <v>260</v>
+        <v>165</v>
       </c>
       <c r="O29" t="s">
         <v>188</v>
       </c>
       <c r="P29">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="Q29" t="s">
         <v>189</v>
@@ -3244,7 +3247,7 @@
         <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>253</v>
       </c>
       <c r="D30" t="s">
         <v>63</v>
@@ -3267,8 +3270,8 @@
       <c r="J30" t="s">
         <v>62</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>38</v>
+      <c r="K30" s="3" t="s">
+        <v>292</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>63</v>
@@ -3277,13 +3280,13 @@
         <v>64</v>
       </c>
       <c r="N30" t="s">
-        <v>168</v>
+        <v>260</v>
       </c>
       <c r="O30" t="s">
         <v>188</v>
       </c>
       <c r="P30">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="Q30" t="s">
         <v>189</v>
@@ -3297,7 +3300,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>265</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
         <v>63</v>
@@ -3320,8 +3323,8 @@
       <c r="J31" t="s">
         <v>62</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>298</v>
+      <c r="K31" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>63</v>
@@ -3330,13 +3333,13 @@
         <v>64</v>
       </c>
       <c r="N31" t="s">
-        <v>270</v>
+        <v>168</v>
       </c>
       <c r="O31" t="s">
         <v>188</v>
       </c>
       <c r="P31">
-        <v>75000</v>
+        <v>50000</v>
       </c>
       <c r="Q31" t="s">
         <v>189</v>
@@ -3509,7 +3512,7 @@
         <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>244</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
         <v>63</v>
@@ -3532,8 +3535,8 @@
       <c r="J35" t="s">
         <v>62</v>
       </c>
-      <c r="K35" s="3" t="s">
-        <v>290</v>
+      <c r="K35" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>63</v>
@@ -3542,13 +3545,13 @@
         <v>64</v>
       </c>
       <c r="N35" t="s">
-        <v>258</v>
+        <v>161</v>
       </c>
       <c r="O35" t="s">
         <v>188</v>
       </c>
       <c r="P35">
-        <v>750000</v>
+        <v>1000000</v>
       </c>
       <c r="Q35" t="s">
         <v>189</v>
@@ -3562,7 +3565,7 @@
         <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>
@@ -3586,7 +3589,7 @@
         <v>62</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>63</v>
@@ -3595,13 +3598,13 @@
         <v>64</v>
       </c>
       <c r="N36" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="O36" t="s">
         <v>188</v>
       </c>
       <c r="P36">
-        <v>1000000</v>
+        <v>2500000</v>
       </c>
       <c r="Q36" t="s">
         <v>189</v>
@@ -3615,7 +3618,7 @@
         <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>81</v>
+        <v>264</v>
       </c>
       <c r="D37" t="s">
         <v>63</v>
@@ -3627,7 +3630,7 @@
         <v>62</v>
       </c>
       <c r="G37" t="s">
-        <v>129</v>
+        <v>276</v>
       </c>
       <c r="H37" t="s">
         <v>63</v>
@@ -3638,8 +3641,8 @@
       <c r="J37" t="s">
         <v>62</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>23</v>
+      <c r="K37" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>63</v>
@@ -3648,13 +3651,13 @@
         <v>64</v>
       </c>
       <c r="N37" t="s">
-        <v>163</v>
+        <v>269</v>
       </c>
       <c r="O37" t="s">
         <v>188</v>
       </c>
       <c r="P37">
-        <v>2500000</v>
+        <v>500</v>
       </c>
       <c r="Q37" t="s">
         <v>189</v>
@@ -3668,7 +3671,7 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="D38" t="s">
         <v>63</v>
@@ -3692,7 +3695,7 @@
         <v>62</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>63</v>
@@ -3701,13 +3704,13 @@
         <v>64</v>
       </c>
       <c r="N38" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="O38" t="s">
         <v>188</v>
       </c>
       <c r="P38">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="Q38" t="s">
         <v>189</v>
@@ -3721,7 +3724,7 @@
         <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D39" t="s">
         <v>63</v>
@@ -3745,7 +3748,7 @@
         <v>62</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>63</v>
@@ -3754,13 +3757,13 @@
         <v>64</v>
       </c>
       <c r="N39" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="O39" t="s">
         <v>188</v>
       </c>
       <c r="P39">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="Q39" t="s">
         <v>189</v>
@@ -3774,7 +3777,7 @@
         <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="D40" t="s">
         <v>63</v>
@@ -3798,7 +3801,7 @@
         <v>62</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>63</v>
@@ -3807,13 +3810,13 @@
         <v>64</v>
       </c>
       <c r="N40" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="O40" t="s">
         <v>188</v>
       </c>
       <c r="P40">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="Q40" t="s">
         <v>189</v>
@@ -3827,7 +3830,7 @@
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="D41" t="s">
         <v>63</v>
@@ -3850,8 +3853,8 @@
       <c r="J41" t="s">
         <v>62</v>
       </c>
-      <c r="K41" s="4" t="s">
-        <v>296</v>
+      <c r="K41" s="3" t="s">
+        <v>300</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>63</v>
@@ -3860,13 +3863,13 @@
         <v>64</v>
       </c>
       <c r="N41" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="O41" t="s">
         <v>188</v>
       </c>
       <c r="P41">
-        <v>5000</v>
+        <v>7500</v>
       </c>
       <c r="Q41" t="s">
         <v>189</v>
@@ -3880,7 +3883,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>271</v>
+        <v>242</v>
       </c>
       <c r="D42" t="s">
         <v>63</v>
@@ -3903,8 +3906,8 @@
       <c r="J42" t="s">
         <v>62</v>
       </c>
-      <c r="K42" s="3" t="s">
-        <v>300</v>
+      <c r="K42" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>63</v>
@@ -3913,13 +3916,13 @@
         <v>64</v>
       </c>
       <c r="N42" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="O42" t="s">
         <v>188</v>
       </c>
       <c r="P42">
-        <v>7500</v>
+        <v>10000</v>
       </c>
       <c r="Q42" t="s">
         <v>189</v>
@@ -3933,7 +3936,7 @@
         <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="D43" t="s">
         <v>63</v>
@@ -3956,8 +3959,8 @@
       <c r="J43" t="s">
         <v>62</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>288</v>
+      <c r="K43" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>63</v>
@@ -3966,13 +3969,13 @@
         <v>64</v>
       </c>
       <c r="N43" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="O43" t="s">
         <v>188</v>
       </c>
       <c r="P43">
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="Q43" t="s">
         <v>189</v>
@@ -3986,7 +3989,7 @@
         <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D44" t="s">
         <v>63</v>
@@ -4010,7 +4013,7 @@
         <v>62</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>63</v>
@@ -4019,13 +4022,13 @@
         <v>64</v>
       </c>
       <c r="N44" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="O44" t="s">
         <v>188</v>
       </c>
       <c r="P44">
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="Q44" t="s">
         <v>189</v>
@@ -4039,7 +4042,7 @@
         <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>256</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -4051,7 +4054,7 @@
         <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>276</v>
+        <v>123</v>
       </c>
       <c r="H45" t="s">
         <v>63</v>
@@ -4062,8 +4065,8 @@
       <c r="J45" t="s">
         <v>62</v>
       </c>
-      <c r="K45" s="3" t="s">
-        <v>295</v>
+      <c r="K45" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>63</v>
@@ -4072,13 +4075,13 @@
         <v>64</v>
       </c>
       <c r="N45" t="s">
-        <v>267</v>
+        <v>134</v>
       </c>
       <c r="O45" t="s">
         <v>188</v>
       </c>
       <c r="P45">
-        <v>50000</v>
+        <v>1</v>
       </c>
       <c r="Q45" t="s">
         <v>189</v>
@@ -4092,7 +4095,7 @@
         <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D46" t="s">
         <v>63</v>
@@ -4116,7 +4119,7 @@
         <v>62</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>63</v>
@@ -4125,13 +4128,13 @@
         <v>64</v>
       </c>
       <c r="N46" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="O46" t="s">
         <v>188</v>
       </c>
       <c r="P46">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q46" t="s">
         <v>189</v>
@@ -4145,7 +4148,7 @@
         <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D47" t="s">
         <v>63</v>
@@ -4169,7 +4172,7 @@
         <v>62</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>63</v>
@@ -4178,13 +4181,13 @@
         <v>64</v>
       </c>
       <c r="N47" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O47" t="s">
         <v>188</v>
       </c>
       <c r="P47">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q47" t="s">
         <v>189</v>
@@ -4198,7 +4201,7 @@
         <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D48" t="s">
         <v>63</v>
@@ -4222,7 +4225,7 @@
         <v>62</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>63</v>
@@ -4231,13 +4234,13 @@
         <v>64</v>
       </c>
       <c r="N48" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O48" t="s">
         <v>188</v>
       </c>
       <c r="P48">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q48" t="s">
         <v>189</v>
@@ -4251,7 +4254,7 @@
         <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D49" t="s">
         <v>63</v>
@@ -4275,7 +4278,7 @@
         <v>62</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>63</v>
@@ -4284,13 +4287,13 @@
         <v>64</v>
       </c>
       <c r="N49" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O49" t="s">
         <v>188</v>
       </c>
       <c r="P49">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="Q49" t="s">
         <v>189</v>
@@ -4304,7 +4307,7 @@
         <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
         <v>63</v>
@@ -4328,7 +4331,7 @@
         <v>62</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>5</v>
+        <v>207</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>63</v>
@@ -4337,13 +4340,13 @@
         <v>64</v>
       </c>
       <c r="N50" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="O50" t="s">
         <v>188</v>
       </c>
       <c r="P50">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="Q50" t="s">
         <v>189</v>
@@ -4357,7 +4360,7 @@
         <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D51" t="s">
         <v>63</v>
@@ -4381,7 +4384,7 @@
         <v>62</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>63</v>
@@ -4390,13 +4393,13 @@
         <v>64</v>
       </c>
       <c r="N51" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O51" t="s">
         <v>188</v>
       </c>
       <c r="P51">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="Q51" t="s">
         <v>189</v>
@@ -4410,7 +4413,7 @@
         <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D52" t="s">
         <v>63</v>
@@ -4434,7 +4437,7 @@
         <v>62</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>63</v>
@@ -4443,13 +4446,13 @@
         <v>64</v>
       </c>
       <c r="N52" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="O52" t="s">
         <v>188</v>
       </c>
       <c r="P52">
-        <v>500</v>
+        <v>1000000</v>
       </c>
       <c r="Q52" t="s">
         <v>189</v>
@@ -4463,7 +4466,7 @@
         <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D53" t="s">
         <v>63</v>
@@ -4475,7 +4478,7 @@
         <v>62</v>
       </c>
       <c r="G53" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="H53" t="s">
         <v>63</v>
@@ -4487,7 +4490,7 @@
         <v>62</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>211</v>
+        <v>45</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>63</v>
@@ -4496,13 +4499,13 @@
         <v>64</v>
       </c>
       <c r="N53" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="O53" t="s">
         <v>188</v>
       </c>
       <c r="P53">
-        <v>1000000</v>
+        <v>10</v>
       </c>
       <c r="Q53" t="s">
         <v>189</v>
@@ -4516,7 +4519,7 @@
         <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D54" t="s">
         <v>63</v>
@@ -4540,7 +4543,7 @@
         <v>62</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>63</v>
@@ -4549,13 +4552,13 @@
         <v>64</v>
       </c>
       <c r="N54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O54" t="s">
         <v>188</v>
       </c>
       <c r="P54">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="Q54" t="s">
         <v>189</v>
@@ -4569,7 +4572,7 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D55" t="s">
         <v>63</v>
@@ -4593,7 +4596,7 @@
         <v>62</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>63</v>
@@ -4602,7 +4605,7 @@
         <v>64</v>
       </c>
       <c r="N55" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="O55" t="s">
         <v>188</v>
@@ -4622,7 +4625,7 @@
         <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D56" t="s">
         <v>63</v>
@@ -4646,7 +4649,7 @@
         <v>62</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>63</v>
@@ -4655,13 +4658,13 @@
         <v>64</v>
       </c>
       <c r="N56" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="O56" t="s">
         <v>188</v>
       </c>
       <c r="P56">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="Q56" t="s">
         <v>189</v>
@@ -4675,7 +4678,7 @@
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D57" t="s">
         <v>63</v>
@@ -4699,7 +4702,7 @@
         <v>62</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>63</v>
@@ -4708,7 +4711,7 @@
         <v>64</v>
       </c>
       <c r="N57" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="O57" t="s">
         <v>188</v>
@@ -4728,7 +4731,7 @@
         <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D58" t="s">
         <v>63</v>
@@ -4752,7 +4755,7 @@
         <v>62</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>63</v>
@@ -4761,13 +4764,13 @@
         <v>64</v>
       </c>
       <c r="N58" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="O58" t="s">
         <v>188</v>
       </c>
       <c r="P58">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="Q58" t="s">
         <v>189</v>
@@ -4781,7 +4784,7 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
         <v>63</v>
@@ -4805,7 +4808,7 @@
         <v>62</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>63</v>
@@ -4814,7 +4817,7 @@
         <v>64</v>
       </c>
       <c r="N59" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="O59" t="s">
         <v>188</v>
@@ -4834,7 +4837,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D60" t="s">
         <v>63</v>
@@ -4858,7 +4861,7 @@
         <v>62</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>63</v>
@@ -4867,13 +4870,13 @@
         <v>64</v>
       </c>
       <c r="N60" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="O60" t="s">
         <v>188</v>
       </c>
       <c r="P60">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="Q60" t="s">
         <v>189</v>
@@ -4887,7 +4890,7 @@
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -4911,7 +4914,7 @@
         <v>62</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>63</v>
@@ -4920,7 +4923,7 @@
         <v>64</v>
       </c>
       <c r="N61" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="O61" t="s">
         <v>188</v>
@@ -4940,7 +4943,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D62" t="s">
         <v>63</v>
@@ -4964,7 +4967,7 @@
         <v>62</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>63</v>
@@ -4973,13 +4976,13 @@
         <v>64</v>
       </c>
       <c r="N62" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="O62" t="s">
         <v>188</v>
       </c>
       <c r="P62">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="Q62" t="s">
         <v>189</v>
@@ -4993,7 +4996,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D63" t="s">
         <v>63</v>
@@ -5017,7 +5020,7 @@
         <v>62</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>63</v>
@@ -5026,7 +5029,7 @@
         <v>64</v>
       </c>
       <c r="N63" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O63" t="s">
         <v>188</v>
@@ -5046,7 +5049,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D64" t="s">
         <v>63</v>
@@ -5070,7 +5073,7 @@
         <v>62</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>63</v>
@@ -5079,13 +5082,13 @@
         <v>64</v>
       </c>
       <c r="N64" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="O64" t="s">
         <v>188</v>
       </c>
       <c r="P64">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="Q64" t="s">
         <v>189</v>
@@ -5099,7 +5102,7 @@
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D65" t="s">
         <v>63</v>
@@ -5123,7 +5126,7 @@
         <v>62</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>63</v>
@@ -5132,13 +5135,13 @@
         <v>64</v>
       </c>
       <c r="N65" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="O65" t="s">
         <v>188</v>
       </c>
       <c r="P65">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="Q65" t="s">
         <v>189</v>
@@ -5152,7 +5155,7 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D66" t="s">
         <v>63</v>
@@ -5176,7 +5179,7 @@
         <v>62</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>63</v>
@@ -5185,13 +5188,13 @@
         <v>64</v>
       </c>
       <c r="N66" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="O66" t="s">
         <v>188</v>
       </c>
       <c r="P66">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="Q66" t="s">
         <v>189</v>
@@ -5205,7 +5208,7 @@
         <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D67" t="s">
         <v>63</v>
@@ -5229,7 +5232,7 @@
         <v>62</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>63</v>
@@ -5238,13 +5241,13 @@
         <v>64</v>
       </c>
       <c r="N67" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="O67" t="s">
         <v>188</v>
       </c>
       <c r="P67">
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="Q67" t="s">
         <v>189</v>
@@ -5258,7 +5261,7 @@
         <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D68" t="s">
         <v>63</v>
@@ -5270,7 +5273,7 @@
         <v>62</v>
       </c>
       <c r="G68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H68" t="s">
         <v>63</v>
@@ -5282,7 +5285,7 @@
         <v>62</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>63</v>
@@ -5291,13 +5294,13 @@
         <v>64</v>
       </c>
       <c r="N68" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="O68" t="s">
         <v>188</v>
       </c>
       <c r="P68">
-        <v>100000</v>
+        <v>50</v>
       </c>
       <c r="Q68" t="s">
         <v>189</v>
@@ -5311,7 +5314,7 @@
         <v>62</v>
       </c>
       <c r="C69" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D69" t="s">
         <v>63</v>
@@ -5335,7 +5338,7 @@
         <v>62</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>63</v>
@@ -5344,13 +5347,13 @@
         <v>64</v>
       </c>
       <c r="N69" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O69" t="s">
         <v>188</v>
       </c>
       <c r="P69">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="Q69" t="s">
         <v>189</v>
@@ -5364,7 +5367,7 @@
         <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D70" t="s">
         <v>63</v>
@@ -5388,7 +5391,7 @@
         <v>62</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>63</v>
@@ -5397,13 +5400,13 @@
         <v>64</v>
       </c>
       <c r="N70" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="O70" t="s">
         <v>188</v>
       </c>
       <c r="P70">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="Q70" t="s">
         <v>189</v>
@@ -5417,7 +5420,7 @@
         <v>62</v>
       </c>
       <c r="C71" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D71" t="s">
         <v>63</v>
@@ -5441,7 +5444,7 @@
         <v>62</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>63</v>
@@ -5450,13 +5453,13 @@
         <v>64</v>
       </c>
       <c r="N71" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O71" t="s">
         <v>188</v>
       </c>
       <c r="P71">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="Q71" t="s">
         <v>189</v>
@@ -5470,7 +5473,7 @@
         <v>62</v>
       </c>
       <c r="C72" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D72" t="s">
         <v>63</v>
@@ -5494,7 +5497,7 @@
         <v>62</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>63</v>
@@ -5503,13 +5506,13 @@
         <v>64</v>
       </c>
       <c r="N72" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O72" t="s">
         <v>188</v>
       </c>
       <c r="P72">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="Q72" t="s">
         <v>189</v>
@@ -5523,7 +5526,7 @@
         <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D73" t="s">
         <v>63</v>
@@ -5547,7 +5550,7 @@
         <v>62</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>63</v>
@@ -5556,13 +5559,13 @@
         <v>64</v>
       </c>
       <c r="N73" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="O73" t="s">
         <v>188</v>
       </c>
       <c r="P73">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="Q73" t="s">
         <v>189</v>
@@ -5576,7 +5579,7 @@
         <v>62</v>
       </c>
       <c r="C74" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D74" t="s">
         <v>63</v>
@@ -5600,7 +5603,7 @@
         <v>62</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>63</v>
@@ -5609,13 +5612,13 @@
         <v>64</v>
       </c>
       <c r="N74" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O74" t="s">
         <v>188</v>
       </c>
       <c r="P74">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="Q74" t="s">
         <v>189</v>
@@ -5629,7 +5632,7 @@
         <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D75" t="s">
         <v>63</v>
@@ -5653,7 +5656,7 @@
         <v>62</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>63</v>
@@ -5662,13 +5665,13 @@
         <v>64</v>
       </c>
       <c r="N75" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="O75" t="s">
         <v>188</v>
       </c>
       <c r="P75">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="Q75" t="s">
         <v>189</v>
@@ -5682,7 +5685,7 @@
         <v>62</v>
       </c>
       <c r="C76" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D76" t="s">
         <v>63</v>
@@ -5694,7 +5697,7 @@
         <v>62</v>
       </c>
       <c r="G76" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H76" t="s">
         <v>63</v>
@@ -5706,7 +5709,7 @@
         <v>62</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>63</v>
@@ -5715,13 +5718,13 @@
         <v>64</v>
       </c>
       <c r="N76" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="O76" t="s">
         <v>188</v>
       </c>
       <c r="P76">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="Q76" t="s">
         <v>189</v>
@@ -5735,7 +5738,7 @@
         <v>62</v>
       </c>
       <c r="C77" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D77" t="s">
         <v>63</v>
@@ -5759,7 +5762,7 @@
         <v>62</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>63</v>
@@ -5788,7 +5791,7 @@
         <v>62</v>
       </c>
       <c r="C78" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D78" t="s">
         <v>63</v>
@@ -5812,7 +5815,7 @@
         <v>62</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>63</v>
@@ -5841,7 +5844,7 @@
         <v>62</v>
       </c>
       <c r="C79" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D79" t="s">
         <v>63</v>
@@ -5865,7 +5868,7 @@
         <v>62</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>63</v>
@@ -5874,13 +5877,13 @@
         <v>64</v>
       </c>
       <c r="N79" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="O79" t="s">
         <v>188</v>
       </c>
       <c r="P79">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="Q79" t="s">
         <v>189</v>
@@ -5894,7 +5897,7 @@
         <v>62</v>
       </c>
       <c r="C80" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D80" t="s">
         <v>63</v>
@@ -5918,7 +5921,7 @@
         <v>62</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>63</v>
@@ -5927,13 +5930,13 @@
         <v>64</v>
       </c>
       <c r="N80" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="O80" t="s">
         <v>188</v>
       </c>
       <c r="P80">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="Q80" t="s">
         <v>189</v>
@@ -5947,7 +5950,7 @@
         <v>62</v>
       </c>
       <c r="C81" t="s">
-        <v>114</v>
+        <v>265</v>
       </c>
       <c r="D81" t="s">
         <v>63</v>
@@ -5970,8 +5973,8 @@
       <c r="J81" t="s">
         <v>62</v>
       </c>
-      <c r="K81" s="1" t="s">
-        <v>20</v>
+      <c r="K81" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="L81" s="1" t="s">
         <v>63</v>
@@ -5980,13 +5983,13 @@
         <v>64</v>
       </c>
       <c r="N81" t="s">
-        <v>158</v>
+        <v>270</v>
       </c>
       <c r="O81" t="s">
         <v>188</v>
       </c>
       <c r="P81">
-        <v>5000</v>
+        <v>75000</v>
       </c>
       <c r="Q81" t="s">
         <v>189</v>

</xml_diff>

<commit_message>
added reward for may
</commit_message>
<xml_diff>
--- a/HutListe.xlsx
+++ b/HutListe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="306">
   <si>
     <t>states/schaf.png</t>
   </si>
@@ -1086,9 +1086,6 @@
     <t>b14</t>
   </si>
   <si>
-    <t>Erreicht wenn du 1.000 Punkte in der Saison März geschafft hast.</t>
-  </si>
-  <si>
     <t>Belohnung für die Besten am Ende einer Saison!</t>
   </si>
   <si>
@@ -1258,6 +1255,18 @@
   </si>
   <si>
     <t>_HIDDEN_</t>
+  </si>
+  <si>
+    <t>&amp;04</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison Mai.</t>
+  </si>
+  <si>
+    <t>pics/sm_macguffin2012-item_12.png</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison März.</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1678,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1679,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="P81" sqref="A2:Q92"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1775,7 +1784,7 @@
         <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H2" t="s">
         <v>63</v>
@@ -1787,7 +1796,7 @@
         <v>62</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>63</v>
@@ -1796,7 +1805,7 @@
         <v>64</v>
       </c>
       <c r="N2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O2" t="s">
         <v>188</v>
@@ -1869,7 +1878,7 @@
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
@@ -1893,7 +1902,7 @@
         <v>62</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>63</v>
@@ -1922,7 +1931,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
@@ -1946,7 +1955,7 @@
         <v>62</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>63</v>
@@ -1955,7 +1964,7 @@
         <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>246</v>
+        <v>169</v>
       </c>
       <c r="O5" t="s">
         <v>188</v>
@@ -1975,7 +1984,7 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -1999,7 +2008,7 @@
         <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>63</v>
@@ -2008,7 +2017,7 @@
         <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O6" t="s">
         <v>188</v>
@@ -2028,7 +2037,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -2052,7 +2061,7 @@
         <v>62</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>63</v>
@@ -2061,7 +2070,7 @@
         <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="O7" t="s">
         <v>188</v>
@@ -2081,7 +2090,7 @@
         <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -2105,7 +2114,7 @@
         <v>62</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>63</v>
@@ -2114,7 +2123,7 @@
         <v>64</v>
       </c>
       <c r="N8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O8" t="s">
         <v>188</v>
@@ -2134,7 +2143,7 @@
         <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -2158,7 +2167,7 @@
         <v>62</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>63</v>
@@ -2167,7 +2176,7 @@
         <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>172</v>
+        <v>305</v>
       </c>
       <c r="O9" t="s">
         <v>188</v>
@@ -2187,7 +2196,7 @@
         <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D10" t="s">
         <v>63</v>
@@ -2211,7 +2220,7 @@
         <v>62</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>63</v>
@@ -2220,7 +2229,7 @@
         <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O10" t="s">
         <v>188</v>
@@ -2240,7 +2249,7 @@
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>206</v>
+        <v>302</v>
       </c>
       <c r="D11" t="s">
         <v>63</v>
@@ -2252,7 +2261,7 @@
         <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>124</v>
+        <v>198</v>
       </c>
       <c r="H11" t="s">
         <v>63</v>
@@ -2264,7 +2273,7 @@
         <v>62</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>27</v>
+        <v>304</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>63</v>
@@ -2273,13 +2282,13 @@
         <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>139</v>
+        <v>303</v>
       </c>
       <c r="O11" t="s">
         <v>188</v>
       </c>
       <c r="P11">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="s">
         <v>189</v>
@@ -2293,7 +2302,7 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>206</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
@@ -2317,7 +2326,7 @@
         <v>62</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>63</v>
@@ -2326,7 +2335,7 @@
         <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O12" t="s">
         <v>188</v>
@@ -2346,7 +2355,7 @@
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
@@ -2370,7 +2379,7 @@
         <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>63</v>
@@ -2379,7 +2388,7 @@
         <v>64</v>
       </c>
       <c r="N13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O13" t="s">
         <v>188</v>
@@ -2399,7 +2408,7 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
@@ -2423,7 +2432,7 @@
         <v>62</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>63</v>
@@ -2432,7 +2441,7 @@
         <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O14" t="s">
         <v>188</v>
@@ -2452,7 +2461,7 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
         <v>63</v>
@@ -2476,7 +2485,7 @@
         <v>62</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>63</v>
@@ -2485,13 +2494,13 @@
         <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O15" t="s">
         <v>188</v>
       </c>
       <c r="P15">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q15" t="s">
         <v>189</v>
@@ -2505,7 +2514,7 @@
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
         <v>63</v>
@@ -2529,7 +2538,7 @@
         <v>62</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>63</v>
@@ -2538,13 +2547,13 @@
         <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O16" t="s">
         <v>188</v>
       </c>
       <c r="P16">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q16" t="s">
         <v>189</v>
@@ -2558,7 +2567,7 @@
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
         <v>63</v>
@@ -2581,8 +2590,8 @@
       <c r="J17" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>293</v>
+      <c r="K17" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>63</v>
@@ -2591,13 +2600,13 @@
         <v>64</v>
       </c>
       <c r="N17" t="s">
-        <v>261</v>
+        <v>149</v>
       </c>
       <c r="O17" t="s">
         <v>188</v>
       </c>
       <c r="P17">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="Q17" t="s">
         <v>189</v>
@@ -2611,7 +2620,7 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="D18" t="s">
         <v>63</v>
@@ -2635,7 +2644,7 @@
         <v>62</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>63</v>
@@ -2644,13 +2653,13 @@
         <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="O18" t="s">
         <v>188</v>
       </c>
       <c r="P18">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q18" t="s">
         <v>189</v>
@@ -2664,7 +2673,7 @@
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>271</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -2687,8 +2696,8 @@
       <c r="J19" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>19</v>
+      <c r="K19" s="3" t="s">
+        <v>300</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>63</v>
@@ -2697,13 +2706,13 @@
         <v>64</v>
       </c>
       <c r="N19" t="s">
-        <v>157</v>
+        <v>274</v>
       </c>
       <c r="O19" t="s">
         <v>188</v>
       </c>
       <c r="P19">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q19" t="s">
         <v>189</v>
@@ -2717,7 +2726,7 @@
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>236</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
@@ -2740,8 +2749,8 @@
       <c r="J20" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>283</v>
+      <c r="K20" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>63</v>
@@ -2750,13 +2759,13 @@
         <v>64</v>
       </c>
       <c r="N20" t="s">
-        <v>238</v>
+        <v>157</v>
       </c>
       <c r="O20" t="s">
         <v>188</v>
       </c>
       <c r="P20">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="Q20" t="s">
         <v>189</v>
@@ -2770,7 +2779,7 @@
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>236</v>
       </c>
       <c r="D21" t="s">
         <v>63</v>
@@ -2793,8 +2802,8 @@
       <c r="J21" t="s">
         <v>62</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>34</v>
+      <c r="K21" s="3" t="s">
+        <v>282</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>63</v>
@@ -2803,13 +2812,13 @@
         <v>64</v>
       </c>
       <c r="N21" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="O21" t="s">
         <v>188</v>
       </c>
       <c r="P21">
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="Q21" t="s">
         <v>189</v>
@@ -2823,7 +2832,7 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>240</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
         <v>63</v>
@@ -2846,8 +2855,8 @@
       <c r="J22" t="s">
         <v>62</v>
       </c>
-      <c r="K22" s="4" t="s">
-        <v>286</v>
+      <c r="K22" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>63</v>
@@ -2856,13 +2865,13 @@
         <v>64</v>
       </c>
       <c r="N22" t="s">
-        <v>249</v>
+        <v>160</v>
       </c>
       <c r="O22" t="s">
         <v>188</v>
       </c>
       <c r="P22">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="Q22" t="s">
         <v>189</v>
@@ -2876,7 +2885,7 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
@@ -2888,7 +2897,7 @@
         <v>62</v>
       </c>
       <c r="G23" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H23" t="s">
         <v>63</v>
@@ -2899,8 +2908,8 @@
       <c r="J23" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>1</v>
+      <c r="K23" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>63</v>
@@ -2909,13 +2918,13 @@
         <v>64</v>
       </c>
       <c r="N23" t="s">
-        <v>133</v>
+        <v>248</v>
       </c>
       <c r="O23" t="s">
         <v>188</v>
       </c>
       <c r="P23">
-        <v>50</v>
+        <v>25000</v>
       </c>
       <c r="Q23" t="s">
         <v>189</v>
@@ -2929,7 +2938,7 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>237</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
@@ -2952,8 +2961,8 @@
       <c r="J24" t="s">
         <v>62</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>284</v>
+      <c r="K24" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>63</v>
@@ -2962,13 +2971,13 @@
         <v>64</v>
       </c>
       <c r="N24" t="s">
-        <v>247</v>
+        <v>133</v>
       </c>
       <c r="O24" t="s">
         <v>188</v>
       </c>
       <c r="P24">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="Q24" t="s">
         <v>189</v>
@@ -2982,7 +2991,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>237</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -3005,8 +3014,8 @@
       <c r="J25" t="s">
         <v>62</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>31</v>
+      <c r="K25" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>63</v>
@@ -3015,13 +3024,13 @@
         <v>64</v>
       </c>
       <c r="N25" t="s">
-        <v>143</v>
+        <v>246</v>
       </c>
       <c r="O25" t="s">
         <v>188</v>
       </c>
       <c r="P25">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q25" t="s">
         <v>189</v>
@@ -3035,7 +3044,7 @@
         <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>243</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
         <v>63</v>
@@ -3058,8 +3067,8 @@
       <c r="J26" t="s">
         <v>62</v>
       </c>
-      <c r="K26" s="4" t="s">
-        <v>289</v>
+      <c r="K26" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>63</v>
@@ -3068,13 +3077,13 @@
         <v>64</v>
       </c>
       <c r="N26" t="s">
-        <v>257</v>
+        <v>143</v>
       </c>
       <c r="O26" t="s">
         <v>188</v>
       </c>
       <c r="P26">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q26" t="s">
         <v>189</v>
@@ -3088,7 +3097,7 @@
         <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>243</v>
       </c>
       <c r="D27" t="s">
         <v>63</v>
@@ -3111,8 +3120,8 @@
       <c r="J27" t="s">
         <v>62</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>24</v>
+      <c r="K27" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>63</v>
@@ -3121,13 +3130,13 @@
         <v>64</v>
       </c>
       <c r="N27" t="s">
-        <v>164</v>
+        <v>256</v>
       </c>
       <c r="O27" t="s">
         <v>188</v>
       </c>
       <c r="P27">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q27" t="s">
         <v>189</v>
@@ -3141,7 +3150,7 @@
         <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>266</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
         <v>63</v>
@@ -3164,8 +3173,8 @@
       <c r="J28" t="s">
         <v>62</v>
       </c>
-      <c r="K28" s="4" t="s">
-        <v>299</v>
+      <c r="K28" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>63</v>
@@ -3174,13 +3183,13 @@
         <v>64</v>
       </c>
       <c r="N28" t="s">
-        <v>273</v>
+        <v>164</v>
       </c>
       <c r="O28" t="s">
         <v>188</v>
       </c>
       <c r="P28">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="Q28" t="s">
         <v>189</v>
@@ -3194,7 +3203,7 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>265</v>
       </c>
       <c r="D29" t="s">
         <v>63</v>
@@ -3217,8 +3226,8 @@
       <c r="J29" t="s">
         <v>62</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>26</v>
+      <c r="K29" s="4" t="s">
+        <v>298</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>63</v>
@@ -3227,13 +3236,13 @@
         <v>64</v>
       </c>
       <c r="N29" t="s">
-        <v>165</v>
+        <v>272</v>
       </c>
       <c r="O29" t="s">
         <v>188</v>
       </c>
       <c r="P29">
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="Q29" t="s">
         <v>189</v>
@@ -3247,7 +3256,7 @@
         <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>253</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
         <v>63</v>
@@ -3270,8 +3279,8 @@
       <c r="J30" t="s">
         <v>62</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>292</v>
+      <c r="K30" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>63</v>
@@ -3280,13 +3289,13 @@
         <v>64</v>
       </c>
       <c r="N30" t="s">
-        <v>260</v>
+        <v>165</v>
       </c>
       <c r="O30" t="s">
         <v>188</v>
       </c>
       <c r="P30">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="Q30" t="s">
         <v>189</v>
@@ -3300,7 +3309,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>252</v>
       </c>
       <c r="D31" t="s">
         <v>63</v>
@@ -3323,8 +3332,8 @@
       <c r="J31" t="s">
         <v>62</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>38</v>
+      <c r="K31" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>63</v>
@@ -3333,13 +3342,13 @@
         <v>64</v>
       </c>
       <c r="N31" t="s">
-        <v>168</v>
+        <v>259</v>
       </c>
       <c r="O31" t="s">
         <v>188</v>
       </c>
       <c r="P31">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="Q31" t="s">
         <v>189</v>
@@ -3353,7 +3362,7 @@
         <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" t="s">
         <v>63</v>
@@ -3377,7 +3386,7 @@
         <v>62</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>63</v>
@@ -3386,13 +3395,13 @@
         <v>64</v>
       </c>
       <c r="N32" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="O32" t="s">
         <v>188</v>
       </c>
       <c r="P32">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="Q32" t="s">
         <v>189</v>
@@ -3406,7 +3415,7 @@
         <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
         <v>63</v>
@@ -3430,7 +3439,7 @@
         <v>62</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>63</v>
@@ -3439,13 +3448,13 @@
         <v>64</v>
       </c>
       <c r="N33" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="O33" t="s">
         <v>188</v>
       </c>
       <c r="P33">
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="Q33" t="s">
         <v>189</v>
@@ -3459,7 +3468,7 @@
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" t="s">
         <v>63</v>
@@ -3483,7 +3492,7 @@
         <v>62</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>63</v>
@@ -3492,13 +3501,13 @@
         <v>64</v>
       </c>
       <c r="N34" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="O34" t="s">
         <v>188</v>
       </c>
       <c r="P34">
-        <v>500000</v>
+        <v>250000</v>
       </c>
       <c r="Q34" t="s">
         <v>189</v>
@@ -3512,7 +3521,7 @@
         <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
         <v>63</v>
@@ -3536,7 +3545,7 @@
         <v>62</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>63</v>
@@ -3545,13 +3554,13 @@
         <v>64</v>
       </c>
       <c r="N35" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="O35" t="s">
         <v>188</v>
       </c>
       <c r="P35">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="Q35" t="s">
         <v>189</v>
@@ -3565,7 +3574,7 @@
         <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>
@@ -3589,7 +3598,7 @@
         <v>62</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>63</v>
@@ -3598,13 +3607,13 @@
         <v>64</v>
       </c>
       <c r="N36" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O36" t="s">
         <v>188</v>
       </c>
       <c r="P36">
-        <v>2500000</v>
+        <v>1000000</v>
       </c>
       <c r="Q36" t="s">
         <v>189</v>
@@ -3618,7 +3627,7 @@
         <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>264</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
         <v>63</v>
@@ -3630,7 +3639,7 @@
         <v>62</v>
       </c>
       <c r="G37" t="s">
-        <v>276</v>
+        <v>129</v>
       </c>
       <c r="H37" t="s">
         <v>63</v>
@@ -3641,8 +3650,8 @@
       <c r="J37" t="s">
         <v>62</v>
       </c>
-      <c r="K37" s="4" t="s">
-        <v>297</v>
+      <c r="K37" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>63</v>
@@ -3651,13 +3660,13 @@
         <v>64</v>
       </c>
       <c r="N37" t="s">
-        <v>269</v>
+        <v>163</v>
       </c>
       <c r="O37" t="s">
         <v>188</v>
       </c>
       <c r="P37">
-        <v>500</v>
+        <v>2500000</v>
       </c>
       <c r="Q37" t="s">
         <v>189</v>
@@ -3671,7 +3680,7 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="D38" t="s">
         <v>63</v>
@@ -3683,7 +3692,7 @@
         <v>62</v>
       </c>
       <c r="G38" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H38" t="s">
         <v>63</v>
@@ -3695,7 +3704,7 @@
         <v>62</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>63</v>
@@ -3704,13 +3713,13 @@
         <v>64</v>
       </c>
       <c r="N38" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="O38" t="s">
         <v>188</v>
       </c>
       <c r="P38">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q38" t="s">
         <v>189</v>
@@ -3724,7 +3733,7 @@
         <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D39" t="s">
         <v>63</v>
@@ -3736,7 +3745,7 @@
         <v>62</v>
       </c>
       <c r="G39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H39" t="s">
         <v>63</v>
@@ -3748,7 +3757,7 @@
         <v>62</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>63</v>
@@ -3757,13 +3766,13 @@
         <v>64</v>
       </c>
       <c r="N39" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="O39" t="s">
         <v>188</v>
       </c>
       <c r="P39">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q39" t="s">
         <v>189</v>
@@ -3777,7 +3786,7 @@
         <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="D40" t="s">
         <v>63</v>
@@ -3789,7 +3798,7 @@
         <v>62</v>
       </c>
       <c r="G40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H40" t="s">
         <v>63</v>
@@ -3801,7 +3810,7 @@
         <v>62</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>63</v>
@@ -3810,13 +3819,13 @@
         <v>64</v>
       </c>
       <c r="N40" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="O40" t="s">
         <v>188</v>
       </c>
       <c r="P40">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q40" t="s">
         <v>189</v>
@@ -3830,7 +3839,7 @@
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D41" t="s">
         <v>63</v>
@@ -3842,7 +3851,7 @@
         <v>62</v>
       </c>
       <c r="G41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H41" t="s">
         <v>63</v>
@@ -3853,8 +3862,8 @@
       <c r="J41" t="s">
         <v>62</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>300</v>
+      <c r="K41" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>63</v>
@@ -3863,13 +3872,13 @@
         <v>64</v>
       </c>
       <c r="N41" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="O41" t="s">
         <v>188</v>
       </c>
       <c r="P41">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="Q41" t="s">
         <v>189</v>
@@ -3883,7 +3892,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="D42" t="s">
         <v>63</v>
@@ -3895,7 +3904,7 @@
         <v>62</v>
       </c>
       <c r="G42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H42" t="s">
         <v>63</v>
@@ -3906,8 +3915,8 @@
       <c r="J42" t="s">
         <v>62</v>
       </c>
-      <c r="K42" s="4" t="s">
-        <v>288</v>
+      <c r="K42" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>63</v>
@@ -3916,13 +3925,13 @@
         <v>64</v>
       </c>
       <c r="N42" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="O42" t="s">
         <v>188</v>
       </c>
       <c r="P42">
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="Q42" t="s">
         <v>189</v>
@@ -3936,7 +3945,7 @@
         <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D43" t="s">
         <v>63</v>
@@ -3948,7 +3957,7 @@
         <v>62</v>
       </c>
       <c r="G43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H43" t="s">
         <v>63</v>
@@ -3959,8 +3968,8 @@
       <c r="J43" t="s">
         <v>62</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>291</v>
+      <c r="K43" s="4" t="s">
+        <v>287</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>63</v>
@@ -3969,13 +3978,13 @@
         <v>64</v>
       </c>
       <c r="N43" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="O43" t="s">
         <v>188</v>
       </c>
       <c r="P43">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="Q43" t="s">
         <v>189</v>
@@ -3989,7 +3998,7 @@
         <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D44" t="s">
         <v>63</v>
@@ -4001,7 +4010,7 @@
         <v>62</v>
       </c>
       <c r="G44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H44" t="s">
         <v>63</v>
@@ -4013,7 +4022,7 @@
         <v>62</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>63</v>
@@ -4022,13 +4031,13 @@
         <v>64</v>
       </c>
       <c r="N44" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="O44" t="s">
         <v>188</v>
       </c>
       <c r="P44">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="Q44" t="s">
         <v>189</v>
@@ -4042,7 +4051,7 @@
         <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>255</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -4054,7 +4063,7 @@
         <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>123</v>
+        <v>275</v>
       </c>
       <c r="H45" t="s">
         <v>63</v>
@@ -4065,8 +4074,8 @@
       <c r="J45" t="s">
         <v>62</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>2</v>
+      <c r="K45" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>63</v>
@@ -4075,13 +4084,13 @@
         <v>64</v>
       </c>
       <c r="N45" t="s">
-        <v>134</v>
+        <v>266</v>
       </c>
       <c r="O45" t="s">
         <v>188</v>
       </c>
       <c r="P45">
-        <v>1</v>
+        <v>50000</v>
       </c>
       <c r="Q45" t="s">
         <v>189</v>
@@ -4095,7 +4104,7 @@
         <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s">
         <v>63</v>
@@ -4119,7 +4128,7 @@
         <v>62</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>63</v>
@@ -4128,13 +4137,13 @@
         <v>64</v>
       </c>
       <c r="N46" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O46" t="s">
         <v>188</v>
       </c>
       <c r="P46">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q46" t="s">
         <v>189</v>
@@ -4148,7 +4157,7 @@
         <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D47" t="s">
         <v>63</v>
@@ -4172,7 +4181,7 @@
         <v>62</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>63</v>
@@ -4181,13 +4190,13 @@
         <v>64</v>
       </c>
       <c r="N47" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="O47" t="s">
         <v>188</v>
       </c>
       <c r="P47">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q47" t="s">
         <v>189</v>
@@ -4201,7 +4210,7 @@
         <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D48" t="s">
         <v>63</v>
@@ -4225,7 +4234,7 @@
         <v>62</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>63</v>
@@ -4234,13 +4243,13 @@
         <v>64</v>
       </c>
       <c r="N48" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O48" t="s">
         <v>188</v>
       </c>
       <c r="P48">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q48" t="s">
         <v>189</v>
@@ -4254,7 +4263,7 @@
         <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D49" t="s">
         <v>63</v>
@@ -4278,7 +4287,7 @@
         <v>62</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>63</v>
@@ -4287,13 +4296,13 @@
         <v>64</v>
       </c>
       <c r="N49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O49" t="s">
         <v>188</v>
       </c>
       <c r="P49">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="Q49" t="s">
         <v>189</v>
@@ -4307,7 +4316,7 @@
         <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
         <v>63</v>
@@ -4331,7 +4340,7 @@
         <v>62</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>207</v>
+        <v>5</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>63</v>
@@ -4340,13 +4349,13 @@
         <v>64</v>
       </c>
       <c r="N50" t="s">
-        <v>208</v>
+        <v>137</v>
       </c>
       <c r="O50" t="s">
         <v>188</v>
       </c>
       <c r="P50">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q50" t="s">
         <v>189</v>
@@ -4360,7 +4369,7 @@
         <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D51" t="s">
         <v>63</v>
@@ -4384,7 +4393,7 @@
         <v>62</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>63</v>
@@ -4393,13 +4402,13 @@
         <v>64</v>
       </c>
       <c r="N51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O51" t="s">
         <v>188</v>
       </c>
       <c r="P51">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="Q51" t="s">
         <v>189</v>
@@ -4413,7 +4422,7 @@
         <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D52" t="s">
         <v>63</v>
@@ -4437,7 +4446,7 @@
         <v>62</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>63</v>
@@ -4446,13 +4455,13 @@
         <v>64</v>
       </c>
       <c r="N52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="O52" t="s">
         <v>188</v>
       </c>
       <c r="P52">
-        <v>1000000</v>
+        <v>500</v>
       </c>
       <c r="Q52" t="s">
         <v>189</v>
@@ -4466,7 +4475,7 @@
         <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53" t="s">
         <v>63</v>
@@ -4478,7 +4487,7 @@
         <v>62</v>
       </c>
       <c r="G53" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H53" t="s">
         <v>63</v>
@@ -4490,7 +4499,7 @@
         <v>62</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>45</v>
+        <v>211</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>63</v>
@@ -4499,13 +4508,13 @@
         <v>64</v>
       </c>
       <c r="N53" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="O53" t="s">
         <v>188</v>
       </c>
       <c r="P53">
-        <v>10</v>
+        <v>1000000</v>
       </c>
       <c r="Q53" t="s">
         <v>189</v>
@@ -4519,7 +4528,7 @@
         <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D54" t="s">
         <v>63</v>
@@ -4543,7 +4552,7 @@
         <v>62</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>63</v>
@@ -4552,13 +4561,13 @@
         <v>64</v>
       </c>
       <c r="N54" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O54" t="s">
         <v>188</v>
       </c>
       <c r="P54">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="Q54" t="s">
         <v>189</v>
@@ -4572,7 +4581,7 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D55" t="s">
         <v>63</v>
@@ -4596,7 +4605,7 @@
         <v>62</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>63</v>
@@ -4605,7 +4614,7 @@
         <v>64</v>
       </c>
       <c r="N55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O55" t="s">
         <v>188</v>
@@ -4625,7 +4634,7 @@
         <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56" t="s">
         <v>63</v>
@@ -4649,7 +4658,7 @@
         <v>62</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>63</v>
@@ -4658,13 +4667,13 @@
         <v>64</v>
       </c>
       <c r="N56" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="O56" t="s">
         <v>188</v>
       </c>
       <c r="P56">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="Q56" t="s">
         <v>189</v>
@@ -4678,7 +4687,7 @@
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D57" t="s">
         <v>63</v>
@@ -4702,7 +4711,7 @@
         <v>62</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>63</v>
@@ -4711,7 +4720,7 @@
         <v>64</v>
       </c>
       <c r="N57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="O57" t="s">
         <v>188</v>
@@ -4731,7 +4740,7 @@
         <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D58" t="s">
         <v>63</v>
@@ -4755,7 +4764,7 @@
         <v>62</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>63</v>
@@ -4764,13 +4773,13 @@
         <v>64</v>
       </c>
       <c r="N58" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="O58" t="s">
         <v>188</v>
       </c>
       <c r="P58">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="Q58" t="s">
         <v>189</v>
@@ -4784,7 +4793,7 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D59" t="s">
         <v>63</v>
@@ -4808,7 +4817,7 @@
         <v>62</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>63</v>
@@ -4817,7 +4826,7 @@
         <v>64</v>
       </c>
       <c r="N59" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="O59" t="s">
         <v>188</v>
@@ -4837,7 +4846,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D60" t="s">
         <v>63</v>
@@ -4861,7 +4870,7 @@
         <v>62</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>63</v>
@@ -4870,13 +4879,13 @@
         <v>64</v>
       </c>
       <c r="N60" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="O60" t="s">
         <v>188</v>
       </c>
       <c r="P60">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q60" t="s">
         <v>189</v>
@@ -4890,7 +4899,7 @@
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -4914,7 +4923,7 @@
         <v>62</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>63</v>
@@ -4923,7 +4932,7 @@
         <v>64</v>
       </c>
       <c r="N61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O61" t="s">
         <v>188</v>
@@ -4943,7 +4952,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D62" t="s">
         <v>63</v>
@@ -4967,7 +4976,7 @@
         <v>62</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>63</v>
@@ -4976,13 +4985,13 @@
         <v>64</v>
       </c>
       <c r="N62" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="O62" t="s">
         <v>188</v>
       </c>
       <c r="P62">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q62" t="s">
         <v>189</v>
@@ -4996,7 +5005,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D63" t="s">
         <v>63</v>
@@ -5020,7 +5029,7 @@
         <v>62</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>63</v>
@@ -5029,7 +5038,7 @@
         <v>64</v>
       </c>
       <c r="N63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O63" t="s">
         <v>188</v>
@@ -5049,7 +5058,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
         <v>63</v>
@@ -5073,7 +5082,7 @@
         <v>62</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>63</v>
@@ -5082,13 +5091,13 @@
         <v>64</v>
       </c>
       <c r="N64" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="O64" t="s">
         <v>188</v>
       </c>
       <c r="P64">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q64" t="s">
         <v>189</v>
@@ -5102,7 +5111,7 @@
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D65" t="s">
         <v>63</v>
@@ -5126,7 +5135,7 @@
         <v>62</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>63</v>
@@ -5135,13 +5144,13 @@
         <v>64</v>
       </c>
       <c r="N65" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="O65" t="s">
         <v>188</v>
       </c>
       <c r="P65">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="Q65" t="s">
         <v>189</v>
@@ -5155,7 +5164,7 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D66" t="s">
         <v>63</v>
@@ -5179,7 +5188,7 @@
         <v>62</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>63</v>
@@ -5188,13 +5197,13 @@
         <v>64</v>
       </c>
       <c r="N66" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="O66" t="s">
         <v>188</v>
       </c>
       <c r="P66">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="Q66" t="s">
         <v>189</v>
@@ -5208,7 +5217,7 @@
         <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D67" t="s">
         <v>63</v>
@@ -5232,7 +5241,7 @@
         <v>62</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>63</v>
@@ -5241,13 +5250,13 @@
         <v>64</v>
       </c>
       <c r="N67" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="O67" t="s">
         <v>188</v>
       </c>
       <c r="P67">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="Q67" t="s">
         <v>189</v>
@@ -5261,7 +5270,7 @@
         <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D68" t="s">
         <v>63</v>
@@ -5273,7 +5282,7 @@
         <v>62</v>
       </c>
       <c r="G68" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H68" t="s">
         <v>63</v>
@@ -5285,7 +5294,7 @@
         <v>62</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>63</v>
@@ -5294,13 +5303,13 @@
         <v>64</v>
       </c>
       <c r="N68" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="O68" t="s">
         <v>188</v>
       </c>
       <c r="P68">
-        <v>50</v>
+        <v>100000</v>
       </c>
       <c r="Q68" t="s">
         <v>189</v>
@@ -5314,7 +5323,7 @@
         <v>62</v>
       </c>
       <c r="C69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D69" t="s">
         <v>63</v>
@@ -5338,7 +5347,7 @@
         <v>62</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>63</v>
@@ -5347,13 +5356,13 @@
         <v>64</v>
       </c>
       <c r="N69" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O69" t="s">
         <v>188</v>
       </c>
       <c r="P69">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="Q69" t="s">
         <v>189</v>
@@ -5367,7 +5376,7 @@
         <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D70" t="s">
         <v>63</v>
@@ -5391,7 +5400,7 @@
         <v>62</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>63</v>
@@ -5400,13 +5409,13 @@
         <v>64</v>
       </c>
       <c r="N70" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O70" t="s">
         <v>188</v>
       </c>
       <c r="P70">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q70" t="s">
         <v>189</v>
@@ -5420,7 +5429,7 @@
         <v>62</v>
       </c>
       <c r="C71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D71" t="s">
         <v>63</v>
@@ -5444,7 +5453,7 @@
         <v>62</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>63</v>
@@ -5453,13 +5462,13 @@
         <v>64</v>
       </c>
       <c r="N71" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O71" t="s">
         <v>188</v>
       </c>
       <c r="P71">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="Q71" t="s">
         <v>189</v>
@@ -5473,7 +5482,7 @@
         <v>62</v>
       </c>
       <c r="C72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D72" t="s">
         <v>63</v>
@@ -5497,7 +5506,7 @@
         <v>62</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>63</v>
@@ -5506,13 +5515,13 @@
         <v>64</v>
       </c>
       <c r="N72" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="O72" t="s">
         <v>188</v>
       </c>
       <c r="P72">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q72" t="s">
         <v>189</v>
@@ -5526,7 +5535,7 @@
         <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D73" t="s">
         <v>63</v>
@@ -5550,7 +5559,7 @@
         <v>62</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>63</v>
@@ -5559,13 +5568,13 @@
         <v>64</v>
       </c>
       <c r="N73" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="O73" t="s">
         <v>188</v>
       </c>
       <c r="P73">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q73" t="s">
         <v>189</v>
@@ -5579,7 +5588,7 @@
         <v>62</v>
       </c>
       <c r="C74" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D74" t="s">
         <v>63</v>
@@ -5603,7 +5612,7 @@
         <v>62</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>63</v>
@@ -5612,13 +5621,13 @@
         <v>64</v>
       </c>
       <c r="N74" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O74" t="s">
         <v>188</v>
       </c>
       <c r="P74">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q74" t="s">
         <v>189</v>
@@ -5632,7 +5641,7 @@
         <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D75" t="s">
         <v>63</v>
@@ -5656,7 +5665,7 @@
         <v>62</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>63</v>
@@ -5665,13 +5674,13 @@
         <v>64</v>
       </c>
       <c r="N75" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="O75" t="s">
         <v>188</v>
       </c>
       <c r="P75">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="Q75" t="s">
         <v>189</v>
@@ -5685,7 +5694,7 @@
         <v>62</v>
       </c>
       <c r="C76" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D76" t="s">
         <v>63</v>
@@ -5697,7 +5706,7 @@
         <v>62</v>
       </c>
       <c r="G76" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H76" t="s">
         <v>63</v>
@@ -5709,7 +5718,7 @@
         <v>62</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>63</v>
@@ -5718,13 +5727,13 @@
         <v>64</v>
       </c>
       <c r="N76" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="O76" t="s">
         <v>188</v>
       </c>
       <c r="P76">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="Q76" t="s">
         <v>189</v>
@@ -5738,7 +5747,7 @@
         <v>62</v>
       </c>
       <c r="C77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D77" t="s">
         <v>63</v>
@@ -5762,7 +5771,7 @@
         <v>62</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>63</v>
@@ -5791,7 +5800,7 @@
         <v>62</v>
       </c>
       <c r="C78" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D78" t="s">
         <v>63</v>
@@ -5815,7 +5824,7 @@
         <v>62</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>63</v>
@@ -5844,7 +5853,7 @@
         <v>62</v>
       </c>
       <c r="C79" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D79" t="s">
         <v>63</v>
@@ -5868,7 +5877,7 @@
         <v>62</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>63</v>
@@ -5877,13 +5886,13 @@
         <v>64</v>
       </c>
       <c r="N79" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="O79" t="s">
         <v>188</v>
       </c>
       <c r="P79">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q79" t="s">
         <v>189</v>
@@ -5897,7 +5906,7 @@
         <v>62</v>
       </c>
       <c r="C80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D80" t="s">
         <v>63</v>
@@ -5921,7 +5930,7 @@
         <v>62</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>63</v>
@@ -5930,13 +5939,13 @@
         <v>64</v>
       </c>
       <c r="N80" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="O80" t="s">
         <v>188</v>
       </c>
       <c r="P80">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q80" t="s">
         <v>189</v>
@@ -5950,7 +5959,7 @@
         <v>62</v>
       </c>
       <c r="C81" t="s">
-        <v>265</v>
+        <v>114</v>
       </c>
       <c r="D81" t="s">
         <v>63</v>
@@ -5973,8 +5982,8 @@
       <c r="J81" t="s">
         <v>62</v>
       </c>
-      <c r="K81" s="3" t="s">
-        <v>298</v>
+      <c r="K81" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="L81" s="1" t="s">
         <v>63</v>
@@ -5983,13 +5992,13 @@
         <v>64</v>
       </c>
       <c r="N81" t="s">
-        <v>270</v>
+        <v>158</v>
       </c>
       <c r="O81" t="s">
         <v>188</v>
       </c>
       <c r="P81">
-        <v>75000</v>
+        <v>5000</v>
       </c>
       <c r="Q81" t="s">
         <v>189</v>
@@ -6003,7 +6012,7 @@
         <v>62</v>
       </c>
       <c r="C82" t="s">
-        <v>118</v>
+        <v>264</v>
       </c>
       <c r="D82" t="s">
         <v>63</v>
@@ -6015,7 +6024,7 @@
         <v>62</v>
       </c>
       <c r="G82" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H82" t="s">
         <v>63</v>
@@ -6026,8 +6035,8 @@
       <c r="J82" t="s">
         <v>62</v>
       </c>
-      <c r="K82" s="1" t="s">
-        <v>190</v>
+      <c r="K82" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>63</v>
@@ -6036,13 +6045,13 @@
         <v>64</v>
       </c>
       <c r="N82" t="s">
-        <v>131</v>
+        <v>269</v>
       </c>
       <c r="O82" t="s">
         <v>188</v>
       </c>
       <c r="P82">
-        <v>50</v>
+        <v>75000</v>
       </c>
       <c r="Q82" t="s">
         <v>189</v>
@@ -6056,7 +6065,7 @@
         <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D83" t="s">
         <v>63</v>
@@ -6080,7 +6089,7 @@
         <v>62</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>63</v>
@@ -6089,13 +6098,13 @@
         <v>64</v>
       </c>
       <c r="N83" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O83" t="s">
         <v>188</v>
       </c>
       <c r="P83">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="Q83" t="s">
         <v>189</v>
@@ -6109,7 +6118,7 @@
         <v>62</v>
       </c>
       <c r="C84" t="s">
-        <v>224</v>
+        <v>119</v>
       </c>
       <c r="D84" t="s">
         <v>63</v>
@@ -6132,8 +6141,8 @@
       <c r="J84" t="s">
         <v>62</v>
       </c>
-      <c r="K84" s="3" t="s">
-        <v>277</v>
+      <c r="K84" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>63</v>
@@ -6142,13 +6151,13 @@
         <v>64</v>
       </c>
       <c r="N84" t="s">
-        <v>230</v>
+        <v>130</v>
       </c>
       <c r="O84" t="s">
         <v>188</v>
       </c>
       <c r="P84">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="Q84" t="s">
         <v>189</v>
@@ -6162,7 +6171,7 @@
         <v>62</v>
       </c>
       <c r="C85" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D85" t="s">
         <v>63</v>
@@ -6185,8 +6194,8 @@
       <c r="J85" t="s">
         <v>62</v>
       </c>
-      <c r="K85" s="1" t="s">
-        <v>280</v>
+      <c r="K85" s="3" t="s">
+        <v>276</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>63</v>
@@ -6195,13 +6204,13 @@
         <v>64</v>
       </c>
       <c r="N85" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="O85" t="s">
         <v>188</v>
       </c>
       <c r="P85">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q85" t="s">
         <v>189</v>
@@ -6215,7 +6224,7 @@
         <v>62</v>
       </c>
       <c r="C86" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D86" t="s">
         <v>63</v>
@@ -6239,7 +6248,7 @@
         <v>62</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>63</v>
@@ -6248,13 +6257,13 @@
         <v>64</v>
       </c>
       <c r="N86" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="O86" t="s">
         <v>188</v>
       </c>
       <c r="P86">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="Q86" t="s">
         <v>189</v>
@@ -6268,7 +6277,7 @@
         <v>62</v>
       </c>
       <c r="C87" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D87" t="s">
         <v>63</v>
@@ -6301,13 +6310,13 @@
         <v>64</v>
       </c>
       <c r="N87" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O87" t="s">
         <v>188</v>
       </c>
       <c r="P87">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="Q87" t="s">
         <v>189</v>
@@ -6321,7 +6330,7 @@
         <v>62</v>
       </c>
       <c r="C88" t="s">
-        <v>120</v>
+        <v>228</v>
       </c>
       <c r="D88" t="s">
         <v>63</v>
@@ -6345,7 +6354,7 @@
         <v>62</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>37</v>
+        <v>280</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>63</v>
@@ -6354,13 +6363,13 @@
         <v>64</v>
       </c>
       <c r="N88" t="s">
-        <v>166</v>
+        <v>234</v>
       </c>
       <c r="O88" t="s">
         <v>188</v>
       </c>
       <c r="P88">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="Q88" t="s">
         <v>189</v>
@@ -6374,7 +6383,7 @@
         <v>62</v>
       </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>120</v>
       </c>
       <c r="D89" t="s">
         <v>63</v>
@@ -6397,8 +6406,8 @@
       <c r="J89" t="s">
         <v>62</v>
       </c>
-      <c r="K89" s="3" t="s">
-        <v>278</v>
+      <c r="K89" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>63</v>
@@ -6407,13 +6416,13 @@
         <v>64</v>
       </c>
       <c r="N89" t="s">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="O89" t="s">
         <v>188</v>
       </c>
       <c r="P89">
-        <v>75000</v>
+        <v>50000</v>
       </c>
       <c r="Q89" t="s">
         <v>189</v>
@@ -6427,7 +6436,7 @@
         <v>62</v>
       </c>
       <c r="C90" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D90" t="s">
         <v>63</v>
@@ -6451,7 +6460,7 @@
         <v>62</v>
       </c>
       <c r="K90" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>63</v>
@@ -6460,13 +6469,13 @@
         <v>64</v>
       </c>
       <c r="N90" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O90" t="s">
         <v>188</v>
       </c>
       <c r="P90">
-        <v>100000</v>
+        <v>75000</v>
       </c>
       <c r="Q90" t="s">
         <v>189</v>
@@ -6480,7 +6489,7 @@
         <v>62</v>
       </c>
       <c r="C91" t="s">
-        <v>121</v>
+        <v>226</v>
       </c>
       <c r="D91" t="s">
         <v>63</v>
@@ -6503,31 +6512,80 @@
       <c r="J91" t="s">
         <v>62</v>
       </c>
-      <c r="K91" s="1" t="s">
+      <c r="K91" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M91" t="s">
+        <v>64</v>
+      </c>
+      <c r="N91" t="s">
+        <v>232</v>
+      </c>
+      <c r="O91" t="s">
+        <v>188</v>
+      </c>
+      <c r="P91">
+        <v>100000</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>61</v>
+      </c>
+      <c r="B92" t="s">
+        <v>62</v>
+      </c>
+      <c r="C92" t="s">
+        <v>121</v>
+      </c>
+      <c r="D92" t="s">
+        <v>63</v>
+      </c>
+      <c r="E92" t="s">
+        <v>122</v>
+      </c>
+      <c r="F92" t="s">
+        <v>62</v>
+      </c>
+      <c r="G92" t="s">
+        <v>125</v>
+      </c>
+      <c r="H92" t="s">
+        <v>63</v>
+      </c>
+      <c r="I92" t="s">
+        <v>60</v>
+      </c>
+      <c r="J92" t="s">
+        <v>62</v>
+      </c>
+      <c r="K92" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L91" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M91" t="s">
-        <v>64</v>
-      </c>
-      <c r="N91" t="s">
+      <c r="L92" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M92" t="s">
+        <v>64</v>
+      </c>
+      <c r="N92" t="s">
         <v>162</v>
       </c>
-      <c r="O91" t="s">
-        <v>188</v>
-      </c>
-      <c r="P91">
+      <c r="O92" t="s">
+        <v>188</v>
+      </c>
+      <c r="P92">
         <v>500000</v>
       </c>
-      <c r="Q91" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
+      <c r="Q92" t="s">
+        <v>189</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added reward for september
</commit_message>
<xml_diff>
--- a/HutListe.xlsx
+++ b/HutListe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1505" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="327">
   <si>
     <t>states/schaf.png</t>
   </si>
@@ -1285,6 +1285,51 @@
   </si>
   <si>
     <t>pics/sm_macguffin2012-item_08.png</t>
+  </si>
+  <si>
+    <t>&amp;07</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison September.</t>
+  </si>
+  <si>
+    <t>&amp;08</t>
+  </si>
+  <si>
+    <t>&amp;09</t>
+  </si>
+  <si>
+    <t>&amp;10</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison Januar.</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison Februar.</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison Juli.</t>
+  </si>
+  <si>
+    <t>&amp;11</t>
+  </si>
+  <si>
+    <t>&amp;12</t>
+  </si>
+  <si>
+    <t>&amp;13</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison Oktober.</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison November.</t>
+  </si>
+  <si>
+    <t>Die Belohnung für das Erreichen von 1.000 Punkten in der Saison Dezember.</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_11-10_frankenstein.gif</t>
   </si>
 </sst>
 </file>
@@ -1413,10 +1458,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:Q94" totalsRowShown="0">
-  <autoFilter ref="A1:Q94"/>
-  <sortState ref="A2:Q94">
-    <sortCondition ref="G1:G94"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:Q101" totalsRowShown="0">
+  <autoFilter ref="A1:Q101"/>
+  <sortState ref="A2:Q101">
+    <sortCondition ref="G1:G101"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" name="A"/>
@@ -1696,7 +1741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1704,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q94"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q94"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="S88" sqref="S88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2426,7 +2471,7 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>205</v>
+        <v>312</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
@@ -2438,7 +2483,7 @@
         <v>62</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="H14" t="s">
         <v>63</v>
@@ -2450,7 +2495,7 @@
         <v>62</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>27</v>
+        <v>326</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>63</v>
@@ -2459,13 +2504,13 @@
         <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>139</v>
+        <v>313</v>
       </c>
       <c r="O14" t="s">
         <v>187</v>
       </c>
       <c r="P14">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="s">
         <v>188</v>
@@ -2479,7 +2524,7 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>314</v>
       </c>
       <c r="D15" t="s">
         <v>63</v>
@@ -2491,7 +2536,7 @@
         <v>62</v>
       </c>
       <c r="G15" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="H15" t="s">
         <v>63</v>
@@ -2502,9 +2547,7 @@
       <c r="J15" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
         <v>63</v>
       </c>
@@ -2512,13 +2555,13 @@
         <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>140</v>
+        <v>317</v>
       </c>
       <c r="O15" t="s">
         <v>187</v>
       </c>
       <c r="P15">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="s">
         <v>188</v>
@@ -2532,7 +2575,7 @@
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>315</v>
       </c>
       <c r="D16" t="s">
         <v>63</v>
@@ -2544,7 +2587,7 @@
         <v>62</v>
       </c>
       <c r="G16" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="H16" t="s">
         <v>63</v>
@@ -2555,9 +2598,7 @@
       <c r="J16" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
         <v>63</v>
       </c>
@@ -2565,13 +2606,13 @@
         <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>141</v>
+        <v>318</v>
       </c>
       <c r="O16" t="s">
         <v>187</v>
       </c>
       <c r="P16">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="s">
         <v>188</v>
@@ -2585,7 +2626,7 @@
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>316</v>
       </c>
       <c r="D17" t="s">
         <v>63</v>
@@ -2597,7 +2638,7 @@
         <v>62</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="H17" t="s">
         <v>63</v>
@@ -2608,9 +2649,7 @@
       <c r="J17" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
         <v>63</v>
       </c>
@@ -2618,13 +2657,13 @@
         <v>64</v>
       </c>
       <c r="N17" t="s">
-        <v>142</v>
+        <v>319</v>
       </c>
       <c r="O17" t="s">
         <v>187</v>
       </c>
       <c r="P17">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="s">
         <v>188</v>
@@ -2638,7 +2677,7 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>320</v>
       </c>
       <c r="D18" t="s">
         <v>63</v>
@@ -2650,7 +2689,7 @@
         <v>62</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="H18" t="s">
         <v>63</v>
@@ -2661,9 +2700,7 @@
       <c r="J18" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
         <v>63</v>
       </c>
@@ -2671,13 +2708,13 @@
         <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>148</v>
+        <v>323</v>
       </c>
       <c r="O18" t="s">
         <v>187</v>
       </c>
       <c r="P18">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="s">
         <v>188</v>
@@ -2691,7 +2728,7 @@
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>321</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -2703,7 +2740,7 @@
         <v>62</v>
       </c>
       <c r="G19" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="H19" t="s">
         <v>63</v>
@@ -2714,9 +2751,7 @@
       <c r="J19" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
         <v>63</v>
       </c>
@@ -2724,13 +2759,13 @@
         <v>64</v>
       </c>
       <c r="N19" t="s">
-        <v>149</v>
+        <v>324</v>
       </c>
       <c r="O19" t="s">
         <v>187</v>
       </c>
       <c r="P19">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="Q19" t="s">
         <v>188</v>
@@ -2744,7 +2779,7 @@
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>252</v>
+        <v>322</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
@@ -2756,7 +2791,7 @@
         <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>197</v>
       </c>
       <c r="H20" t="s">
         <v>63</v>
@@ -2767,9 +2802,7 @@
       <c r="J20" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>291</v>
-      </c>
+      <c r="K20" s="1"/>
       <c r="L20" s="1" t="s">
         <v>63</v>
       </c>
@@ -2777,13 +2810,13 @@
         <v>64</v>
       </c>
       <c r="N20" t="s">
-        <v>259</v>
+        <v>325</v>
       </c>
       <c r="O20" t="s">
         <v>187</v>
       </c>
       <c r="P20">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Q20" t="s">
         <v>188</v>
@@ -2797,7 +2830,7 @@
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>270</v>
+        <v>205</v>
       </c>
       <c r="D21" t="s">
         <v>63</v>
@@ -2820,8 +2853,8 @@
       <c r="J21" t="s">
         <v>62</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>299</v>
+      <c r="K21" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>63</v>
@@ -2830,13 +2863,13 @@
         <v>64</v>
       </c>
       <c r="N21" t="s">
-        <v>273</v>
+        <v>139</v>
       </c>
       <c r="O21" t="s">
         <v>187</v>
       </c>
       <c r="P21">
-        <v>2500</v>
+        <v>25</v>
       </c>
       <c r="Q21" t="s">
         <v>188</v>
@@ -2850,7 +2883,7 @@
         <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
         <v>63</v>
@@ -2874,7 +2907,7 @@
         <v>62</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>63</v>
@@ -2883,13 +2916,13 @@
         <v>64</v>
       </c>
       <c r="N22" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="O22" t="s">
         <v>187</v>
       </c>
       <c r="P22">
-        <v>5000</v>
+        <v>25</v>
       </c>
       <c r="Q22" t="s">
         <v>188</v>
@@ -2903,7 +2936,7 @@
         <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>235</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
@@ -2926,8 +2959,8 @@
       <c r="J23" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>281</v>
+      <c r="K23" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>63</v>
@@ -2936,13 +2969,13 @@
         <v>64</v>
       </c>
       <c r="N23" t="s">
-        <v>237</v>
+        <v>141</v>
       </c>
       <c r="O23" t="s">
         <v>187</v>
       </c>
       <c r="P23">
-        <v>7500</v>
+        <v>25</v>
       </c>
       <c r="Q23" t="s">
         <v>188</v>
@@ -2956,7 +2989,7 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
@@ -2980,7 +3013,7 @@
         <v>62</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>63</v>
@@ -2989,13 +3022,13 @@
         <v>64</v>
       </c>
       <c r="N24" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="O24" t="s">
         <v>187</v>
       </c>
       <c r="P24">
-        <v>10000</v>
+        <v>25</v>
       </c>
       <c r="Q24" t="s">
         <v>188</v>
@@ -3009,7 +3042,7 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>239</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
@@ -3032,8 +3065,8 @@
       <c r="J25" t="s">
         <v>62</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>284</v>
+      <c r="K25" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>63</v>
@@ -3042,13 +3075,13 @@
         <v>64</v>
       </c>
       <c r="N25" t="s">
-        <v>247</v>
+        <v>148</v>
       </c>
       <c r="O25" t="s">
         <v>187</v>
       </c>
       <c r="P25">
-        <v>25000</v>
+        <v>100</v>
       </c>
       <c r="Q25" t="s">
         <v>188</v>
@@ -3062,7 +3095,7 @@
         <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>63</v>
@@ -3074,7 +3107,7 @@
         <v>62</v>
       </c>
       <c r="G26" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H26" t="s">
         <v>63</v>
@@ -3086,7 +3119,7 @@
         <v>62</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>63</v>
@@ -3095,13 +3128,13 @@
         <v>64</v>
       </c>
       <c r="N26" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="O26" t="s">
         <v>187</v>
       </c>
       <c r="P26">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="Q26" t="s">
         <v>188</v>
@@ -3115,7 +3148,7 @@
         <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="D27" t="s">
         <v>63</v>
@@ -3127,7 +3160,7 @@
         <v>62</v>
       </c>
       <c r="G27" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H27" t="s">
         <v>63</v>
@@ -3139,7 +3172,7 @@
         <v>62</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>63</v>
@@ -3148,13 +3181,13 @@
         <v>64</v>
       </c>
       <c r="N27" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="O27" t="s">
         <v>187</v>
       </c>
       <c r="P27">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="Q27" t="s">
         <v>188</v>
@@ -3168,7 +3201,7 @@
         <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>270</v>
       </c>
       <c r="D28" t="s">
         <v>63</v>
@@ -3180,7 +3213,7 @@
         <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H28" t="s">
         <v>63</v>
@@ -3191,8 +3224,8 @@
       <c r="J28" t="s">
         <v>62</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>31</v>
+      <c r="K28" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>63</v>
@@ -3201,13 +3234,13 @@
         <v>64</v>
       </c>
       <c r="N28" t="s">
-        <v>143</v>
+        <v>273</v>
       </c>
       <c r="O28" t="s">
         <v>187</v>
       </c>
       <c r="P28">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="Q28" t="s">
         <v>188</v>
@@ -3221,7 +3254,7 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>242</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
         <v>63</v>
@@ -3233,7 +3266,7 @@
         <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H29" t="s">
         <v>63</v>
@@ -3244,8 +3277,8 @@
       <c r="J29" t="s">
         <v>62</v>
       </c>
-      <c r="K29" s="4" t="s">
-        <v>287</v>
+      <c r="K29" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>63</v>
@@ -3254,13 +3287,13 @@
         <v>64</v>
       </c>
       <c r="N29" t="s">
-        <v>255</v>
+        <v>157</v>
       </c>
       <c r="O29" t="s">
         <v>187</v>
       </c>
       <c r="P29">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="Q29" t="s">
         <v>188</v>
@@ -3274,7 +3307,7 @@
         <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>235</v>
       </c>
       <c r="D30" t="s">
         <v>63</v>
@@ -3286,7 +3319,7 @@
         <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H30" t="s">
         <v>63</v>
@@ -3297,8 +3330,8 @@
       <c r="J30" t="s">
         <v>62</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>24</v>
+      <c r="K30" s="3" t="s">
+        <v>281</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>63</v>
@@ -3307,13 +3340,13 @@
         <v>64</v>
       </c>
       <c r="N30" t="s">
-        <v>163</v>
+        <v>237</v>
       </c>
       <c r="O30" t="s">
         <v>187</v>
       </c>
       <c r="P30">
-        <v>5000</v>
+        <v>7500</v>
       </c>
       <c r="Q30" t="s">
         <v>188</v>
@@ -3327,7 +3360,7 @@
         <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>264</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
         <v>63</v>
@@ -3339,7 +3372,7 @@
         <v>62</v>
       </c>
       <c r="G31" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H31" t="s">
         <v>63</v>
@@ -3350,8 +3383,8 @@
       <c r="J31" t="s">
         <v>62</v>
       </c>
-      <c r="K31" s="4" t="s">
-        <v>297</v>
+      <c r="K31" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>63</v>
@@ -3360,13 +3393,13 @@
         <v>64</v>
       </c>
       <c r="N31" t="s">
-        <v>271</v>
+        <v>160</v>
       </c>
       <c r="O31" t="s">
         <v>187</v>
       </c>
       <c r="P31">
-        <v>7500</v>
+        <v>10000</v>
       </c>
       <c r="Q31" t="s">
         <v>188</v>
@@ -3380,7 +3413,7 @@
         <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>239</v>
       </c>
       <c r="D32" t="s">
         <v>63</v>
@@ -3392,7 +3425,7 @@
         <v>62</v>
       </c>
       <c r="G32" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H32" t="s">
         <v>63</v>
@@ -3403,8 +3436,8 @@
       <c r="J32" t="s">
         <v>62</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>26</v>
+      <c r="K32" s="4" t="s">
+        <v>284</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>63</v>
@@ -3413,13 +3446,13 @@
         <v>64</v>
       </c>
       <c r="N32" t="s">
-        <v>164</v>
+        <v>247</v>
       </c>
       <c r="O32" t="s">
         <v>187</v>
       </c>
       <c r="P32">
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="Q32" t="s">
         <v>188</v>
@@ -3433,7 +3466,7 @@
         <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>251</v>
+        <v>72</v>
       </c>
       <c r="D33" t="s">
         <v>63</v>
@@ -3456,8 +3489,8 @@
       <c r="J33" t="s">
         <v>62</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>290</v>
+      <c r="K33" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>63</v>
@@ -3466,13 +3499,13 @@
         <v>64</v>
       </c>
       <c r="N33" t="s">
-        <v>258</v>
+        <v>133</v>
       </c>
       <c r="O33" t="s">
         <v>187</v>
       </c>
       <c r="P33">
-        <v>25000</v>
+        <v>50</v>
       </c>
       <c r="Q33" t="s">
         <v>188</v>
@@ -3486,7 +3519,7 @@
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>236</v>
       </c>
       <c r="D34" t="s">
         <v>63</v>
@@ -3509,8 +3542,8 @@
       <c r="J34" t="s">
         <v>62</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>38</v>
+      <c r="K34" s="3" t="s">
+        <v>282</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>63</v>
@@ -3519,13 +3552,13 @@
         <v>64</v>
       </c>
       <c r="N34" t="s">
-        <v>167</v>
+        <v>245</v>
       </c>
       <c r="O34" t="s">
         <v>187</v>
       </c>
       <c r="P34">
-        <v>50000</v>
+        <v>500</v>
       </c>
       <c r="Q34" t="s">
         <v>188</v>
@@ -3539,7 +3572,7 @@
         <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D35" t="s">
         <v>63</v>
@@ -3563,7 +3596,7 @@
         <v>62</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>63</v>
@@ -3572,13 +3605,13 @@
         <v>64</v>
       </c>
       <c r="N35" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O35" t="s">
         <v>187</v>
       </c>
       <c r="P35">
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="Q35" t="s">
         <v>188</v>
@@ -3592,7 +3625,7 @@
         <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>242</v>
       </c>
       <c r="D36" t="s">
         <v>63</v>
@@ -3615,8 +3648,8 @@
       <c r="J36" t="s">
         <v>62</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>44</v>
+      <c r="K36" s="4" t="s">
+        <v>287</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>63</v>
@@ -3625,13 +3658,13 @@
         <v>64</v>
       </c>
       <c r="N36" t="s">
-        <v>172</v>
+        <v>255</v>
       </c>
       <c r="O36" t="s">
         <v>187</v>
       </c>
       <c r="P36">
-        <v>250000</v>
+        <v>2500</v>
       </c>
       <c r="Q36" t="s">
         <v>188</v>
@@ -3645,7 +3678,7 @@
         <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
         <v>63</v>
@@ -3669,7 +3702,7 @@
         <v>62</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>63</v>
@@ -3678,13 +3711,13 @@
         <v>64</v>
       </c>
       <c r="N37" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="O37" t="s">
         <v>187</v>
       </c>
       <c r="P37">
-        <v>500000</v>
+        <v>5000</v>
       </c>
       <c r="Q37" t="s">
         <v>188</v>
@@ -3698,7 +3731,7 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>264</v>
       </c>
       <c r="D38" t="s">
         <v>63</v>
@@ -3721,8 +3754,8 @@
       <c r="J38" t="s">
         <v>62</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>35</v>
+      <c r="K38" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>63</v>
@@ -3731,13 +3764,13 @@
         <v>64</v>
       </c>
       <c r="N38" t="s">
-        <v>161</v>
+        <v>271</v>
       </c>
       <c r="O38" t="s">
         <v>187</v>
       </c>
       <c r="P38">
-        <v>1000000</v>
+        <v>7500</v>
       </c>
       <c r="Q38" t="s">
         <v>188</v>
@@ -3751,7 +3784,7 @@
         <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
         <v>63</v>
@@ -3775,7 +3808,7 @@
         <v>62</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>63</v>
@@ -3784,13 +3817,13 @@
         <v>64</v>
       </c>
       <c r="N39" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="O39" t="s">
         <v>187</v>
       </c>
       <c r="P39">
-        <v>2500000</v>
+        <v>10000</v>
       </c>
       <c r="Q39" t="s">
         <v>188</v>
@@ -3804,7 +3837,7 @@
         <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D40" t="s">
         <v>63</v>
@@ -3816,7 +3849,7 @@
         <v>62</v>
       </c>
       <c r="G40" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="H40" t="s">
         <v>63</v>
@@ -3827,8 +3860,8 @@
       <c r="J40" t="s">
         <v>62</v>
       </c>
-      <c r="K40" s="4" t="s">
-        <v>295</v>
+      <c r="K40" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>63</v>
@@ -3837,13 +3870,13 @@
         <v>64</v>
       </c>
       <c r="N40" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="O40" t="s">
         <v>187</v>
       </c>
       <c r="P40">
-        <v>500</v>
+        <v>25000</v>
       </c>
       <c r="Q40" t="s">
         <v>188</v>
@@ -3857,7 +3890,7 @@
         <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>238</v>
+        <v>76</v>
       </c>
       <c r="D41" t="s">
         <v>63</v>
@@ -3869,7 +3902,7 @@
         <v>62</v>
       </c>
       <c r="G41" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="H41" t="s">
         <v>63</v>
@@ -3880,8 +3913,8 @@
       <c r="J41" t="s">
         <v>62</v>
       </c>
-      <c r="K41" s="4" t="s">
-        <v>283</v>
+      <c r="K41" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>63</v>
@@ -3890,13 +3923,13 @@
         <v>64</v>
       </c>
       <c r="N41" t="s">
-        <v>246</v>
+        <v>167</v>
       </c>
       <c r="O41" t="s">
         <v>187</v>
       </c>
       <c r="P41">
-        <v>1000</v>
+        <v>50000</v>
       </c>
       <c r="Q41" t="s">
         <v>188</v>
@@ -3910,7 +3943,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>240</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
         <v>63</v>
@@ -3922,7 +3955,7 @@
         <v>62</v>
       </c>
       <c r="G42" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="H42" t="s">
         <v>63</v>
@@ -3933,8 +3966,8 @@
       <c r="J42" t="s">
         <v>62</v>
       </c>
-      <c r="K42" s="4" t="s">
-        <v>285</v>
+      <c r="K42" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>63</v>
@@ -3943,13 +3976,13 @@
         <v>64</v>
       </c>
       <c r="N42" t="s">
-        <v>248</v>
+        <v>146</v>
       </c>
       <c r="O42" t="s">
         <v>187</v>
       </c>
       <c r="P42">
-        <v>2500</v>
+        <v>100000</v>
       </c>
       <c r="Q42" t="s">
         <v>188</v>
@@ -3963,7 +3996,7 @@
         <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>261</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
         <v>63</v>
@@ -3975,7 +4008,7 @@
         <v>62</v>
       </c>
       <c r="G43" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="H43" t="s">
         <v>63</v>
@@ -3986,8 +4019,8 @@
       <c r="J43" t="s">
         <v>62</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>294</v>
+      <c r="K43" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>63</v>
@@ -3996,13 +4029,13 @@
         <v>64</v>
       </c>
       <c r="N43" t="s">
-        <v>266</v>
+        <v>172</v>
       </c>
       <c r="O43" t="s">
         <v>187</v>
       </c>
       <c r="P43">
-        <v>5000</v>
+        <v>250000</v>
       </c>
       <c r="Q43" t="s">
         <v>188</v>
@@ -4016,7 +4049,7 @@
         <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>269</v>
+        <v>79</v>
       </c>
       <c r="D44" t="s">
         <v>63</v>
@@ -4028,7 +4061,7 @@
         <v>62</v>
       </c>
       <c r="G44" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="H44" t="s">
         <v>63</v>
@@ -4039,8 +4072,8 @@
       <c r="J44" t="s">
         <v>62</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>298</v>
+      <c r="K44" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>63</v>
@@ -4049,13 +4082,13 @@
         <v>64</v>
       </c>
       <c r="N44" t="s">
-        <v>272</v>
+        <v>147</v>
       </c>
       <c r="O44" t="s">
         <v>187</v>
       </c>
       <c r="P44">
-        <v>7500</v>
+        <v>500000</v>
       </c>
       <c r="Q44" t="s">
         <v>188</v>
@@ -4069,7 +4102,7 @@
         <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>241</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -4081,7 +4114,7 @@
         <v>62</v>
       </c>
       <c r="G45" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="H45" t="s">
         <v>63</v>
@@ -4092,8 +4125,8 @@
       <c r="J45" t="s">
         <v>62</v>
       </c>
-      <c r="K45" s="4" t="s">
-        <v>286</v>
+      <c r="K45" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>63</v>
@@ -4102,13 +4135,13 @@
         <v>64</v>
       </c>
       <c r="N45" t="s">
-        <v>249</v>
+        <v>161</v>
       </c>
       <c r="O45" t="s">
         <v>187</v>
       </c>
       <c r="P45">
-        <v>10000</v>
+        <v>1000000</v>
       </c>
       <c r="Q45" t="s">
         <v>188</v>
@@ -4122,7 +4155,7 @@
         <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>250</v>
+        <v>81</v>
       </c>
       <c r="D46" t="s">
         <v>63</v>
@@ -4134,7 +4167,7 @@
         <v>62</v>
       </c>
       <c r="G46" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="H46" t="s">
         <v>63</v>
@@ -4145,8 +4178,8 @@
       <c r="J46" t="s">
         <v>62</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>289</v>
+      <c r="K46" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>63</v>
@@ -4155,13 +4188,13 @@
         <v>64</v>
       </c>
       <c r="N46" t="s">
-        <v>257</v>
+        <v>162</v>
       </c>
       <c r="O46" t="s">
         <v>187</v>
       </c>
       <c r="P46">
-        <v>25000</v>
+        <v>2500000</v>
       </c>
       <c r="Q46" t="s">
         <v>188</v>
@@ -4175,7 +4208,7 @@
         <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="D47" t="s">
         <v>63</v>
@@ -4198,8 +4231,8 @@
       <c r="J47" t="s">
         <v>62</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>293</v>
+      <c r="K47" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>63</v>
@@ -4208,13 +4241,13 @@
         <v>64</v>
       </c>
       <c r="N47" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="O47" t="s">
         <v>187</v>
       </c>
       <c r="P47">
-        <v>50000</v>
+        <v>500</v>
       </c>
       <c r="Q47" t="s">
         <v>188</v>
@@ -4228,7 +4261,7 @@
         <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>238</v>
       </c>
       <c r="D48" t="s">
         <v>63</v>
@@ -4240,7 +4273,7 @@
         <v>62</v>
       </c>
       <c r="G48" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H48" t="s">
         <v>63</v>
@@ -4251,8 +4284,8 @@
       <c r="J48" t="s">
         <v>62</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>2</v>
+      <c r="K48" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>63</v>
@@ -4261,13 +4294,13 @@
         <v>64</v>
       </c>
       <c r="N48" t="s">
-        <v>134</v>
+        <v>246</v>
       </c>
       <c r="O48" t="s">
         <v>187</v>
       </c>
       <c r="P48">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="Q48" t="s">
         <v>188</v>
@@ -4281,7 +4314,7 @@
         <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>240</v>
       </c>
       <c r="D49" t="s">
         <v>63</v>
@@ -4293,7 +4326,7 @@
         <v>62</v>
       </c>
       <c r="G49" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H49" t="s">
         <v>63</v>
@@ -4304,8 +4337,8 @@
       <c r="J49" t="s">
         <v>62</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>6</v>
+      <c r="K49" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>63</v>
@@ -4314,13 +4347,13 @@
         <v>64</v>
       </c>
       <c r="N49" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="O49" t="s">
         <v>187</v>
       </c>
       <c r="P49">
-        <v>5</v>
+        <v>2500</v>
       </c>
       <c r="Q49" t="s">
         <v>188</v>
@@ -4334,7 +4367,7 @@
         <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>261</v>
       </c>
       <c r="D50" t="s">
         <v>63</v>
@@ -4346,7 +4379,7 @@
         <v>62</v>
       </c>
       <c r="G50" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H50" t="s">
         <v>63</v>
@@ -4357,8 +4390,8 @@
       <c r="J50" t="s">
         <v>62</v>
       </c>
-      <c r="K50" s="1" t="s">
-        <v>3</v>
+      <c r="K50" s="4" t="s">
+        <v>294</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>63</v>
@@ -4367,13 +4400,13 @@
         <v>64</v>
       </c>
       <c r="N50" t="s">
-        <v>135</v>
+        <v>266</v>
       </c>
       <c r="O50" t="s">
         <v>187</v>
       </c>
       <c r="P50">
-        <v>10</v>
+        <v>5000</v>
       </c>
       <c r="Q50" t="s">
         <v>188</v>
@@ -4387,7 +4420,7 @@
         <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>85</v>
+        <v>269</v>
       </c>
       <c r="D51" t="s">
         <v>63</v>
@@ -4399,7 +4432,7 @@
         <v>62</v>
       </c>
       <c r="G51" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H51" t="s">
         <v>63</v>
@@ -4410,8 +4443,8 @@
       <c r="J51" t="s">
         <v>62</v>
       </c>
-      <c r="K51" s="1" t="s">
-        <v>4</v>
+      <c r="K51" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>63</v>
@@ -4420,13 +4453,13 @@
         <v>64</v>
       </c>
       <c r="N51" t="s">
-        <v>136</v>
+        <v>272</v>
       </c>
       <c r="O51" t="s">
         <v>187</v>
       </c>
       <c r="P51">
-        <v>20</v>
+        <v>7500</v>
       </c>
       <c r="Q51" t="s">
         <v>188</v>
@@ -4440,7 +4473,7 @@
         <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>86</v>
+        <v>241</v>
       </c>
       <c r="D52" t="s">
         <v>63</v>
@@ -4452,7 +4485,7 @@
         <v>62</v>
       </c>
       <c r="G52" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H52" t="s">
         <v>63</v>
@@ -4463,8 +4496,8 @@
       <c r="J52" t="s">
         <v>62</v>
       </c>
-      <c r="K52" s="1" t="s">
-        <v>5</v>
+      <c r="K52" s="4" t="s">
+        <v>286</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>63</v>
@@ -4473,13 +4506,13 @@
         <v>64</v>
       </c>
       <c r="N52" t="s">
-        <v>137</v>
+        <v>249</v>
       </c>
       <c r="O52" t="s">
         <v>187</v>
       </c>
       <c r="P52">
-        <v>25</v>
+        <v>10000</v>
       </c>
       <c r="Q52" t="s">
         <v>188</v>
@@ -4493,7 +4526,7 @@
         <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>250</v>
       </c>
       <c r="D53" t="s">
         <v>63</v>
@@ -4505,7 +4538,7 @@
         <v>62</v>
       </c>
       <c r="G53" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H53" t="s">
         <v>63</v>
@@ -4516,8 +4549,8 @@
       <c r="J53" t="s">
         <v>62</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>206</v>
+      <c r="K53" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>63</v>
@@ -4526,13 +4559,13 @@
         <v>64</v>
       </c>
       <c r="N53" t="s">
-        <v>207</v>
+        <v>257</v>
       </c>
       <c r="O53" t="s">
         <v>187</v>
       </c>
       <c r="P53">
-        <v>100</v>
+        <v>25000</v>
       </c>
       <c r="Q53" t="s">
         <v>188</v>
@@ -4546,7 +4579,7 @@
         <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>254</v>
       </c>
       <c r="D54" t="s">
         <v>63</v>
@@ -4558,7 +4591,7 @@
         <v>62</v>
       </c>
       <c r="G54" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H54" t="s">
         <v>63</v>
@@ -4569,8 +4602,8 @@
       <c r="J54" t="s">
         <v>62</v>
       </c>
-      <c r="K54" s="1" t="s">
-        <v>209</v>
+      <c r="K54" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>63</v>
@@ -4579,13 +4612,13 @@
         <v>64</v>
       </c>
       <c r="N54" t="s">
-        <v>208</v>
+        <v>265</v>
       </c>
       <c r="O54" t="s">
         <v>187</v>
       </c>
       <c r="P54">
-        <v>500</v>
+        <v>50000</v>
       </c>
       <c r="Q54" t="s">
         <v>188</v>
@@ -4599,7 +4632,7 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D55" t="s">
         <v>63</v>
@@ -4623,7 +4656,7 @@
         <v>62</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>210</v>
+        <v>2</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>63</v>
@@ -4632,13 +4665,13 @@
         <v>64</v>
       </c>
       <c r="N55" t="s">
-        <v>211</v>
+        <v>134</v>
       </c>
       <c r="O55" t="s">
         <v>187</v>
       </c>
       <c r="P55">
-        <v>1000000</v>
+        <v>1</v>
       </c>
       <c r="Q55" t="s">
         <v>188</v>
@@ -4652,7 +4685,7 @@
         <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D56" t="s">
         <v>63</v>
@@ -4664,7 +4697,7 @@
         <v>62</v>
       </c>
       <c r="G56" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H56" t="s">
         <v>63</v>
@@ -4676,7 +4709,7 @@
         <v>62</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>63</v>
@@ -4685,13 +4718,13 @@
         <v>64</v>
       </c>
       <c r="N56" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="O56" t="s">
         <v>187</v>
       </c>
       <c r="P56">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q56" t="s">
         <v>188</v>
@@ -4705,7 +4738,7 @@
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D57" t="s">
         <v>63</v>
@@ -4717,7 +4750,7 @@
         <v>62</v>
       </c>
       <c r="G57" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H57" t="s">
         <v>63</v>
@@ -4729,7 +4762,7 @@
         <v>62</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>63</v>
@@ -4738,13 +4771,13 @@
         <v>64</v>
       </c>
       <c r="N57" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="O57" t="s">
         <v>187</v>
       </c>
       <c r="P57">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="Q57" t="s">
         <v>188</v>
@@ -4758,7 +4791,7 @@
         <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D58" t="s">
         <v>63</v>
@@ -4770,7 +4803,7 @@
         <v>62</v>
       </c>
       <c r="G58" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H58" t="s">
         <v>63</v>
@@ -4782,7 +4815,7 @@
         <v>62</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>63</v>
@@ -4791,13 +4824,13 @@
         <v>64</v>
       </c>
       <c r="N58" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
       <c r="O58" t="s">
         <v>187</v>
       </c>
       <c r="P58">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="Q58" t="s">
         <v>188</v>
@@ -4811,7 +4844,7 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D59" t="s">
         <v>63</v>
@@ -4823,7 +4856,7 @@
         <v>62</v>
       </c>
       <c r="G59" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H59" t="s">
         <v>63</v>
@@ -4835,7 +4868,7 @@
         <v>62</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>63</v>
@@ -4844,13 +4877,13 @@
         <v>64</v>
       </c>
       <c r="N59" t="s">
-        <v>180</v>
+        <v>137</v>
       </c>
       <c r="O59" t="s">
         <v>187</v>
       </c>
       <c r="P59">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="Q59" t="s">
         <v>188</v>
@@ -4864,7 +4897,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D60" t="s">
         <v>63</v>
@@ -4876,7 +4909,7 @@
         <v>62</v>
       </c>
       <c r="G60" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H60" t="s">
         <v>63</v>
@@ -4888,7 +4921,7 @@
         <v>62</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>56</v>
+        <v>206</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>63</v>
@@ -4897,13 +4930,13 @@
         <v>64</v>
       </c>
       <c r="N60" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="O60" t="s">
         <v>187</v>
       </c>
       <c r="P60">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="Q60" t="s">
         <v>188</v>
@@ -4917,7 +4950,7 @@
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -4929,7 +4962,7 @@
         <v>62</v>
       </c>
       <c r="G61" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H61" t="s">
         <v>63</v>
@@ -4941,7 +4974,7 @@
         <v>62</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>63</v>
@@ -4950,7 +4983,7 @@
         <v>64</v>
       </c>
       <c r="N61" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="O61" t="s">
         <v>187</v>
@@ -4970,7 +5003,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D62" t="s">
         <v>63</v>
@@ -4982,7 +5015,7 @@
         <v>62</v>
       </c>
       <c r="G62" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H62" t="s">
         <v>63</v>
@@ -4994,7 +5027,7 @@
         <v>62</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>46</v>
+        <v>210</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>63</v>
@@ -5003,13 +5036,13 @@
         <v>64</v>
       </c>
       <c r="N62" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="O62" t="s">
         <v>187</v>
       </c>
       <c r="P62">
-        <v>500</v>
+        <v>1000000</v>
       </c>
       <c r="Q62" t="s">
         <v>188</v>
@@ -5023,7 +5056,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D63" t="s">
         <v>63</v>
@@ -5047,7 +5080,7 @@
         <v>62</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>63</v>
@@ -5056,13 +5089,13 @@
         <v>64</v>
       </c>
       <c r="N63" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="O63" t="s">
         <v>187</v>
       </c>
       <c r="P63">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="Q63" t="s">
         <v>188</v>
@@ -5076,7 +5109,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D64" t="s">
         <v>63</v>
@@ -5100,7 +5133,7 @@
         <v>62</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>63</v>
@@ -5109,13 +5142,13 @@
         <v>64</v>
       </c>
       <c r="N64" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="O64" t="s">
         <v>187</v>
       </c>
       <c r="P64">
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="Q64" t="s">
         <v>188</v>
@@ -5129,7 +5162,7 @@
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D65" t="s">
         <v>63</v>
@@ -5153,7 +5186,7 @@
         <v>62</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>63</v>
@@ -5162,13 +5195,13 @@
         <v>64</v>
       </c>
       <c r="N65" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="O65" t="s">
         <v>187</v>
       </c>
       <c r="P65">
-        <v>2500</v>
+        <v>150</v>
       </c>
       <c r="Q65" t="s">
         <v>188</v>
@@ -5182,7 +5215,7 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D66" t="s">
         <v>63</v>
@@ -5206,7 +5239,7 @@
         <v>62</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>63</v>
@@ -5215,13 +5248,13 @@
         <v>64</v>
       </c>
       <c r="N66" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="O66" t="s">
         <v>187</v>
       </c>
       <c r="P66">
-        <v>2500</v>
+        <v>250</v>
       </c>
       <c r="Q66" t="s">
         <v>188</v>
@@ -5235,7 +5268,7 @@
         <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D67" t="s">
         <v>63</v>
@@ -5259,7 +5292,7 @@
         <v>62</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>63</v>
@@ -5268,13 +5301,13 @@
         <v>64</v>
       </c>
       <c r="N67" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O67" t="s">
         <v>187</v>
       </c>
       <c r="P67">
-        <v>5000</v>
+        <v>250</v>
       </c>
       <c r="Q67" t="s">
         <v>188</v>
@@ -5288,7 +5321,7 @@
         <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D68" t="s">
         <v>63</v>
@@ -5312,7 +5345,7 @@
         <v>62</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>63</v>
@@ -5321,13 +5354,13 @@
         <v>64</v>
       </c>
       <c r="N68" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="O68" t="s">
         <v>187</v>
       </c>
       <c r="P68">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="Q68" t="s">
         <v>188</v>
@@ -5341,7 +5374,7 @@
         <v>62</v>
       </c>
       <c r="C69" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D69" t="s">
         <v>63</v>
@@ -5365,7 +5398,7 @@
         <v>62</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>63</v>
@@ -5374,13 +5407,13 @@
         <v>64</v>
       </c>
       <c r="N69" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="O69" t="s">
         <v>187</v>
       </c>
       <c r="P69">
-        <v>50000</v>
+        <v>500</v>
       </c>
       <c r="Q69" t="s">
         <v>188</v>
@@ -5394,7 +5427,7 @@
         <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D70" t="s">
         <v>63</v>
@@ -5418,7 +5451,7 @@
         <v>62</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>63</v>
@@ -5427,13 +5460,13 @@
         <v>64</v>
       </c>
       <c r="N70" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="O70" t="s">
         <v>187</v>
       </c>
       <c r="P70">
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="Q70" t="s">
         <v>188</v>
@@ -5447,7 +5480,7 @@
         <v>62</v>
       </c>
       <c r="C71" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D71" t="s">
         <v>63</v>
@@ -5459,7 +5492,7 @@
         <v>62</v>
       </c>
       <c r="G71" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H71" t="s">
         <v>63</v>
@@ -5471,7 +5504,7 @@
         <v>62</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>63</v>
@@ -5480,13 +5513,13 @@
         <v>64</v>
       </c>
       <c r="N71" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="O71" t="s">
         <v>187</v>
       </c>
       <c r="P71">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="Q71" t="s">
         <v>188</v>
@@ -5500,7 +5533,7 @@
         <v>62</v>
       </c>
       <c r="C72" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D72" t="s">
         <v>63</v>
@@ -5512,7 +5545,7 @@
         <v>62</v>
       </c>
       <c r="G72" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H72" t="s">
         <v>63</v>
@@ -5524,7 +5557,7 @@
         <v>62</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>63</v>
@@ -5533,13 +5566,13 @@
         <v>64</v>
       </c>
       <c r="N72" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="O72" t="s">
         <v>187</v>
       </c>
       <c r="P72">
-        <v>100</v>
+        <v>2500</v>
       </c>
       <c r="Q72" t="s">
         <v>188</v>
@@ -5553,7 +5586,7 @@
         <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D73" t="s">
         <v>63</v>
@@ -5565,7 +5598,7 @@
         <v>62</v>
       </c>
       <c r="G73" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H73" t="s">
         <v>63</v>
@@ -5577,7 +5610,7 @@
         <v>62</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>63</v>
@@ -5586,13 +5619,13 @@
         <v>64</v>
       </c>
       <c r="N73" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="O73" t="s">
         <v>187</v>
       </c>
       <c r="P73">
-        <v>200</v>
+        <v>2500</v>
       </c>
       <c r="Q73" t="s">
         <v>188</v>
@@ -5606,7 +5639,7 @@
         <v>62</v>
       </c>
       <c r="C74" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D74" t="s">
         <v>63</v>
@@ -5618,7 +5651,7 @@
         <v>62</v>
       </c>
       <c r="G74" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H74" t="s">
         <v>63</v>
@@ -5630,7 +5663,7 @@
         <v>62</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>63</v>
@@ -5639,13 +5672,13 @@
         <v>64</v>
       </c>
       <c r="N74" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="O74" t="s">
         <v>187</v>
       </c>
       <c r="P74">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="Q74" t="s">
         <v>188</v>
@@ -5659,7 +5692,7 @@
         <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D75" t="s">
         <v>63</v>
@@ -5671,7 +5704,7 @@
         <v>62</v>
       </c>
       <c r="G75" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H75" t="s">
         <v>63</v>
@@ -5683,7 +5716,7 @@
         <v>62</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>63</v>
@@ -5692,13 +5725,13 @@
         <v>64</v>
       </c>
       <c r="N75" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="O75" t="s">
         <v>187</v>
       </c>
       <c r="P75">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="Q75" t="s">
         <v>188</v>
@@ -5712,7 +5745,7 @@
         <v>62</v>
       </c>
       <c r="C76" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D76" t="s">
         <v>63</v>
@@ -5724,7 +5757,7 @@
         <v>62</v>
       </c>
       <c r="G76" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H76" t="s">
         <v>63</v>
@@ -5736,7 +5769,7 @@
         <v>62</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>63</v>
@@ -5745,13 +5778,13 @@
         <v>64</v>
       </c>
       <c r="N76" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="O76" t="s">
         <v>187</v>
       </c>
       <c r="P76">
-        <v>2500</v>
+        <v>50000</v>
       </c>
       <c r="Q76" t="s">
         <v>188</v>
@@ -5765,7 +5798,7 @@
         <v>62</v>
       </c>
       <c r="C77" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D77" t="s">
         <v>63</v>
@@ -5777,7 +5810,7 @@
         <v>62</v>
       </c>
       <c r="G77" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H77" t="s">
         <v>63</v>
@@ -5789,7 +5822,7 @@
         <v>62</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>63</v>
@@ -5798,13 +5831,13 @@
         <v>64</v>
       </c>
       <c r="N77" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="O77" t="s">
         <v>187</v>
       </c>
       <c r="P77">
-        <v>5000</v>
+        <v>100000</v>
       </c>
       <c r="Q77" t="s">
         <v>188</v>
@@ -5818,7 +5851,7 @@
         <v>62</v>
       </c>
       <c r="C78" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D78" t="s">
         <v>63</v>
@@ -5842,7 +5875,7 @@
         <v>62</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>63</v>
@@ -5851,13 +5884,13 @@
         <v>64</v>
       </c>
       <c r="N78" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="O78" t="s">
         <v>187</v>
       </c>
       <c r="P78">
-        <v>10000</v>
+        <v>50</v>
       </c>
       <c r="Q78" t="s">
         <v>188</v>
@@ -5871,7 +5904,7 @@
         <v>62</v>
       </c>
       <c r="C79" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D79" t="s">
         <v>63</v>
@@ -5883,7 +5916,7 @@
         <v>62</v>
       </c>
       <c r="G79" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H79" t="s">
         <v>63</v>
@@ -5895,7 +5928,7 @@
         <v>62</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>63</v>
@@ -5904,13 +5937,13 @@
         <v>64</v>
       </c>
       <c r="N79" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="O79" t="s">
         <v>187</v>
       </c>
       <c r="P79">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="Q79" t="s">
         <v>188</v>
@@ -5924,7 +5957,7 @@
         <v>62</v>
       </c>
       <c r="C80" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D80" t="s">
         <v>63</v>
@@ -5936,7 +5969,7 @@
         <v>62</v>
       </c>
       <c r="G80" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H80" t="s">
         <v>63</v>
@@ -5948,7 +5981,7 @@
         <v>62</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>63</v>
@@ -5957,13 +5990,13 @@
         <v>64</v>
       </c>
       <c r="N80" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="O80" t="s">
         <v>187</v>
       </c>
       <c r="P80">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="Q80" t="s">
         <v>188</v>
@@ -5977,7 +6010,7 @@
         <v>62</v>
       </c>
       <c r="C81" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D81" t="s">
         <v>63</v>
@@ -5989,7 +6022,7 @@
         <v>62</v>
       </c>
       <c r="G81" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H81" t="s">
         <v>63</v>
@@ -6001,7 +6034,7 @@
         <v>62</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L81" s="1" t="s">
         <v>63</v>
@@ -6010,13 +6043,13 @@
         <v>64</v>
       </c>
       <c r="N81" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="O81" t="s">
         <v>187</v>
       </c>
       <c r="P81">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q81" t="s">
         <v>188</v>
@@ -6030,7 +6063,7 @@
         <v>62</v>
       </c>
       <c r="C82" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D82" t="s">
         <v>63</v>
@@ -6042,7 +6075,7 @@
         <v>62</v>
       </c>
       <c r="G82" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H82" t="s">
         <v>63</v>
@@ -6054,7 +6087,7 @@
         <v>62</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>63</v>
@@ -6063,13 +6096,13 @@
         <v>64</v>
       </c>
       <c r="N82" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="O82" t="s">
         <v>187</v>
       </c>
       <c r="P82">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q82" t="s">
         <v>188</v>
@@ -6083,7 +6116,7 @@
         <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D83" t="s">
         <v>63</v>
@@ -6095,7 +6128,7 @@
         <v>62</v>
       </c>
       <c r="G83" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H83" t="s">
         <v>63</v>
@@ -6107,7 +6140,7 @@
         <v>62</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>63</v>
@@ -6116,13 +6149,13 @@
         <v>64</v>
       </c>
       <c r="N83" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O83" t="s">
         <v>187</v>
       </c>
       <c r="P83">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q83" t="s">
         <v>188</v>
@@ -6136,7 +6169,7 @@
         <v>62</v>
       </c>
       <c r="C84" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="D84" t="s">
         <v>63</v>
@@ -6148,7 +6181,7 @@
         <v>62</v>
       </c>
       <c r="G84" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H84" t="s">
         <v>63</v>
@@ -6159,8 +6192,8 @@
       <c r="J84" t="s">
         <v>62</v>
       </c>
-      <c r="K84" s="3" t="s">
-        <v>296</v>
+      <c r="K84" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>63</v>
@@ -6169,13 +6202,13 @@
         <v>64</v>
       </c>
       <c r="N84" t="s">
-        <v>268</v>
+        <v>155</v>
       </c>
       <c r="O84" t="s">
         <v>187</v>
       </c>
       <c r="P84">
-        <v>75000</v>
+        <v>5000</v>
       </c>
       <c r="Q84" t="s">
         <v>188</v>
@@ -6189,7 +6222,7 @@
         <v>62</v>
       </c>
       <c r="C85" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D85" t="s">
         <v>63</v>
@@ -6201,7 +6234,7 @@
         <v>62</v>
       </c>
       <c r="G85" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H85" t="s">
         <v>63</v>
@@ -6213,7 +6246,7 @@
         <v>62</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>189</v>
+        <v>32</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>63</v>
@@ -6222,13 +6255,13 @@
         <v>64</v>
       </c>
       <c r="N85" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="O85" t="s">
         <v>187</v>
       </c>
       <c r="P85">
-        <v>50</v>
+        <v>10000</v>
       </c>
       <c r="Q85" t="s">
         <v>188</v>
@@ -6242,7 +6275,7 @@
         <v>62</v>
       </c>
       <c r="C86" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D86" t="s">
         <v>63</v>
@@ -6254,7 +6287,7 @@
         <v>62</v>
       </c>
       <c r="G86" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H86" t="s">
         <v>63</v>
@@ -6266,7 +6299,7 @@
         <v>62</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>63</v>
@@ -6275,13 +6308,13 @@
         <v>64</v>
       </c>
       <c r="N86" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="O86" t="s">
         <v>187</v>
       </c>
       <c r="P86">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="Q86" t="s">
         <v>188</v>
@@ -6295,7 +6328,7 @@
         <v>62</v>
       </c>
       <c r="C87" t="s">
-        <v>223</v>
+        <v>116</v>
       </c>
       <c r="D87" t="s">
         <v>63</v>
@@ -6307,7 +6340,7 @@
         <v>62</v>
       </c>
       <c r="G87" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H87" t="s">
         <v>63</v>
@@ -6318,8 +6351,8 @@
       <c r="J87" t="s">
         <v>62</v>
       </c>
-      <c r="K87" s="3" t="s">
-        <v>275</v>
+      <c r="K87" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="L87" s="1" t="s">
         <v>63</v>
@@ -6328,13 +6361,13 @@
         <v>64</v>
       </c>
       <c r="N87" t="s">
-        <v>229</v>
+        <v>159</v>
       </c>
       <c r="O87" t="s">
         <v>187</v>
       </c>
       <c r="P87">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="Q87" t="s">
         <v>188</v>
@@ -6348,7 +6381,7 @@
         <v>62</v>
       </c>
       <c r="C88" t="s">
-        <v>226</v>
+        <v>117</v>
       </c>
       <c r="D88" t="s">
         <v>63</v>
@@ -6360,7 +6393,7 @@
         <v>62</v>
       </c>
       <c r="G88" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H88" t="s">
         <v>63</v>
@@ -6372,7 +6405,7 @@
         <v>62</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>278</v>
+        <v>22</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>63</v>
@@ -6381,7 +6414,7 @@
         <v>64</v>
       </c>
       <c r="N88" t="s">
-        <v>232</v>
+        <v>159</v>
       </c>
       <c r="O88" t="s">
         <v>187</v>
@@ -6401,7 +6434,7 @@
         <v>62</v>
       </c>
       <c r="C89" t="s">
-        <v>228</v>
+        <v>113</v>
       </c>
       <c r="D89" t="s">
         <v>63</v>
@@ -6413,7 +6446,7 @@
         <v>62</v>
       </c>
       <c r="G89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H89" t="s">
         <v>63</v>
@@ -6425,7 +6458,7 @@
         <v>62</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>280</v>
+        <v>7</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>63</v>
@@ -6434,13 +6467,13 @@
         <v>64</v>
       </c>
       <c r="N89" t="s">
-        <v>234</v>
+        <v>144</v>
       </c>
       <c r="O89" t="s">
         <v>187</v>
       </c>
       <c r="P89">
-        <v>10000</v>
+        <v>2500</v>
       </c>
       <c r="Q89" t="s">
         <v>188</v>
@@ -6454,7 +6487,7 @@
         <v>62</v>
       </c>
       <c r="C90" t="s">
-        <v>227</v>
+        <v>114</v>
       </c>
       <c r="D90" t="s">
         <v>63</v>
@@ -6466,7 +6499,7 @@
         <v>62</v>
       </c>
       <c r="G90" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H90" t="s">
         <v>63</v>
@@ -6478,7 +6511,7 @@
         <v>62</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>279</v>
+        <v>20</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>63</v>
@@ -6487,13 +6520,13 @@
         <v>64</v>
       </c>
       <c r="N90" t="s">
-        <v>233</v>
+        <v>158</v>
       </c>
       <c r="O90" t="s">
         <v>187</v>
       </c>
       <c r="P90">
-        <v>25000</v>
+        <v>5000</v>
       </c>
       <c r="Q90" t="s">
         <v>188</v>
@@ -6507,7 +6540,7 @@
         <v>62</v>
       </c>
       <c r="C91" t="s">
-        <v>120</v>
+        <v>263</v>
       </c>
       <c r="D91" t="s">
         <v>63</v>
@@ -6519,7 +6552,7 @@
         <v>62</v>
       </c>
       <c r="G91" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H91" t="s">
         <v>63</v>
@@ -6530,8 +6563,8 @@
       <c r="J91" t="s">
         <v>62</v>
       </c>
-      <c r="K91" s="1" t="s">
-        <v>37</v>
+      <c r="K91" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>63</v>
@@ -6540,13 +6573,13 @@
         <v>64</v>
       </c>
       <c r="N91" t="s">
-        <v>165</v>
+        <v>268</v>
       </c>
       <c r="O91" t="s">
         <v>187</v>
       </c>
       <c r="P91">
-        <v>50000</v>
+        <v>75000</v>
       </c>
       <c r="Q91" t="s">
         <v>188</v>
@@ -6560,7 +6593,7 @@
         <v>62</v>
       </c>
       <c r="C92" t="s">
-        <v>224</v>
+        <v>118</v>
       </c>
       <c r="D92" t="s">
         <v>63</v>
@@ -6583,8 +6616,8 @@
       <c r="J92" t="s">
         <v>62</v>
       </c>
-      <c r="K92" s="3" t="s">
-        <v>276</v>
+      <c r="K92" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>63</v>
@@ -6593,13 +6626,13 @@
         <v>64</v>
       </c>
       <c r="N92" t="s">
-        <v>230</v>
+        <v>131</v>
       </c>
       <c r="O92" t="s">
         <v>187</v>
       </c>
       <c r="P92">
-        <v>75000</v>
+        <v>50</v>
       </c>
       <c r="Q92" t="s">
         <v>188</v>
@@ -6613,7 +6646,7 @@
         <v>62</v>
       </c>
       <c r="C93" t="s">
-        <v>225</v>
+        <v>119</v>
       </c>
       <c r="D93" t="s">
         <v>63</v>
@@ -6636,8 +6669,8 @@
       <c r="J93" t="s">
         <v>62</v>
       </c>
-      <c r="K93" s="3" t="s">
-        <v>277</v>
+      <c r="K93" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>63</v>
@@ -6646,13 +6679,13 @@
         <v>64</v>
       </c>
       <c r="N93" t="s">
-        <v>231</v>
+        <v>130</v>
       </c>
       <c r="O93" t="s">
         <v>187</v>
       </c>
       <c r="P93">
-        <v>100000</v>
+        <v>200</v>
       </c>
       <c r="Q93" t="s">
         <v>188</v>
@@ -6666,7 +6699,7 @@
         <v>62</v>
       </c>
       <c r="C94" t="s">
-        <v>121</v>
+        <v>223</v>
       </c>
       <c r="D94" t="s">
         <v>63</v>
@@ -6689,25 +6722,396 @@
       <c r="J94" t="s">
         <v>62</v>
       </c>
-      <c r="K94" s="1" t="s">
+      <c r="K94" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M94" t="s">
+        <v>64</v>
+      </c>
+      <c r="N94" t="s">
+        <v>229</v>
+      </c>
+      <c r="O94" t="s">
+        <v>187</v>
+      </c>
+      <c r="P94">
+        <v>500</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>61</v>
+      </c>
+      <c r="B95" t="s">
+        <v>62</v>
+      </c>
+      <c r="C95" t="s">
+        <v>226</v>
+      </c>
+      <c r="D95" t="s">
+        <v>63</v>
+      </c>
+      <c r="E95" t="s">
+        <v>122</v>
+      </c>
+      <c r="F95" t="s">
+        <v>62</v>
+      </c>
+      <c r="G95" t="s">
+        <v>125</v>
+      </c>
+      <c r="H95" t="s">
+        <v>63</v>
+      </c>
+      <c r="I95" t="s">
+        <v>60</v>
+      </c>
+      <c r="J95" t="s">
+        <v>62</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M95" t="s">
+        <v>64</v>
+      </c>
+      <c r="N95" t="s">
+        <v>232</v>
+      </c>
+      <c r="O95" t="s">
+        <v>187</v>
+      </c>
+      <c r="P95">
+        <v>1000</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>61</v>
+      </c>
+      <c r="B96" t="s">
+        <v>62</v>
+      </c>
+      <c r="C96" t="s">
+        <v>228</v>
+      </c>
+      <c r="D96" t="s">
+        <v>63</v>
+      </c>
+      <c r="E96" t="s">
+        <v>122</v>
+      </c>
+      <c r="F96" t="s">
+        <v>62</v>
+      </c>
+      <c r="G96" t="s">
+        <v>125</v>
+      </c>
+      <c r="H96" t="s">
+        <v>63</v>
+      </c>
+      <c r="I96" t="s">
+        <v>60</v>
+      </c>
+      <c r="J96" t="s">
+        <v>62</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M96" t="s">
+        <v>64</v>
+      </c>
+      <c r="N96" t="s">
+        <v>234</v>
+      </c>
+      <c r="O96" t="s">
+        <v>187</v>
+      </c>
+      <c r="P96">
+        <v>10000</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>61</v>
+      </c>
+      <c r="B97" t="s">
+        <v>62</v>
+      </c>
+      <c r="C97" t="s">
+        <v>227</v>
+      </c>
+      <c r="D97" t="s">
+        <v>63</v>
+      </c>
+      <c r="E97" t="s">
+        <v>122</v>
+      </c>
+      <c r="F97" t="s">
+        <v>62</v>
+      </c>
+      <c r="G97" t="s">
+        <v>125</v>
+      </c>
+      <c r="H97" t="s">
+        <v>63</v>
+      </c>
+      <c r="I97" t="s">
+        <v>60</v>
+      </c>
+      <c r="J97" t="s">
+        <v>62</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M97" t="s">
+        <v>64</v>
+      </c>
+      <c r="N97" t="s">
+        <v>233</v>
+      </c>
+      <c r="O97" t="s">
+        <v>187</v>
+      </c>
+      <c r="P97">
+        <v>25000</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" t="s">
+        <v>62</v>
+      </c>
+      <c r="C98" t="s">
+        <v>120</v>
+      </c>
+      <c r="D98" t="s">
+        <v>63</v>
+      </c>
+      <c r="E98" t="s">
+        <v>122</v>
+      </c>
+      <c r="F98" t="s">
+        <v>62</v>
+      </c>
+      <c r="G98" t="s">
+        <v>125</v>
+      </c>
+      <c r="H98" t="s">
+        <v>63</v>
+      </c>
+      <c r="I98" t="s">
+        <v>60</v>
+      </c>
+      <c r="J98" t="s">
+        <v>62</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M98" t="s">
+        <v>64</v>
+      </c>
+      <c r="N98" t="s">
+        <v>165</v>
+      </c>
+      <c r="O98" t="s">
+        <v>187</v>
+      </c>
+      <c r="P98">
+        <v>50000</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>61</v>
+      </c>
+      <c r="B99" t="s">
+        <v>62</v>
+      </c>
+      <c r="C99" t="s">
+        <v>224</v>
+      </c>
+      <c r="D99" t="s">
+        <v>63</v>
+      </c>
+      <c r="E99" t="s">
+        <v>122</v>
+      </c>
+      <c r="F99" t="s">
+        <v>62</v>
+      </c>
+      <c r="G99" t="s">
+        <v>125</v>
+      </c>
+      <c r="H99" t="s">
+        <v>63</v>
+      </c>
+      <c r="I99" t="s">
+        <v>60</v>
+      </c>
+      <c r="J99" t="s">
+        <v>62</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M99" t="s">
+        <v>64</v>
+      </c>
+      <c r="N99" t="s">
+        <v>230</v>
+      </c>
+      <c r="O99" t="s">
+        <v>187</v>
+      </c>
+      <c r="P99">
+        <v>75000</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>61</v>
+      </c>
+      <c r="B100" t="s">
+        <v>62</v>
+      </c>
+      <c r="C100" t="s">
+        <v>225</v>
+      </c>
+      <c r="D100" t="s">
+        <v>63</v>
+      </c>
+      <c r="E100" t="s">
+        <v>122</v>
+      </c>
+      <c r="F100" t="s">
+        <v>62</v>
+      </c>
+      <c r="G100" t="s">
+        <v>125</v>
+      </c>
+      <c r="H100" t="s">
+        <v>63</v>
+      </c>
+      <c r="I100" t="s">
+        <v>60</v>
+      </c>
+      <c r="J100" t="s">
+        <v>62</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M100" t="s">
+        <v>64</v>
+      </c>
+      <c r="N100" t="s">
+        <v>231</v>
+      </c>
+      <c r="O100" t="s">
+        <v>187</v>
+      </c>
+      <c r="P100">
+        <v>100000</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B101" t="s">
+        <v>62</v>
+      </c>
+      <c r="C101" t="s">
+        <v>121</v>
+      </c>
+      <c r="D101" t="s">
+        <v>63</v>
+      </c>
+      <c r="E101" t="s">
+        <v>122</v>
+      </c>
+      <c r="F101" t="s">
+        <v>62</v>
+      </c>
+      <c r="G101" t="s">
+        <v>125</v>
+      </c>
+      <c r="H101" t="s">
+        <v>63</v>
+      </c>
+      <c r="I101" t="s">
+        <v>60</v>
+      </c>
+      <c r="J101" t="s">
+        <v>62</v>
+      </c>
+      <c r="K101" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L94" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M94" t="s">
-        <v>64</v>
-      </c>
-      <c r="N94" t="s">
+      <c r="L101" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M101" t="s">
+        <v>64</v>
+      </c>
+      <c r="N101" t="s">
         <v>305</v>
       </c>
-      <c r="O94" t="s">
-        <v>187</v>
-      </c>
-      <c r="P94">
+      <c r="O101" t="s">
+        <v>187</v>
+      </c>
+      <c r="P101">
         <v>500000</v>
       </c>
-      <c r="Q94" t="s">
+      <c r="Q101" t="s">
         <v>188</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made value color codes adjustable
</commit_message>
<xml_diff>
--- a/HutListe.xlsx
+++ b/HutListe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="340">
   <si>
     <t>states/schaf.png</t>
   </si>
@@ -1330,6 +1330,45 @@
   </si>
   <si>
     <t>pics/sm_abo_11-10_frankenstein.gif</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_14-02_hockey.gif</t>
+  </si>
+  <si>
+    <t>c01</t>
+  </si>
+  <si>
+    <t>c02</t>
+  </si>
+  <si>
+    <t>c03</t>
+  </si>
+  <si>
+    <t>c04</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_14-03_costumes_bee.png</t>
+  </si>
+  <si>
+    <t>Die Königin unter den Insekten. Oder noch besser?</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_14-03_costumes_cow.png</t>
+  </si>
+  <si>
+    <t>Niemand ist so nützlich wie du!</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_14-03_costumes_fly.png</t>
+  </si>
+  <si>
+    <t>Kein Einhorn kann ohne dich existieren!</t>
+  </si>
+  <si>
+    <t>pics/sm_abo_14-07_hulahoop.gif</t>
+  </si>
+  <si>
+    <t>Damit zeigst du allen wie toll ein Kreis sein kann!</t>
   </si>
 </sst>
 </file>
@@ -1458,10 +1497,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:Q101" totalsRowShown="0">
-  <autoFilter ref="A1:Q101"/>
-  <sortState ref="A2:Q101">
-    <sortCondition ref="G1:G101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:Q106" totalsRowShown="0">
+  <autoFilter ref="A1:Q106"/>
+  <sortState ref="A2:Q106">
+    <sortCondition ref="G1:G106"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" name="A"/>
@@ -1741,7 +1780,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1749,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="S88" sqref="S88"/>
+    <sheetView tabSelected="1" topLeftCell="F79" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2547,7 +2586,9 @@
       <c r="J15" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="L15" s="1" t="s">
         <v>63</v>
       </c>
@@ -4632,7 +4673,7 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>331</v>
       </c>
       <c r="D55" t="s">
         <v>63</v>
@@ -4644,7 +4685,7 @@
         <v>62</v>
       </c>
       <c r="G55" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H55" t="s">
         <v>63</v>
@@ -4656,7 +4697,7 @@
         <v>62</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>2</v>
+        <v>338</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>63</v>
@@ -4665,13 +4706,13 @@
         <v>64</v>
       </c>
       <c r="N55" t="s">
-        <v>134</v>
+        <v>339</v>
       </c>
       <c r="O55" t="s">
         <v>187</v>
       </c>
       <c r="P55">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="Q55" t="s">
         <v>188</v>
@@ -4685,7 +4726,7 @@
         <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D56" t="s">
         <v>63</v>
@@ -4709,7 +4750,7 @@
         <v>62</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>63</v>
@@ -4718,13 +4759,13 @@
         <v>64</v>
       </c>
       <c r="N56" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O56" t="s">
         <v>187</v>
       </c>
       <c r="P56">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q56" t="s">
         <v>188</v>
@@ -4738,7 +4779,7 @@
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D57" t="s">
         <v>63</v>
@@ -4762,7 +4803,7 @@
         <v>62</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>63</v>
@@ -4771,13 +4812,13 @@
         <v>64</v>
       </c>
       <c r="N57" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="O57" t="s">
         <v>187</v>
       </c>
       <c r="P57">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q57" t="s">
         <v>188</v>
@@ -4791,7 +4832,7 @@
         <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D58" t="s">
         <v>63</v>
@@ -4815,7 +4856,7 @@
         <v>62</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>63</v>
@@ -4824,13 +4865,13 @@
         <v>64</v>
       </c>
       <c r="N58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O58" t="s">
         <v>187</v>
       </c>
       <c r="P58">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q58" t="s">
         <v>188</v>
@@ -4844,7 +4885,7 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D59" t="s">
         <v>63</v>
@@ -4868,7 +4909,7 @@
         <v>62</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>63</v>
@@ -4877,13 +4918,13 @@
         <v>64</v>
       </c>
       <c r="N59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O59" t="s">
         <v>187</v>
       </c>
       <c r="P59">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="Q59" t="s">
         <v>188</v>
@@ -4897,7 +4938,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D60" t="s">
         <v>63</v>
@@ -4921,7 +4962,7 @@
         <v>62</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>206</v>
+        <v>5</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>63</v>
@@ -4930,13 +4971,13 @@
         <v>64</v>
       </c>
       <c r="N60" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
       <c r="O60" t="s">
         <v>187</v>
       </c>
       <c r="P60">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q60" t="s">
         <v>188</v>
@@ -4950,7 +4991,7 @@
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -4974,7 +5015,7 @@
         <v>62</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>63</v>
@@ -4983,13 +5024,13 @@
         <v>64</v>
       </c>
       <c r="N61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O61" t="s">
         <v>187</v>
       </c>
       <c r="P61">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="Q61" t="s">
         <v>188</v>
@@ -5003,7 +5044,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D62" t="s">
         <v>63</v>
@@ -5027,7 +5068,7 @@
         <v>62</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>63</v>
@@ -5036,13 +5077,13 @@
         <v>64</v>
       </c>
       <c r="N62" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="O62" t="s">
         <v>187</v>
       </c>
       <c r="P62">
-        <v>1000000</v>
+        <v>500</v>
       </c>
       <c r="Q62" t="s">
         <v>188</v>
@@ -5056,7 +5097,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D63" t="s">
         <v>63</v>
@@ -5068,7 +5109,7 @@
         <v>62</v>
       </c>
       <c r="G63" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H63" t="s">
         <v>63</v>
@@ -5080,7 +5121,7 @@
         <v>62</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>63</v>
@@ -5089,13 +5130,13 @@
         <v>64</v>
       </c>
       <c r="N63" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="O63" t="s">
         <v>187</v>
       </c>
       <c r="P63">
-        <v>10</v>
+        <v>1000000</v>
       </c>
       <c r="Q63" t="s">
         <v>188</v>
@@ -5109,7 +5150,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D64" t="s">
         <v>63</v>
@@ -5133,7 +5174,7 @@
         <v>62</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>63</v>
@@ -5142,13 +5183,13 @@
         <v>64</v>
       </c>
       <c r="N64" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O64" t="s">
         <v>187</v>
       </c>
       <c r="P64">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="Q64" t="s">
         <v>188</v>
@@ -5162,7 +5203,7 @@
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D65" t="s">
         <v>63</v>
@@ -5186,7 +5227,7 @@
         <v>62</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>63</v>
@@ -5195,7 +5236,7 @@
         <v>64</v>
       </c>
       <c r="N65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O65" t="s">
         <v>187</v>
@@ -5215,7 +5256,7 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D66" t="s">
         <v>63</v>
@@ -5239,7 +5280,7 @@
         <v>62</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>63</v>
@@ -5248,13 +5289,13 @@
         <v>64</v>
       </c>
       <c r="N66" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="O66" t="s">
         <v>187</v>
       </c>
       <c r="P66">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="Q66" t="s">
         <v>188</v>
@@ -5268,7 +5309,7 @@
         <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D67" t="s">
         <v>63</v>
@@ -5292,7 +5333,7 @@
         <v>62</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>63</v>
@@ -5301,7 +5342,7 @@
         <v>64</v>
       </c>
       <c r="N67" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O67" t="s">
         <v>187</v>
@@ -5321,7 +5362,7 @@
         <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D68" t="s">
         <v>63</v>
@@ -5345,7 +5386,7 @@
         <v>62</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>63</v>
@@ -5354,13 +5395,13 @@
         <v>64</v>
       </c>
       <c r="N68" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="O68" t="s">
         <v>187</v>
       </c>
       <c r="P68">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="Q68" t="s">
         <v>188</v>
@@ -5374,7 +5415,7 @@
         <v>62</v>
       </c>
       <c r="C69" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D69" t="s">
         <v>63</v>
@@ -5398,7 +5439,7 @@
         <v>62</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>63</v>
@@ -5407,7 +5448,7 @@
         <v>64</v>
       </c>
       <c r="N69" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="O69" t="s">
         <v>187</v>
@@ -5427,7 +5468,7 @@
         <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D70" t="s">
         <v>63</v>
@@ -5451,7 +5492,7 @@
         <v>62</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>63</v>
@@ -5460,13 +5501,13 @@
         <v>64</v>
       </c>
       <c r="N70" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="O70" t="s">
         <v>187</v>
       </c>
       <c r="P70">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q70" t="s">
         <v>188</v>
@@ -5480,7 +5521,7 @@
         <v>62</v>
       </c>
       <c r="C71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D71" t="s">
         <v>63</v>
@@ -5504,7 +5545,7 @@
         <v>62</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>63</v>
@@ -5513,7 +5554,7 @@
         <v>64</v>
       </c>
       <c r="N71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O71" t="s">
         <v>187</v>
@@ -5533,7 +5574,7 @@
         <v>62</v>
       </c>
       <c r="C72" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D72" t="s">
         <v>63</v>
@@ -5557,7 +5598,7 @@
         <v>62</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>63</v>
@@ -5566,13 +5607,13 @@
         <v>64</v>
       </c>
       <c r="N72" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="O72" t="s">
         <v>187</v>
       </c>
       <c r="P72">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q72" t="s">
         <v>188</v>
@@ -5586,7 +5627,7 @@
         <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D73" t="s">
         <v>63</v>
@@ -5610,7 +5651,7 @@
         <v>62</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>63</v>
@@ -5619,7 +5660,7 @@
         <v>64</v>
       </c>
       <c r="N73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O73" t="s">
         <v>187</v>
@@ -5639,7 +5680,7 @@
         <v>62</v>
       </c>
       <c r="C74" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D74" t="s">
         <v>63</v>
@@ -5663,7 +5704,7 @@
         <v>62</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>63</v>
@@ -5672,13 +5713,13 @@
         <v>64</v>
       </c>
       <c r="N74" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="O74" t="s">
         <v>187</v>
       </c>
       <c r="P74">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q74" t="s">
         <v>188</v>
@@ -5692,7 +5733,7 @@
         <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D75" t="s">
         <v>63</v>
@@ -5716,7 +5757,7 @@
         <v>62</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>63</v>
@@ -5725,13 +5766,13 @@
         <v>64</v>
       </c>
       <c r="N75" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="O75" t="s">
         <v>187</v>
       </c>
       <c r="P75">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="Q75" t="s">
         <v>188</v>
@@ -5745,7 +5786,7 @@
         <v>62</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D76" t="s">
         <v>63</v>
@@ -5769,7 +5810,7 @@
         <v>62</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>63</v>
@@ -5778,13 +5819,13 @@
         <v>64</v>
       </c>
       <c r="N76" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="O76" t="s">
         <v>187</v>
       </c>
       <c r="P76">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="Q76" t="s">
         <v>188</v>
@@ -5798,7 +5839,7 @@
         <v>62</v>
       </c>
       <c r="C77" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D77" t="s">
         <v>63</v>
@@ -5822,7 +5863,7 @@
         <v>62</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>63</v>
@@ -5831,13 +5872,13 @@
         <v>64</v>
       </c>
       <c r="N77" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="O77" t="s">
         <v>187</v>
       </c>
       <c r="P77">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="Q77" t="s">
         <v>188</v>
@@ -5851,7 +5892,7 @@
         <v>62</v>
       </c>
       <c r="C78" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D78" t="s">
         <v>63</v>
@@ -5863,7 +5904,7 @@
         <v>62</v>
       </c>
       <c r="G78" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H78" t="s">
         <v>63</v>
@@ -5875,7 +5916,7 @@
         <v>62</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>63</v>
@@ -5884,13 +5925,13 @@
         <v>64</v>
       </c>
       <c r="N78" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="O78" t="s">
         <v>187</v>
       </c>
       <c r="P78">
-        <v>50</v>
+        <v>100000</v>
       </c>
       <c r="Q78" t="s">
         <v>188</v>
@@ -5904,7 +5945,7 @@
         <v>62</v>
       </c>
       <c r="C79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D79" t="s">
         <v>63</v>
@@ -5928,7 +5969,7 @@
         <v>62</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>63</v>
@@ -5937,13 +5978,13 @@
         <v>64</v>
       </c>
       <c r="N79" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O79" t="s">
         <v>187</v>
       </c>
       <c r="P79">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="Q79" t="s">
         <v>188</v>
@@ -5957,7 +5998,7 @@
         <v>62</v>
       </c>
       <c r="C80" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D80" t="s">
         <v>63</v>
@@ -5981,7 +6022,7 @@
         <v>62</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>63</v>
@@ -5990,13 +6031,13 @@
         <v>64</v>
       </c>
       <c r="N80" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O80" t="s">
         <v>187</v>
       </c>
       <c r="P80">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q80" t="s">
         <v>188</v>
@@ -6010,7 +6051,7 @@
         <v>62</v>
       </c>
       <c r="C81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D81" t="s">
         <v>63</v>
@@ -6034,7 +6075,7 @@
         <v>62</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L81" s="1" t="s">
         <v>63</v>
@@ -6043,13 +6084,13 @@
         <v>64</v>
       </c>
       <c r="N81" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O81" t="s">
         <v>187</v>
       </c>
       <c r="P81">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="Q81" t="s">
         <v>188</v>
@@ -6063,7 +6104,7 @@
         <v>62</v>
       </c>
       <c r="C82" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D82" t="s">
         <v>63</v>
@@ -6087,7 +6128,7 @@
         <v>62</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>63</v>
@@ -6096,13 +6137,13 @@
         <v>64</v>
       </c>
       <c r="N82" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="O82" t="s">
         <v>187</v>
       </c>
       <c r="P82">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q82" t="s">
         <v>188</v>
@@ -6116,7 +6157,7 @@
         <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D83" t="s">
         <v>63</v>
@@ -6140,7 +6181,7 @@
         <v>62</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>63</v>
@@ -6149,13 +6190,13 @@
         <v>64</v>
       </c>
       <c r="N83" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="O83" t="s">
         <v>187</v>
       </c>
       <c r="P83">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q83" t="s">
         <v>188</v>
@@ -6169,7 +6210,7 @@
         <v>62</v>
       </c>
       <c r="C84" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D84" t="s">
         <v>63</v>
@@ -6193,7 +6234,7 @@
         <v>62</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>63</v>
@@ -6202,13 +6243,13 @@
         <v>64</v>
       </c>
       <c r="N84" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O84" t="s">
         <v>187</v>
       </c>
       <c r="P84">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q84" t="s">
         <v>188</v>
@@ -6222,7 +6263,7 @@
         <v>62</v>
       </c>
       <c r="C85" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D85" t="s">
         <v>63</v>
@@ -6246,7 +6287,7 @@
         <v>62</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>63</v>
@@ -6255,13 +6296,13 @@
         <v>64</v>
       </c>
       <c r="N85" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="O85" t="s">
         <v>187</v>
       </c>
       <c r="P85">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="Q85" t="s">
         <v>188</v>
@@ -6275,7 +6316,7 @@
         <v>62</v>
       </c>
       <c r="C86" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D86" t="s">
         <v>63</v>
@@ -6287,7 +6328,7 @@
         <v>62</v>
       </c>
       <c r="G86" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H86" t="s">
         <v>63</v>
@@ -6299,7 +6340,7 @@
         <v>62</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>63</v>
@@ -6308,13 +6349,13 @@
         <v>64</v>
       </c>
       <c r="N86" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="O86" t="s">
         <v>187</v>
       </c>
       <c r="P86">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="Q86" t="s">
         <v>188</v>
@@ -6328,7 +6369,7 @@
         <v>62</v>
       </c>
       <c r="C87" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D87" t="s">
         <v>63</v>
@@ -6352,7 +6393,7 @@
         <v>62</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="L87" s="1" t="s">
         <v>63</v>
@@ -6381,7 +6422,7 @@
         <v>62</v>
       </c>
       <c r="C88" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D88" t="s">
         <v>63</v>
@@ -6405,7 +6446,7 @@
         <v>62</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>63</v>
@@ -6434,7 +6475,7 @@
         <v>62</v>
       </c>
       <c r="C89" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D89" t="s">
         <v>63</v>
@@ -6458,7 +6499,7 @@
         <v>62</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>63</v>
@@ -6467,13 +6508,13 @@
         <v>64</v>
       </c>
       <c r="N89" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="O89" t="s">
         <v>187</v>
       </c>
       <c r="P89">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q89" t="s">
         <v>188</v>
@@ -6487,7 +6528,7 @@
         <v>62</v>
       </c>
       <c r="C90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D90" t="s">
         <v>63</v>
@@ -6511,7 +6552,7 @@
         <v>62</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>63</v>
@@ -6520,13 +6561,13 @@
         <v>64</v>
       </c>
       <c r="N90" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="O90" t="s">
         <v>187</v>
       </c>
       <c r="P90">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q90" t="s">
         <v>188</v>
@@ -6540,7 +6581,7 @@
         <v>62</v>
       </c>
       <c r="C91" t="s">
-        <v>263</v>
+        <v>114</v>
       </c>
       <c r="D91" t="s">
         <v>63</v>
@@ -6563,8 +6604,8 @@
       <c r="J91" t="s">
         <v>62</v>
       </c>
-      <c r="K91" s="3" t="s">
-        <v>296</v>
+      <c r="K91" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>63</v>
@@ -6573,13 +6614,13 @@
         <v>64</v>
       </c>
       <c r="N91" t="s">
-        <v>268</v>
+        <v>158</v>
       </c>
       <c r="O91" t="s">
         <v>187</v>
       </c>
       <c r="P91">
-        <v>75000</v>
+        <v>5000</v>
       </c>
       <c r="Q91" t="s">
         <v>188</v>
@@ -6593,7 +6634,7 @@
         <v>62</v>
       </c>
       <c r="C92" t="s">
-        <v>118</v>
+        <v>263</v>
       </c>
       <c r="D92" t="s">
         <v>63</v>
@@ -6605,7 +6646,7 @@
         <v>62</v>
       </c>
       <c r="G92" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H92" t="s">
         <v>63</v>
@@ -6616,8 +6657,8 @@
       <c r="J92" t="s">
         <v>62</v>
       </c>
-      <c r="K92" s="1" t="s">
-        <v>189</v>
+      <c r="K92" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>63</v>
@@ -6626,13 +6667,13 @@
         <v>64</v>
       </c>
       <c r="N92" t="s">
-        <v>131</v>
+        <v>268</v>
       </c>
       <c r="O92" t="s">
         <v>187</v>
       </c>
       <c r="P92">
-        <v>50</v>
+        <v>75000</v>
       </c>
       <c r="Q92" t="s">
         <v>188</v>
@@ -6646,7 +6687,7 @@
         <v>62</v>
       </c>
       <c r="C93" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D93" t="s">
         <v>63</v>
@@ -6670,7 +6711,7 @@
         <v>62</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>63</v>
@@ -6679,13 +6720,13 @@
         <v>64</v>
       </c>
       <c r="N93" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O93" t="s">
         <v>187</v>
       </c>
       <c r="P93">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="Q93" t="s">
         <v>188</v>
@@ -6699,7 +6740,7 @@
         <v>62</v>
       </c>
       <c r="C94" t="s">
-        <v>223</v>
+        <v>119</v>
       </c>
       <c r="D94" t="s">
         <v>63</v>
@@ -6722,8 +6763,8 @@
       <c r="J94" t="s">
         <v>62</v>
       </c>
-      <c r="K94" s="3" t="s">
-        <v>275</v>
+      <c r="K94" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>63</v>
@@ -6732,13 +6773,13 @@
         <v>64</v>
       </c>
       <c r="N94" t="s">
-        <v>229</v>
+        <v>130</v>
       </c>
       <c r="O94" t="s">
         <v>187</v>
       </c>
       <c r="P94">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="Q94" t="s">
         <v>188</v>
@@ -6752,7 +6793,7 @@
         <v>62</v>
       </c>
       <c r="C95" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D95" t="s">
         <v>63</v>
@@ -6775,8 +6816,8 @@
       <c r="J95" t="s">
         <v>62</v>
       </c>
-      <c r="K95" s="1" t="s">
-        <v>278</v>
+      <c r="K95" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>63</v>
@@ -6785,13 +6826,13 @@
         <v>64</v>
       </c>
       <c r="N95" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O95" t="s">
         <v>187</v>
       </c>
       <c r="P95">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q95" t="s">
         <v>188</v>
@@ -6805,7 +6846,7 @@
         <v>62</v>
       </c>
       <c r="C96" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D96" t="s">
         <v>63</v>
@@ -6829,7 +6870,7 @@
         <v>62</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>63</v>
@@ -6838,13 +6879,13 @@
         <v>64</v>
       </c>
       <c r="N96" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="O96" t="s">
         <v>187</v>
       </c>
       <c r="P96">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="Q96" t="s">
         <v>188</v>
@@ -6858,7 +6899,7 @@
         <v>62</v>
       </c>
       <c r="C97" t="s">
-        <v>227</v>
+        <v>330</v>
       </c>
       <c r="D97" t="s">
         <v>63</v>
@@ -6882,7 +6923,7 @@
         <v>62</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>279</v>
+        <v>336</v>
       </c>
       <c r="L97" s="1" t="s">
         <v>63</v>
@@ -6891,13 +6932,13 @@
         <v>64</v>
       </c>
       <c r="N97" t="s">
-        <v>233</v>
+        <v>337</v>
       </c>
       <c r="O97" t="s">
         <v>187</v>
       </c>
       <c r="P97">
-        <v>25000</v>
+        <v>2500</v>
       </c>
       <c r="Q97" t="s">
         <v>188</v>
@@ -6911,7 +6952,7 @@
         <v>62</v>
       </c>
       <c r="C98" t="s">
-        <v>120</v>
+        <v>328</v>
       </c>
       <c r="D98" t="s">
         <v>63</v>
@@ -6935,7 +6976,7 @@
         <v>62</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>37</v>
+        <v>332</v>
       </c>
       <c r="L98" s="1" t="s">
         <v>63</v>
@@ -6944,13 +6985,13 @@
         <v>64</v>
       </c>
       <c r="N98" t="s">
-        <v>165</v>
+        <v>333</v>
       </c>
       <c r="O98" t="s">
         <v>187</v>
       </c>
       <c r="P98">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="Q98" t="s">
         <v>188</v>
@@ -6964,7 +7005,7 @@
         <v>62</v>
       </c>
       <c r="C99" t="s">
-        <v>224</v>
+        <v>329</v>
       </c>
       <c r="D99" t="s">
         <v>63</v>
@@ -6987,8 +7028,8 @@
       <c r="J99" t="s">
         <v>62</v>
       </c>
-      <c r="K99" s="3" t="s">
-        <v>276</v>
+      <c r="K99" s="1" t="s">
+        <v>334</v>
       </c>
       <c r="L99" s="1" t="s">
         <v>63</v>
@@ -6997,13 +7038,13 @@
         <v>64</v>
       </c>
       <c r="N99" t="s">
-        <v>230</v>
+        <v>335</v>
       </c>
       <c r="O99" t="s">
         <v>187</v>
       </c>
       <c r="P99">
-        <v>75000</v>
+        <v>7500</v>
       </c>
       <c r="Q99" t="s">
         <v>188</v>
@@ -7017,7 +7058,7 @@
         <v>62</v>
       </c>
       <c r="C100" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D100" t="s">
         <v>63</v>
@@ -7040,8 +7081,8 @@
       <c r="J100" t="s">
         <v>62</v>
       </c>
-      <c r="K100" s="3" t="s">
-        <v>277</v>
+      <c r="K100" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="L100" s="1" t="s">
         <v>63</v>
@@ -7050,13 +7091,13 @@
         <v>64</v>
       </c>
       <c r="N100" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="O100" t="s">
         <v>187</v>
       </c>
       <c r="P100">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="Q100" t="s">
         <v>188</v>
@@ -7070,7 +7111,7 @@
         <v>62</v>
       </c>
       <c r="C101" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="D101" t="s">
         <v>63</v>
@@ -7094,26 +7135,242 @@
         <v>62</v>
       </c>
       <c r="K101" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M101" t="s">
+        <v>64</v>
+      </c>
+      <c r="N101" t="s">
+        <v>233</v>
+      </c>
+      <c r="O101" t="s">
+        <v>187</v>
+      </c>
+      <c r="P101">
+        <v>25000</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>61</v>
+      </c>
+      <c r="B102" t="s">
+        <v>62</v>
+      </c>
+      <c r="C102" t="s">
+        <v>120</v>
+      </c>
+      <c r="D102" t="s">
+        <v>63</v>
+      </c>
+      <c r="E102" t="s">
+        <v>122</v>
+      </c>
+      <c r="F102" t="s">
+        <v>62</v>
+      </c>
+      <c r="G102" t="s">
+        <v>125</v>
+      </c>
+      <c r="H102" t="s">
+        <v>63</v>
+      </c>
+      <c r="I102" t="s">
+        <v>60</v>
+      </c>
+      <c r="J102" t="s">
+        <v>62</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M102" t="s">
+        <v>64</v>
+      </c>
+      <c r="N102" t="s">
+        <v>165</v>
+      </c>
+      <c r="O102" t="s">
+        <v>187</v>
+      </c>
+      <c r="P102">
+        <v>50000</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>61</v>
+      </c>
+      <c r="B103" t="s">
+        <v>62</v>
+      </c>
+      <c r="C103" t="s">
+        <v>224</v>
+      </c>
+      <c r="D103" t="s">
+        <v>63</v>
+      </c>
+      <c r="E103" t="s">
+        <v>122</v>
+      </c>
+      <c r="F103" t="s">
+        <v>62</v>
+      </c>
+      <c r="G103" t="s">
+        <v>125</v>
+      </c>
+      <c r="H103" t="s">
+        <v>63</v>
+      </c>
+      <c r="I103" t="s">
+        <v>60</v>
+      </c>
+      <c r="J103" t="s">
+        <v>62</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M103" t="s">
+        <v>64</v>
+      </c>
+      <c r="N103" t="s">
+        <v>230</v>
+      </c>
+      <c r="O103" t="s">
+        <v>187</v>
+      </c>
+      <c r="P103">
+        <v>75000</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>61</v>
+      </c>
+      <c r="B104" t="s">
+        <v>62</v>
+      </c>
+      <c r="C104" t="s">
+        <v>225</v>
+      </c>
+      <c r="D104" t="s">
+        <v>63</v>
+      </c>
+      <c r="E104" t="s">
+        <v>122</v>
+      </c>
+      <c r="F104" t="s">
+        <v>62</v>
+      </c>
+      <c r="G104" t="s">
+        <v>125</v>
+      </c>
+      <c r="H104" t="s">
+        <v>63</v>
+      </c>
+      <c r="I104" t="s">
+        <v>60</v>
+      </c>
+      <c r="J104" t="s">
+        <v>62</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M104" t="s">
+        <v>64</v>
+      </c>
+      <c r="N104" t="s">
+        <v>231</v>
+      </c>
+      <c r="O104" t="s">
+        <v>187</v>
+      </c>
+      <c r="P104">
+        <v>100000</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>61</v>
+      </c>
+      <c r="B105" t="s">
+        <v>62</v>
+      </c>
+      <c r="C105" t="s">
+        <v>121</v>
+      </c>
+      <c r="D105" t="s">
+        <v>63</v>
+      </c>
+      <c r="E105" t="s">
+        <v>122</v>
+      </c>
+      <c r="F105" t="s">
+        <v>62</v>
+      </c>
+      <c r="G105" t="s">
+        <v>125</v>
+      </c>
+      <c r="H105" t="s">
+        <v>63</v>
+      </c>
+      <c r="I105" t="s">
+        <v>60</v>
+      </c>
+      <c r="J105" t="s">
+        <v>62</v>
+      </c>
+      <c r="K105" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L101" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M101" t="s">
-        <v>64</v>
-      </c>
-      <c r="N101" t="s">
+      <c r="L105" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M105" t="s">
+        <v>64</v>
+      </c>
+      <c r="N105" t="s">
         <v>305</v>
       </c>
-      <c r="O101" t="s">
-        <v>187</v>
-      </c>
-      <c r="P101">
+      <c r="O105" t="s">
+        <v>187</v>
+      </c>
+      <c r="P105">
         <v>500000</v>
       </c>
-      <c r="Q101" t="s">
-        <v>188</v>
-      </c>
+      <c r="Q105" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
made number black, added witch hat
</commit_message>
<xml_diff>
--- a/HutListe.xlsx
+++ b/HutListe.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="343">
   <si>
     <t>states/schaf.png</t>
   </si>
@@ -1369,6 +1369,15 @@
   </si>
   <si>
     <t>Damit zeigst du allen wie toll ein Kreis sein kann!</t>
+  </si>
+  <si>
+    <t>pics/sm_witch.gif</t>
+  </si>
+  <si>
+    <t>So ein Besen kann vielfältig verwendet werden. Von der richtigen Person!</t>
+  </si>
+  <si>
+    <t>b26</t>
   </si>
 </sst>
 </file>
@@ -1780,7 +1789,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1790,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F79" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q105"/>
+    <sheetView tabSelected="1" topLeftCell="F85" workbookViewId="0">
+      <selection activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1927,7 +1936,7 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -1951,7 +1960,7 @@
         <v>62</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>190</v>
+        <v>25</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>63</v>
@@ -1960,7 +1969,7 @@
         <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>132</v>
+        <v>304</v>
       </c>
       <c r="O3" t="s">
         <v>187</v>
@@ -2086,7 +2095,7 @@
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -2110,7 +2119,7 @@
         <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>63</v>
@@ -2119,7 +2128,7 @@
         <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="O6" t="s">
         <v>187</v>
@@ -2139,7 +2148,7 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>204</v>
+        <v>301</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
@@ -2163,7 +2172,7 @@
         <v>62</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>42</v>
+        <v>303</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>63</v>
@@ -2172,7 +2181,7 @@
         <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>170</v>
+        <v>302</v>
       </c>
       <c r="O7" t="s">
         <v>187</v>
@@ -2192,7 +2201,7 @@
         <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>202</v>
+        <v>306</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
@@ -2216,7 +2225,7 @@
         <v>62</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>43</v>
+        <v>308</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>63</v>
@@ -2225,7 +2234,7 @@
         <v>64</v>
       </c>
       <c r="N8" t="s">
-        <v>171</v>
+        <v>307</v>
       </c>
       <c r="O8" t="s">
         <v>187</v>
@@ -2245,7 +2254,7 @@
         <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>309</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -2269,7 +2278,7 @@
         <v>62</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>25</v>
+        <v>311</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>63</v>
@@ -2278,7 +2287,7 @@
         <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="O9" t="s">
         <v>187</v>
@@ -2298,7 +2307,7 @@
         <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>253</v>
+        <v>312</v>
       </c>
       <c r="D10" t="s">
         <v>63</v>
@@ -2321,8 +2330,8 @@
       <c r="J10" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>292</v>
+      <c r="K10" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>63</v>
@@ -2331,7 +2340,7 @@
         <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
       <c r="O10" t="s">
         <v>187</v>
@@ -2351,7 +2360,7 @@
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>301</v>
+        <v>314</v>
       </c>
       <c r="D11" t="s">
         <v>63</v>
@@ -2375,7 +2384,7 @@
         <v>62</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>303</v>
+        <v>327</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>63</v>
@@ -2384,7 +2393,7 @@
         <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="O11" t="s">
         <v>187</v>
@@ -2404,7 +2413,7 @@
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
@@ -2427,9 +2436,7 @@
       <c r="J12" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>308</v>
-      </c>
+      <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
         <v>63</v>
       </c>
@@ -2437,7 +2444,7 @@
         <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="O12" t="s">
         <v>187</v>
@@ -2457,7 +2464,7 @@
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
@@ -2480,9 +2487,7 @@
       <c r="J13" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>311</v>
-      </c>
+      <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
         <v>63</v>
       </c>
@@ -2490,7 +2495,7 @@
         <v>64</v>
       </c>
       <c r="N13" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="O13" t="s">
         <v>187</v>
@@ -2510,7 +2515,7 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
@@ -2533,9 +2538,7 @@
       <c r="J14" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>326</v>
-      </c>
+      <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
         <v>63</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="O14" t="s">
         <v>187</v>
@@ -2563,7 +2566,7 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="D15" t="s">
         <v>63</v>
@@ -2586,9 +2589,7 @@
       <c r="J15" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>327</v>
-      </c>
+      <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
         <v>63</v>
       </c>
@@ -2596,7 +2597,7 @@
         <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="O15" t="s">
         <v>187</v>
@@ -2616,7 +2617,7 @@
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="D16" t="s">
         <v>63</v>
@@ -2647,7 +2648,7 @@
         <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="O16" t="s">
         <v>187</v>
@@ -2667,7 +2668,7 @@
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>316</v>
+        <v>253</v>
       </c>
       <c r="D17" t="s">
         <v>63</v>
@@ -2690,7 +2691,9 @@
       <c r="J17" t="s">
         <v>62</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="3" t="s">
+        <v>292</v>
+      </c>
       <c r="L17" s="1" t="s">
         <v>63</v>
       </c>
@@ -2698,7 +2701,7 @@
         <v>64</v>
       </c>
       <c r="N17" t="s">
-        <v>319</v>
+        <v>260</v>
       </c>
       <c r="O17" t="s">
         <v>187</v>
@@ -2718,7 +2721,7 @@
         <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>320</v>
+        <v>198</v>
       </c>
       <c r="D18" t="s">
         <v>63</v>
@@ -2741,7 +2744,9 @@
       <c r="J18" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="L18" s="1" t="s">
         <v>63</v>
       </c>
@@ -2749,7 +2754,7 @@
         <v>64</v>
       </c>
       <c r="N18" t="s">
-        <v>323</v>
+        <v>132</v>
       </c>
       <c r="O18" t="s">
         <v>187</v>
@@ -2769,7 +2774,7 @@
         <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>321</v>
+        <v>203</v>
       </c>
       <c r="D19" t="s">
         <v>63</v>
@@ -2792,7 +2797,9 @@
       <c r="J19" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="L19" s="1" t="s">
         <v>63</v>
       </c>
@@ -2800,7 +2807,7 @@
         <v>64</v>
       </c>
       <c r="N19" t="s">
-        <v>324</v>
+        <v>169</v>
       </c>
       <c r="O19" t="s">
         <v>187</v>
@@ -2820,7 +2827,7 @@
         <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>322</v>
+        <v>204</v>
       </c>
       <c r="D20" t="s">
         <v>63</v>
@@ -2843,7 +2850,9 @@
       <c r="J20" t="s">
         <v>62</v>
       </c>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="L20" s="1" t="s">
         <v>63</v>
       </c>
@@ -2851,7 +2860,7 @@
         <v>64</v>
       </c>
       <c r="N20" t="s">
-        <v>325</v>
+        <v>170</v>
       </c>
       <c r="O20" t="s">
         <v>187</v>
@@ -3984,7 +3993,7 @@
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>342</v>
       </c>
       <c r="D42" t="s">
         <v>63</v>
@@ -4007,8 +4016,8 @@
       <c r="J42" t="s">
         <v>62</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>8</v>
+      <c r="K42" s="3" t="s">
+        <v>340</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>63</v>
@@ -4017,13 +4026,13 @@
         <v>64</v>
       </c>
       <c r="N42" t="s">
-        <v>146</v>
+        <v>341</v>
       </c>
       <c r="O42" t="s">
         <v>187</v>
       </c>
       <c r="P42">
-        <v>100000</v>
+        <v>75000</v>
       </c>
       <c r="Q42" t="s">
         <v>188</v>
@@ -4037,7 +4046,7 @@
         <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s">
         <v>63</v>
@@ -4061,7 +4070,7 @@
         <v>62</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>63</v>
@@ -4070,13 +4079,13 @@
         <v>64</v>
       </c>
       <c r="N43" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="O43" t="s">
         <v>187</v>
       </c>
       <c r="P43">
-        <v>250000</v>
+        <v>100000</v>
       </c>
       <c r="Q43" t="s">
         <v>188</v>
@@ -4090,7 +4099,7 @@
         <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D44" t="s">
         <v>63</v>
@@ -4114,7 +4123,7 @@
         <v>62</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>63</v>
@@ -4123,13 +4132,13 @@
         <v>64</v>
       </c>
       <c r="N44" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="O44" t="s">
         <v>187</v>
       </c>
       <c r="P44">
-        <v>500000</v>
+        <v>250000</v>
       </c>
       <c r="Q44" t="s">
         <v>188</v>
@@ -4143,7 +4152,7 @@
         <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
         <v>63</v>
@@ -4167,7 +4176,7 @@
         <v>62</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>63</v>
@@ -4176,13 +4185,13 @@
         <v>64</v>
       </c>
       <c r="N45" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="O45" t="s">
         <v>187</v>
       </c>
       <c r="P45">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="Q45" t="s">
         <v>188</v>
@@ -4196,7 +4205,7 @@
         <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D46" t="s">
         <v>63</v>
@@ -4220,7 +4229,7 @@
         <v>62</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>63</v>
@@ -4229,13 +4238,13 @@
         <v>64</v>
       </c>
       <c r="N46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O46" t="s">
         <v>187</v>
       </c>
       <c r="P46">
-        <v>2500000</v>
+        <v>1000000</v>
       </c>
       <c r="Q46" t="s">
         <v>188</v>
@@ -4249,7 +4258,7 @@
         <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>262</v>
+        <v>81</v>
       </c>
       <c r="D47" t="s">
         <v>63</v>
@@ -4261,7 +4270,7 @@
         <v>62</v>
       </c>
       <c r="G47" t="s">
-        <v>274</v>
+        <v>129</v>
       </c>
       <c r="H47" t="s">
         <v>63</v>
@@ -4272,8 +4281,8 @@
       <c r="J47" t="s">
         <v>62</v>
       </c>
-      <c r="K47" s="4" t="s">
-        <v>295</v>
+      <c r="K47" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>63</v>
@@ -4282,13 +4291,13 @@
         <v>64</v>
       </c>
       <c r="N47" t="s">
-        <v>267</v>
+        <v>162</v>
       </c>
       <c r="O47" t="s">
         <v>187</v>
       </c>
       <c r="P47">
-        <v>500</v>
+        <v>2500000</v>
       </c>
       <c r="Q47" t="s">
         <v>188</v>
@@ -4302,7 +4311,7 @@
         <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="D48" t="s">
         <v>63</v>
@@ -4326,7 +4335,7 @@
         <v>62</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>63</v>
@@ -4335,13 +4344,13 @@
         <v>64</v>
       </c>
       <c r="N48" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="O48" t="s">
         <v>187</v>
       </c>
       <c r="P48">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q48" t="s">
         <v>188</v>
@@ -4355,7 +4364,7 @@
         <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D49" t="s">
         <v>63</v>
@@ -4379,7 +4388,7 @@
         <v>62</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>63</v>
@@ -4388,13 +4397,13 @@
         <v>64</v>
       </c>
       <c r="N49" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O49" t="s">
         <v>187</v>
       </c>
       <c r="P49">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q49" t="s">
         <v>188</v>
@@ -4408,7 +4417,7 @@
         <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="D50" t="s">
         <v>63</v>
@@ -4432,7 +4441,7 @@
         <v>62</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>63</v>
@@ -4441,13 +4450,13 @@
         <v>64</v>
       </c>
       <c r="N50" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="O50" t="s">
         <v>187</v>
       </c>
       <c r="P50">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q50" t="s">
         <v>188</v>
@@ -4461,7 +4470,7 @@
         <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D51" t="s">
         <v>63</v>
@@ -4484,8 +4493,8 @@
       <c r="J51" t="s">
         <v>62</v>
       </c>
-      <c r="K51" s="3" t="s">
-        <v>298</v>
+      <c r="K51" s="4" t="s">
+        <v>294</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>63</v>
@@ -4494,13 +4503,13 @@
         <v>64</v>
       </c>
       <c r="N51" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="O51" t="s">
         <v>187</v>
       </c>
       <c r="P51">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="Q51" t="s">
         <v>188</v>
@@ -4514,7 +4523,7 @@
         <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>241</v>
+        <v>269</v>
       </c>
       <c r="D52" t="s">
         <v>63</v>
@@ -4537,8 +4546,8 @@
       <c r="J52" t="s">
         <v>62</v>
       </c>
-      <c r="K52" s="4" t="s">
-        <v>286</v>
+      <c r="K52" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>63</v>
@@ -4547,13 +4556,13 @@
         <v>64</v>
       </c>
       <c r="N52" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
       <c r="O52" t="s">
         <v>187</v>
       </c>
       <c r="P52">
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="Q52" t="s">
         <v>188</v>
@@ -4567,7 +4576,7 @@
         <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="D53" t="s">
         <v>63</v>
@@ -4590,8 +4599,8 @@
       <c r="J53" t="s">
         <v>62</v>
       </c>
-      <c r="K53" s="3" t="s">
-        <v>289</v>
+      <c r="K53" s="4" t="s">
+        <v>286</v>
       </c>
       <c r="L53" s="1" t="s">
         <v>63</v>
@@ -4600,13 +4609,13 @@
         <v>64</v>
       </c>
       <c r="N53" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="O53" t="s">
         <v>187</v>
       </c>
       <c r="P53">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="Q53" t="s">
         <v>188</v>
@@ -4620,7 +4629,7 @@
         <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D54" t="s">
         <v>63</v>
@@ -4644,7 +4653,7 @@
         <v>62</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>63</v>
@@ -4653,13 +4662,13 @@
         <v>64</v>
       </c>
       <c r="N54" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="O54" t="s">
         <v>187</v>
       </c>
       <c r="P54">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="Q54" t="s">
         <v>188</v>
@@ -4673,7 +4682,7 @@
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>331</v>
+        <v>254</v>
       </c>
       <c r="D55" t="s">
         <v>63</v>
@@ -4696,8 +4705,8 @@
       <c r="J55" t="s">
         <v>62</v>
       </c>
-      <c r="K55" s="1" t="s">
-        <v>338</v>
+      <c r="K55" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>63</v>
@@ -4706,13 +4715,13 @@
         <v>64</v>
       </c>
       <c r="N55" t="s">
-        <v>339</v>
+        <v>265</v>
       </c>
       <c r="O55" t="s">
         <v>187</v>
       </c>
       <c r="P55">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="Q55" t="s">
         <v>188</v>
@@ -4726,7 +4735,7 @@
         <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>331</v>
       </c>
       <c r="D56" t="s">
         <v>63</v>
@@ -4738,7 +4747,7 @@
         <v>62</v>
       </c>
       <c r="G56" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="H56" t="s">
         <v>63</v>
@@ -4750,7 +4759,7 @@
         <v>62</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>2</v>
+        <v>338</v>
       </c>
       <c r="L56" s="1" t="s">
         <v>63</v>
@@ -4759,13 +4768,13 @@
         <v>64</v>
       </c>
       <c r="N56" t="s">
-        <v>134</v>
+        <v>339</v>
       </c>
       <c r="O56" t="s">
         <v>187</v>
       </c>
       <c r="P56">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="Q56" t="s">
         <v>188</v>
@@ -4779,7 +4788,7 @@
         <v>62</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D57" t="s">
         <v>63</v>
@@ -4803,7 +4812,7 @@
         <v>62</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>63</v>
@@ -4812,13 +4821,13 @@
         <v>64</v>
       </c>
       <c r="N57" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O57" t="s">
         <v>187</v>
       </c>
       <c r="P57">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Q57" t="s">
         <v>188</v>
@@ -4832,7 +4841,7 @@
         <v>62</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D58" t="s">
         <v>63</v>
@@ -4856,7 +4865,7 @@
         <v>62</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>63</v>
@@ -4865,13 +4874,13 @@
         <v>64</v>
       </c>
       <c r="N58" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="O58" t="s">
         <v>187</v>
       </c>
       <c r="P58">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q58" t="s">
         <v>188</v>
@@ -4885,7 +4894,7 @@
         <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D59" t="s">
         <v>63</v>
@@ -4909,7 +4918,7 @@
         <v>62</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>63</v>
@@ -4918,13 +4927,13 @@
         <v>64</v>
       </c>
       <c r="N59" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O59" t="s">
         <v>187</v>
       </c>
       <c r="P59">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q59" t="s">
         <v>188</v>
@@ -4938,7 +4947,7 @@
         <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D60" t="s">
         <v>63</v>
@@ -4962,7 +4971,7 @@
         <v>62</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>63</v>
@@ -4971,13 +4980,13 @@
         <v>64</v>
       </c>
       <c r="N60" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O60" t="s">
         <v>187</v>
       </c>
       <c r="P60">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="Q60" t="s">
         <v>188</v>
@@ -4991,7 +5000,7 @@
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -5015,7 +5024,7 @@
         <v>62</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>206</v>
+        <v>5</v>
       </c>
       <c r="L61" s="1" t="s">
         <v>63</v>
@@ -5024,13 +5033,13 @@
         <v>64</v>
       </c>
       <c r="N61" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
       <c r="O61" t="s">
         <v>187</v>
       </c>
       <c r="P61">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q61" t="s">
         <v>188</v>
@@ -5044,7 +5053,7 @@
         <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D62" t="s">
         <v>63</v>
@@ -5068,7 +5077,7 @@
         <v>62</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>63</v>
@@ -5077,13 +5086,13 @@
         <v>64</v>
       </c>
       <c r="N62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O62" t="s">
         <v>187</v>
       </c>
       <c r="P62">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="Q62" t="s">
         <v>188</v>
@@ -5097,7 +5106,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D63" t="s">
         <v>63</v>
@@ -5121,7 +5130,7 @@
         <v>62</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>63</v>
@@ -5130,13 +5139,13 @@
         <v>64</v>
       </c>
       <c r="N63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="O63" t="s">
         <v>187</v>
       </c>
       <c r="P63">
-        <v>1000000</v>
+        <v>500</v>
       </c>
       <c r="Q63" t="s">
         <v>188</v>
@@ -5150,7 +5159,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D64" t="s">
         <v>63</v>
@@ -5162,7 +5171,7 @@
         <v>62</v>
       </c>
       <c r="G64" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H64" t="s">
         <v>63</v>
@@ -5174,7 +5183,7 @@
         <v>62</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>63</v>
@@ -5183,13 +5192,13 @@
         <v>64</v>
       </c>
       <c r="N64" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="O64" t="s">
         <v>187</v>
       </c>
       <c r="P64">
-        <v>10</v>
+        <v>1000000</v>
       </c>
       <c r="Q64" t="s">
         <v>188</v>
@@ -5203,7 +5212,7 @@
         <v>62</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D65" t="s">
         <v>63</v>
@@ -5227,7 +5236,7 @@
         <v>62</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>63</v>
@@ -5236,13 +5245,13 @@
         <v>64</v>
       </c>
       <c r="N65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O65" t="s">
         <v>187</v>
       </c>
       <c r="P65">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="Q65" t="s">
         <v>188</v>
@@ -5256,7 +5265,7 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D66" t="s">
         <v>63</v>
@@ -5280,7 +5289,7 @@
         <v>62</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>63</v>
@@ -5289,7 +5298,7 @@
         <v>64</v>
       </c>
       <c r="N66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O66" t="s">
         <v>187</v>
@@ -5309,7 +5318,7 @@
         <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D67" t="s">
         <v>63</v>
@@ -5333,7 +5342,7 @@
         <v>62</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>63</v>
@@ -5342,13 +5351,13 @@
         <v>64</v>
       </c>
       <c r="N67" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="O67" t="s">
         <v>187</v>
       </c>
       <c r="P67">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="Q67" t="s">
         <v>188</v>
@@ -5362,7 +5371,7 @@
         <v>62</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D68" t="s">
         <v>63</v>
@@ -5386,7 +5395,7 @@
         <v>62</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>63</v>
@@ -5395,7 +5404,7 @@
         <v>64</v>
       </c>
       <c r="N68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O68" t="s">
         <v>187</v>
@@ -5415,7 +5424,7 @@
         <v>62</v>
       </c>
       <c r="C69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D69" t="s">
         <v>63</v>
@@ -5439,7 +5448,7 @@
         <v>62</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="L69" s="1" t="s">
         <v>63</v>
@@ -5448,13 +5457,13 @@
         <v>64</v>
       </c>
       <c r="N69" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="O69" t="s">
         <v>187</v>
       </c>
       <c r="P69">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="Q69" t="s">
         <v>188</v>
@@ -5468,7 +5477,7 @@
         <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D70" t="s">
         <v>63</v>
@@ -5492,7 +5501,7 @@
         <v>62</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L70" s="1" t="s">
         <v>63</v>
@@ -5501,7 +5510,7 @@
         <v>64</v>
       </c>
       <c r="N70" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="O70" t="s">
         <v>187</v>
@@ -5521,7 +5530,7 @@
         <v>62</v>
       </c>
       <c r="C71" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D71" t="s">
         <v>63</v>
@@ -5545,7 +5554,7 @@
         <v>62</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>63</v>
@@ -5554,13 +5563,13 @@
         <v>64</v>
       </c>
       <c r="N71" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="O71" t="s">
         <v>187</v>
       </c>
       <c r="P71">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q71" t="s">
         <v>188</v>
@@ -5574,7 +5583,7 @@
         <v>62</v>
       </c>
       <c r="C72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D72" t="s">
         <v>63</v>
@@ -5598,7 +5607,7 @@
         <v>62</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>63</v>
@@ -5607,7 +5616,7 @@
         <v>64</v>
       </c>
       <c r="N72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O72" t="s">
         <v>187</v>
@@ -5627,7 +5636,7 @@
         <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D73" t="s">
         <v>63</v>
@@ -5651,7 +5660,7 @@
         <v>62</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>63</v>
@@ -5660,13 +5669,13 @@
         <v>64</v>
       </c>
       <c r="N73" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="O73" t="s">
         <v>187</v>
       </c>
       <c r="P73">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q73" t="s">
         <v>188</v>
@@ -5680,7 +5689,7 @@
         <v>62</v>
       </c>
       <c r="C74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D74" t="s">
         <v>63</v>
@@ -5704,7 +5713,7 @@
         <v>62</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L74" s="1" t="s">
         <v>63</v>
@@ -5713,7 +5722,7 @@
         <v>64</v>
       </c>
       <c r="N74" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O74" t="s">
         <v>187</v>
@@ -5733,7 +5742,7 @@
         <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D75" t="s">
         <v>63</v>
@@ -5757,7 +5766,7 @@
         <v>62</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>63</v>
@@ -5766,13 +5775,13 @@
         <v>64</v>
       </c>
       <c r="N75" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="O75" t="s">
         <v>187</v>
       </c>
       <c r="P75">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q75" t="s">
         <v>188</v>
@@ -5786,7 +5795,7 @@
         <v>62</v>
       </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D76" t="s">
         <v>63</v>
@@ -5810,7 +5819,7 @@
         <v>62</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>63</v>
@@ -5819,13 +5828,13 @@
         <v>64</v>
       </c>
       <c r="N76" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="O76" t="s">
         <v>187</v>
       </c>
       <c r="P76">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="Q76" t="s">
         <v>188</v>
@@ -5839,7 +5848,7 @@
         <v>62</v>
       </c>
       <c r="C77" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D77" t="s">
         <v>63</v>
@@ -5863,7 +5872,7 @@
         <v>62</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="L77" s="1" t="s">
         <v>63</v>
@@ -5872,13 +5881,13 @@
         <v>64</v>
       </c>
       <c r="N77" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="O77" t="s">
         <v>187</v>
       </c>
       <c r="P77">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="Q77" t="s">
         <v>188</v>
@@ -5892,7 +5901,7 @@
         <v>62</v>
       </c>
       <c r="C78" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D78" t="s">
         <v>63</v>
@@ -5916,7 +5925,7 @@
         <v>62</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L78" s="1" t="s">
         <v>63</v>
@@ -5925,13 +5934,13 @@
         <v>64</v>
       </c>
       <c r="N78" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="O78" t="s">
         <v>187</v>
       </c>
       <c r="P78">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="Q78" t="s">
         <v>188</v>
@@ -5945,7 +5954,7 @@
         <v>62</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D79" t="s">
         <v>63</v>
@@ -5957,7 +5966,7 @@
         <v>62</v>
       </c>
       <c r="G79" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H79" t="s">
         <v>63</v>
@@ -5969,7 +5978,7 @@
         <v>62</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>63</v>
@@ -5978,13 +5987,13 @@
         <v>64</v>
       </c>
       <c r="N79" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="O79" t="s">
         <v>187</v>
       </c>
       <c r="P79">
-        <v>50</v>
+        <v>100000</v>
       </c>
       <c r="Q79" t="s">
         <v>188</v>
@@ -5998,7 +6007,7 @@
         <v>62</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D80" t="s">
         <v>63</v>
@@ -6022,7 +6031,7 @@
         <v>62</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>63</v>
@@ -6031,13 +6040,13 @@
         <v>64</v>
       </c>
       <c r="N80" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O80" t="s">
         <v>187</v>
       </c>
       <c r="P80">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="Q80" t="s">
         <v>188</v>
@@ -6051,7 +6060,7 @@
         <v>62</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D81" t="s">
         <v>63</v>
@@ -6075,7 +6084,7 @@
         <v>62</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L81" s="1" t="s">
         <v>63</v>
@@ -6084,13 +6093,13 @@
         <v>64</v>
       </c>
       <c r="N81" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O81" t="s">
         <v>187</v>
       </c>
       <c r="P81">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q81" t="s">
         <v>188</v>
@@ -6104,7 +6113,7 @@
         <v>62</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D82" t="s">
         <v>63</v>
@@ -6128,7 +6137,7 @@
         <v>62</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>63</v>
@@ -6137,13 +6146,13 @@
         <v>64</v>
       </c>
       <c r="N82" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O82" t="s">
         <v>187</v>
       </c>
       <c r="P82">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="Q82" t="s">
         <v>188</v>
@@ -6157,7 +6166,7 @@
         <v>62</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D83" t="s">
         <v>63</v>
@@ -6181,7 +6190,7 @@
         <v>62</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>63</v>
@@ -6190,13 +6199,13 @@
         <v>64</v>
       </c>
       <c r="N83" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="O83" t="s">
         <v>187</v>
       </c>
       <c r="P83">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q83" t="s">
         <v>188</v>
@@ -6210,7 +6219,7 @@
         <v>62</v>
       </c>
       <c r="C84" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D84" t="s">
         <v>63</v>
@@ -6234,7 +6243,7 @@
         <v>62</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>63</v>
@@ -6243,13 +6252,13 @@
         <v>64</v>
       </c>
       <c r="N84" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="O84" t="s">
         <v>187</v>
       </c>
       <c r="P84">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q84" t="s">
         <v>188</v>
@@ -6263,7 +6272,7 @@
         <v>62</v>
       </c>
       <c r="C85" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D85" t="s">
         <v>63</v>
@@ -6287,7 +6296,7 @@
         <v>62</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>63</v>
@@ -6296,13 +6305,13 @@
         <v>64</v>
       </c>
       <c r="N85" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O85" t="s">
         <v>187</v>
       </c>
       <c r="P85">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q85" t="s">
         <v>188</v>
@@ -6316,7 +6325,7 @@
         <v>62</v>
       </c>
       <c r="C86" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D86" t="s">
         <v>63</v>
@@ -6340,7 +6349,7 @@
         <v>62</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>63</v>
@@ -6349,13 +6358,13 @@
         <v>64</v>
       </c>
       <c r="N86" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="O86" t="s">
         <v>187</v>
       </c>
       <c r="P86">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="Q86" t="s">
         <v>188</v>
@@ -6369,7 +6378,7 @@
         <v>62</v>
       </c>
       <c r="C87" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D87" t="s">
         <v>63</v>
@@ -6381,7 +6390,7 @@
         <v>62</v>
       </c>
       <c r="G87" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H87" t="s">
         <v>63</v>
@@ -6393,7 +6402,7 @@
         <v>62</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L87" s="1" t="s">
         <v>63</v>
@@ -6402,13 +6411,13 @@
         <v>64</v>
       </c>
       <c r="N87" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="O87" t="s">
         <v>187</v>
       </c>
       <c r="P87">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="Q87" t="s">
         <v>188</v>
@@ -6422,7 +6431,7 @@
         <v>62</v>
       </c>
       <c r="C88" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D88" t="s">
         <v>63</v>
@@ -6446,7 +6455,7 @@
         <v>62</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>63</v>
@@ -6475,7 +6484,7 @@
         <v>62</v>
       </c>
       <c r="C89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D89" t="s">
         <v>63</v>
@@ -6499,7 +6508,7 @@
         <v>62</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>63</v>
@@ -6528,7 +6537,7 @@
         <v>62</v>
       </c>
       <c r="C90" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D90" t="s">
         <v>63</v>
@@ -6552,7 +6561,7 @@
         <v>62</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>63</v>
@@ -6561,13 +6570,13 @@
         <v>64</v>
       </c>
       <c r="N90" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="O90" t="s">
         <v>187</v>
       </c>
       <c r="P90">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q90" t="s">
         <v>188</v>
@@ -6581,7 +6590,7 @@
         <v>62</v>
       </c>
       <c r="C91" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D91" t="s">
         <v>63</v>
@@ -6605,7 +6614,7 @@
         <v>62</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>63</v>
@@ -6614,13 +6623,13 @@
         <v>64</v>
       </c>
       <c r="N91" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="O91" t="s">
         <v>187</v>
       </c>
       <c r="P91">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q91" t="s">
         <v>188</v>
@@ -6634,7 +6643,7 @@
         <v>62</v>
       </c>
       <c r="C92" t="s">
-        <v>263</v>
+        <v>114</v>
       </c>
       <c r="D92" t="s">
         <v>63</v>
@@ -6657,8 +6666,8 @@
       <c r="J92" t="s">
         <v>62</v>
       </c>
-      <c r="K92" s="3" t="s">
-        <v>296</v>
+      <c r="K92" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>63</v>
@@ -6667,13 +6676,13 @@
         <v>64</v>
       </c>
       <c r="N92" t="s">
-        <v>268</v>
+        <v>158</v>
       </c>
       <c r="O92" t="s">
         <v>187</v>
       </c>
       <c r="P92">
-        <v>75000</v>
+        <v>5000</v>
       </c>
       <c r="Q92" t="s">
         <v>188</v>
@@ -6687,7 +6696,7 @@
         <v>62</v>
       </c>
       <c r="C93" t="s">
-        <v>118</v>
+        <v>263</v>
       </c>
       <c r="D93" t="s">
         <v>63</v>
@@ -6699,7 +6708,7 @@
         <v>62</v>
       </c>
       <c r="G93" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H93" t="s">
         <v>63</v>
@@ -6710,8 +6719,8 @@
       <c r="J93" t="s">
         <v>62</v>
       </c>
-      <c r="K93" s="1" t="s">
-        <v>189</v>
+      <c r="K93" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>63</v>
@@ -6720,13 +6729,13 @@
         <v>64</v>
       </c>
       <c r="N93" t="s">
-        <v>131</v>
+        <v>268</v>
       </c>
       <c r="O93" t="s">
         <v>187</v>
       </c>
       <c r="P93">
-        <v>50</v>
+        <v>75000</v>
       </c>
       <c r="Q93" t="s">
         <v>188</v>
@@ -6740,7 +6749,7 @@
         <v>62</v>
       </c>
       <c r="C94" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D94" t="s">
         <v>63</v>
@@ -6764,7 +6773,7 @@
         <v>62</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>63</v>
@@ -6773,13 +6782,13 @@
         <v>64</v>
       </c>
       <c r="N94" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O94" t="s">
         <v>187</v>
       </c>
       <c r="P94">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="Q94" t="s">
         <v>188</v>
@@ -6793,7 +6802,7 @@
         <v>62</v>
       </c>
       <c r="C95" t="s">
-        <v>223</v>
+        <v>119</v>
       </c>
       <c r="D95" t="s">
         <v>63</v>
@@ -6816,8 +6825,8 @@
       <c r="J95" t="s">
         <v>62</v>
       </c>
-      <c r="K95" s="3" t="s">
-        <v>275</v>
+      <c r="K95" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>63</v>
@@ -6826,13 +6835,13 @@
         <v>64</v>
       </c>
       <c r="N95" t="s">
-        <v>229</v>
+        <v>130</v>
       </c>
       <c r="O95" t="s">
         <v>187</v>
       </c>
       <c r="P95">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="Q95" t="s">
         <v>188</v>
@@ -6846,7 +6855,7 @@
         <v>62</v>
       </c>
       <c r="C96" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D96" t="s">
         <v>63</v>
@@ -6869,8 +6878,8 @@
       <c r="J96" t="s">
         <v>62</v>
       </c>
-      <c r="K96" s="1" t="s">
-        <v>278</v>
+      <c r="K96" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>63</v>
@@ -6879,13 +6888,13 @@
         <v>64</v>
       </c>
       <c r="N96" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O96" t="s">
         <v>187</v>
       </c>
       <c r="P96">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="Q96" t="s">
         <v>188</v>
@@ -6899,7 +6908,7 @@
         <v>62</v>
       </c>
       <c r="C97" t="s">
-        <v>330</v>
+        <v>226</v>
       </c>
       <c r="D97" t="s">
         <v>63</v>
@@ -6923,7 +6932,7 @@
         <v>62</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>336</v>
+        <v>278</v>
       </c>
       <c r="L97" s="1" t="s">
         <v>63</v>
@@ -6932,13 +6941,13 @@
         <v>64</v>
       </c>
       <c r="N97" t="s">
-        <v>337</v>
+        <v>232</v>
       </c>
       <c r="O97" t="s">
         <v>187</v>
       </c>
       <c r="P97">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="Q97" t="s">
         <v>188</v>
@@ -6952,7 +6961,7 @@
         <v>62</v>
       </c>
       <c r="C98" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D98" t="s">
         <v>63</v>
@@ -6976,7 +6985,7 @@
         <v>62</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="L98" s="1" t="s">
         <v>63</v>
@@ -6985,13 +6994,13 @@
         <v>64</v>
       </c>
       <c r="N98" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="O98" t="s">
         <v>187</v>
       </c>
       <c r="P98">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="Q98" t="s">
         <v>188</v>
@@ -7005,7 +7014,7 @@
         <v>62</v>
       </c>
       <c r="C99" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D99" t="s">
         <v>63</v>
@@ -7029,7 +7038,7 @@
         <v>62</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L99" s="1" t="s">
         <v>63</v>
@@ -7038,13 +7047,13 @@
         <v>64</v>
       </c>
       <c r="N99" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O99" t="s">
         <v>187</v>
       </c>
       <c r="P99">
-        <v>7500</v>
+        <v>5000</v>
       </c>
       <c r="Q99" t="s">
         <v>188</v>
@@ -7058,7 +7067,7 @@
         <v>62</v>
       </c>
       <c r="C100" t="s">
-        <v>228</v>
+        <v>329</v>
       </c>
       <c r="D100" t="s">
         <v>63</v>
@@ -7082,7 +7091,7 @@
         <v>62</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>280</v>
+        <v>334</v>
       </c>
       <c r="L100" s="1" t="s">
         <v>63</v>
@@ -7091,13 +7100,13 @@
         <v>64</v>
       </c>
       <c r="N100" t="s">
-        <v>234</v>
+        <v>335</v>
       </c>
       <c r="O100" t="s">
         <v>187</v>
       </c>
       <c r="P100">
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="Q100" t="s">
         <v>188</v>
@@ -7111,7 +7120,7 @@
         <v>62</v>
       </c>
       <c r="C101" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D101" t="s">
         <v>63</v>
@@ -7135,7 +7144,7 @@
         <v>62</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L101" s="1" t="s">
         <v>63</v>
@@ -7144,13 +7153,13 @@
         <v>64</v>
       </c>
       <c r="N101" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="O101" t="s">
         <v>187</v>
       </c>
       <c r="P101">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="Q101" t="s">
         <v>188</v>
@@ -7164,7 +7173,7 @@
         <v>62</v>
       </c>
       <c r="C102" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="D102" t="s">
         <v>63</v>
@@ -7188,7 +7197,7 @@
         <v>62</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>37</v>
+        <v>279</v>
       </c>
       <c r="L102" s="1" t="s">
         <v>63</v>
@@ -7197,13 +7206,13 @@
         <v>64</v>
       </c>
       <c r="N102" t="s">
-        <v>165</v>
+        <v>233</v>
       </c>
       <c r="O102" t="s">
         <v>187</v>
       </c>
       <c r="P102">
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="Q102" t="s">
         <v>188</v>
@@ -7217,7 +7226,7 @@
         <v>62</v>
       </c>
       <c r="C103" t="s">
-        <v>224</v>
+        <v>120</v>
       </c>
       <c r="D103" t="s">
         <v>63</v>
@@ -7240,8 +7249,8 @@
       <c r="J103" t="s">
         <v>62</v>
       </c>
-      <c r="K103" s="3" t="s">
-        <v>276</v>
+      <c r="K103" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="L103" s="1" t="s">
         <v>63</v>
@@ -7250,13 +7259,13 @@
         <v>64</v>
       </c>
       <c r="N103" t="s">
-        <v>230</v>
+        <v>165</v>
       </c>
       <c r="O103" t="s">
         <v>187</v>
       </c>
       <c r="P103">
-        <v>75000</v>
+        <v>50000</v>
       </c>
       <c r="Q103" t="s">
         <v>188</v>
@@ -7270,7 +7279,7 @@
         <v>62</v>
       </c>
       <c r="C104" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D104" t="s">
         <v>63</v>
@@ -7294,7 +7303,7 @@
         <v>62</v>
       </c>
       <c r="K104" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L104" s="1" t="s">
         <v>63</v>
@@ -7303,13 +7312,13 @@
         <v>64</v>
       </c>
       <c r="N104" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O104" t="s">
         <v>187</v>
       </c>
       <c r="P104">
-        <v>100000</v>
+        <v>75000</v>
       </c>
       <c r="Q104" t="s">
         <v>188</v>
@@ -7323,7 +7332,7 @@
         <v>62</v>
       </c>
       <c r="C105" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
       <c r="D105" t="s">
         <v>63</v>
@@ -7346,31 +7355,80 @@
       <c r="J105" t="s">
         <v>62</v>
       </c>
-      <c r="K105" s="1" t="s">
+      <c r="K105" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M105" t="s">
+        <v>64</v>
+      </c>
+      <c r="N105" t="s">
+        <v>231</v>
+      </c>
+      <c r="O105" t="s">
+        <v>187</v>
+      </c>
+      <c r="P105">
+        <v>100000</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>61</v>
+      </c>
+      <c r="B106" t="s">
+        <v>62</v>
+      </c>
+      <c r="C106" t="s">
+        <v>121</v>
+      </c>
+      <c r="D106" t="s">
+        <v>63</v>
+      </c>
+      <c r="E106" t="s">
+        <v>122</v>
+      </c>
+      <c r="F106" t="s">
+        <v>62</v>
+      </c>
+      <c r="G106" t="s">
+        <v>125</v>
+      </c>
+      <c r="H106" t="s">
+        <v>63</v>
+      </c>
+      <c r="I106" t="s">
+        <v>60</v>
+      </c>
+      <c r="J106" t="s">
+        <v>62</v>
+      </c>
+      <c r="K106" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L105" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M105" t="s">
-        <v>64</v>
-      </c>
-      <c r="N105" t="s">
+      <c r="L106" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M106" t="s">
+        <v>64</v>
+      </c>
+      <c r="N106" t="s">
         <v>305</v>
       </c>
-      <c r="O105" t="s">
-        <v>187</v>
-      </c>
-      <c r="P105">
+      <c r="O106" t="s">
+        <v>187</v>
+      </c>
+      <c r="P106">
         <v>500000</v>
       </c>
-      <c r="Q105" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K106" s="1"/>
-      <c r="L106" s="1"/>
+      <c r="Q106" t="s">
+        <v>188</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>